<commit_message>
adjusting stubs to be more meaningful data types
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -472,10 +472,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:O18"/>
+  <dimension ref="B1:P18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,16 +483,16 @@
     <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="7" max="7" width="15.140625" customWidth="1"/>
     <col min="8" max="8" width="48.140625" customWidth="1"/>
-    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="4.5703125" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -513,7 +513,7 @@
         <v>9.3860571338892989</v>
       </c>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -534,7 +534,7 @@
         <v>18.496214623545704</v>
       </c>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -555,23 +555,23 @@
         <v>10.646448169374416</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="G6" s="3">
         <f>SUM(G3:G5)</f>
         <v>38.528719926809416</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0</v>
       </c>
@@ -614,8 +614,12 @@
         <f>SQRT((M9-M10)^2 + (N9-N10)^2)</f>
         <v>54.684766462557853</v>
       </c>
-    </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P9" t="str">
+        <f>"("&amp;"'"&amp;K9&amp;"'"&amp;", "&amp;"'"&amp;L9&amp;"'"&amp;", "&amp;M9&amp;", "&amp;N9&amp;")"&amp;",\"</f>
+        <v>('Alabama', 'Montgomery', 32.361538, -86.279118),\</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>1</v>
       </c>
@@ -658,8 +662,12 @@
         <f t="shared" ref="O10:O16" si="1">SQRT((M10-M11)^2 + (N10-N11)^2)</f>
         <v>34.799846620320231</v>
       </c>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P10" t="str">
+        <f t="shared" ref="P10:P17" si="2">"("&amp;"'"&amp;K10&amp;"'"&amp;", "&amp;"'"&amp;L10&amp;"'"&amp;", "&amp;M10&amp;", "&amp;N10&amp;")"&amp;",\"</f>
+        <v>('Alaska', 'Juneau', 58.301935, -134.41974),\</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>2</v>
       </c>
@@ -676,7 +684,7 @@
         <v>-112.07384399999999</v>
       </c>
       <c r="G11">
-        <f t="shared" ref="G11:G16" si="2">SQRT((E11-E12)^2 + (F11-F12)^2)</f>
+        <f t="shared" ref="G11:G16" si="3">SQRT((E11-E12)^2 + (F11-F12)^2)</f>
         <v>19.784662294868419</v>
       </c>
       <c r="H11" t="str">
@@ -702,8 +710,12 @@
         <f t="shared" si="1"/>
         <v>13.606290263811601</v>
       </c>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P11" t="str">
+        <f t="shared" si="2"/>
+        <v>('Colorado', 'Denver', 39.7391667, -104.984167),\</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>3</v>
       </c>
@@ -720,7 +732,7 @@
         <v>-92.331121999999993</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.387087905160527</v>
       </c>
       <c r="H12" t="str">
@@ -746,8 +758,12 @@
         <f t="shared" si="1"/>
         <v>29.387087905160527</v>
       </c>
-    </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P12" t="str">
+        <f t="shared" si="2"/>
+        <v>('Arkansas', 'Little Rock', 34.736009, -92.331122),\</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>4</v>
       </c>
@@ -764,7 +780,7 @@
         <v>-121.468926</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.527192671043313</v>
       </c>
       <c r="H13" t="str">
@@ -790,8 +806,12 @@
         <f t="shared" si="1"/>
         <v>10.693480559697486</v>
       </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P13" t="str">
+        <f t="shared" si="2"/>
+        <v>('California', 'Sacramento', 38.555605, -121.468926),\</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>5</v>
       </c>
@@ -808,7 +828,7 @@
         <v>-104.984167</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>32.370745241011633</v>
       </c>
       <c r="H14" t="str">
@@ -834,8 +854,12 @@
         <f t="shared" si="1"/>
         <v>40.265487390607653</v>
       </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P14" t="str">
+        <f t="shared" si="2"/>
+        <v>('Arizona', 'Phoenix', 33.448457, -112.073844),\</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>6</v>
       </c>
@@ -852,7 +876,7 @@
         <v>-72.677000000000007</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.8610283806605139</v>
       </c>
       <c r="H15" t="str">
@@ -878,8 +902,12 @@
         <f t="shared" si="1"/>
         <v>3.8610283806605139</v>
       </c>
-    </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P15" t="str">
+        <f t="shared" si="2"/>
+        <v>('Connecticut', 'Hartford', 41.767, -72.677),\</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>7</v>
       </c>
@@ -896,7 +924,7 @@
         <v>-75.526754999999994</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12.343378233484788</v>
       </c>
       <c r="H16" t="str">
@@ -922,8 +950,12 @@
         <f t="shared" si="1"/>
         <v>12.343378233484788</v>
       </c>
-    </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P16" t="str">
+        <f t="shared" si="2"/>
+        <v>('Delaware', 'Dover', 39.161921, -75.526755),\</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>8</v>
       </c>
@@ -966,8 +998,12 @@
         <f>SQRT((M17-M9)^2 + (N17-N9)^2)</f>
         <v>2.7699334876036334</v>
       </c>
-    </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="P17" t="str">
+        <f t="shared" si="2"/>
+        <v>('Florida', 'Tallahassee', 30.4518, -84.27277),\</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G18" s="3">
         <f>SUM(G9:G17)</f>
         <v>205.15085979420317</v>

</xml_diff>

<commit_message>
fixed bug - a variable assignment needed copy.copy
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -9,11 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="6990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="6990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$C$3:$C$51</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="174">
   <si>
     <t>Kentucky</t>
   </si>
@@ -96,12 +100,465 @@
   </si>
   <si>
     <t>test_swap_cities</t>
+  </si>
+  <si>
+    <t>Junea</t>
+  </si>
+  <si>
+    <t>Pheonix</t>
+  </si>
+  <si>
+    <t>0  . Frankfort           --&gt;       1  . Dover               Cost</t>
+  </si>
+  <si>
+    <t>1  . Dover               --&gt;       2  . Helana              Cost</t>
+  </si>
+  <si>
+    <t>2  . Helana              --&gt;       3  . Austin              Cost</t>
+  </si>
+  <si>
+    <t>3  . Austin              --&gt;       4  . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>4  . Montpelier          --&gt;       5  . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>5  . Sacramento          --&gt;       6  . Boston              Cost</t>
+  </si>
+  <si>
+    <t>6  . Boston              --&gt;       7  . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>7  . Santa Fe            --&gt;       8  . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>8  . Salt Lake City      --&gt;       9  . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>9  . Lansing             --&gt;       10 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>10 . Juneau              --&gt;       11 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>11 . Hartford            --&gt;       12 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>12 . Indianapolis        --&gt;       13 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>13 . Albany              --&gt;       14 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>14 . Raleigh             --&gt;       15 . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>15 . Little Rock         --&gt;       16 . Madison             Cost</t>
+  </si>
+  <si>
+    <t>16 . Madison             --&gt;       17 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>17 . Lincoln             --&gt;       18 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>18 . Concord             --&gt;       19 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>19 . Nashville           --&gt;       20 . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>20 . Honolulu            --&gt;       21 . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>21 . Phoenix             --&gt;       22 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>22 . Atlanta             --&gt;       23 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>23 . Boise               --&gt;       24 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>24 . Columbia            --&gt;       25 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>25 . Richmond            --&gt;       26 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>26 . Bismarck            --&gt;       27 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>27 . Tallahassee         --&gt;       28 . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>28 . Harrisburg          --&gt;       29 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>29 . Providence          --&gt;       30 . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>30 . Columbus            --&gt;       31 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>31 . Denver              --&gt;       32 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>32 . Topeka              --&gt;       33 . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>33 . Cheyenne            --&gt;       34 . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>34 . Carson City         --&gt;       35 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>35 . Annapolis           --&gt;       36 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>36 . Oklahoma City       --&gt;       37 . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>37 . Charleston          --&gt;       38 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>38 . Pierre              --&gt;       39 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>39 . Jackson             --&gt;       40 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>40 . Des Moines          --&gt;       41 . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>41 . Olympia             --&gt;       42 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>42 . Springfield         --&gt;       43 . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>43 . Montgomery          --&gt;       44 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>44 . Saint Paul          --&gt;       45 . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>45 . Trenton             --&gt;       46 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>46 . Baton Rouge         --&gt;       47 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>47 . Jefferson City      --&gt;       48 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>48 . Augusta             --&gt;       49 . Salem               Cost</t>
+  </si>
+  <si>
+    <t>Tests</t>
+  </si>
+  <si>
+    <t>0  . Sacramento          --&gt;       1  . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>1  . Cheyenne            --&gt;       2  . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>2  . Harrisburg          --&gt;       3  . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>3  . Montpelier          --&gt;       4  . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>4  . Little Rock         --&gt;       5  . Concord             Cost</t>
+  </si>
+  <si>
+    <t>5  . Concord             --&gt;       6  . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>6  . Columbia            --&gt;       7  . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>7  . Indianapolis        --&gt;       8  . Boston              Cost</t>
+  </si>
+  <si>
+    <t>8  . Boston              --&gt;       9  . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>9  . Springfield         --&gt;       10 . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>10 . Charleston          --&gt;       11 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>11 . Juneau              --&gt;       12 . Salem               Cost</t>
+  </si>
+  <si>
+    <t>12 . Salem               --&gt;       13 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>13 . Atlanta             --&gt;       14 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>14 . Hartford            --&gt;       15 . Austin              Cost</t>
+  </si>
+  <si>
+    <t>15 . Austin              --&gt;       16 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>16 . Raleigh             --&gt;       17 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>17 . Jackson             --&gt;       18 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>18 . Baton Rouge         --&gt;       19 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>19 . Providence          --&gt;       20 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>20 . Des Moines          --&gt;       21 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>21 . Annapolis           --&gt;       22 . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>22 . Trenton             --&gt;       23 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>23 . Helana              --&gt;       24 . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>24 . Salt Lake City      --&gt;       25 . Dover               Cost</t>
+  </si>
+  <si>
+    <t>25 . Dover               --&gt;       26 . Madison             Cost</t>
+  </si>
+  <si>
+    <t>26 . Madison             --&gt;       27 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>27 . Bismarck            --&gt;       28 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>28 . Lansing             --&gt;       29 . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>29 . Montgomery          --&gt;       30 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>30 . Albany              --&gt;       31 . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>31 . Olympia             --&gt;       32 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>32 . Richmond            --&gt;       33 . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>33 . Carson City         --&gt;       34 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>34 . Topeka              --&gt;       35 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>35 . Lincoln             --&gt;       36 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>36 . Jefferson City      --&gt;       37 . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>37 . Honolulu            --&gt;       38 . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>38 . Frankfort           --&gt;       39 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>39 . Boise               --&gt;       40 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>40 . Augusta             --&gt;       41 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>41 . Saint Paul          --&gt;       42 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>42 . Denver              --&gt;       43 . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>43 . Columbus            --&gt;       44 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>44 . Nashville           --&gt;       45 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>45 . Tallahassee         --&gt;       46 . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>46 . Santa Fe            --&gt;       47 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>47 . Oklahoma City       --&gt;       48 . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>48 . Phoenix             --&gt;       49 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>0  . Trenton             --&gt;       1  . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>1  . Sacramento          --&gt;       2  . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>2  . Atlanta             --&gt;       3  . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>3  . Hartford            --&gt;       4  . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>4  . Charleston          --&gt;       5  . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>5  . Montgomery          --&gt;       6  . Salem               Cost</t>
+  </si>
+  <si>
+    <t>6  . Salem               --&gt;       7  . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>7  . Lincoln             --&gt;       8  . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>8  . Frankfort           --&gt;       9  . Madison             Cost</t>
+  </si>
+  <si>
+    <t>9  . Madison             --&gt;       10 . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>10 . Little Rock         --&gt;       11 . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>11 . Columbus            --&gt;       12 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>12 . Albany              --&gt;       13 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>13 . Raleigh             --&gt;       14 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>14 . Augusta             --&gt;       15 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>15 . Juneau              --&gt;       16 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>16 . Jackson             --&gt;       17 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>17 . Jefferson City      --&gt;       18 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>18 . Columbia            --&gt;       19 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>19 . Tallahassee         --&gt;       20 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>20 . Denver              --&gt;       21 . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>21 . Phoenix             --&gt;       22 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>22 . Boise               --&gt;       23 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>23 . Indianapolis        --&gt;       24 . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>24 . Carson City         --&gt;       25 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>25 . Baton Rouge         --&gt;       26 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>26 . Springfield         --&gt;       27 . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>27 . Honolulu            --&gt;       28 . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>28 . Salt Lake City      --&gt;       29 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>29 . Oklahoma City       --&gt;       30 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>30 . Annapolis           --&gt;       31 . Dover               Cost</t>
+  </si>
+  <si>
+    <t>31 . Dover               --&gt;       32 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>32 . Lansing             --&gt;       33 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>33 . Helana              --&gt;       34 . Austin              Cost</t>
+  </si>
+  <si>
+    <t>34 . Austin              --&gt;       35 . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>35 . Montpelier          --&gt;       36 . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>36 . Santa Fe            --&gt;       37 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>37 . Bismarck            --&gt;       38 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>38 . Pierre              --&gt;       39 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>39 . Saint Paul          --&gt;       40 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>40 . Des Moines          --&gt;       41 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>41 . Nashville           --&gt;       42 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>42 . Richmond            --&gt;       43 . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>43 . Cheyenne            --&gt;       44 . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>44 . Harrisburg          --&gt;       45 . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>45 . Olympia             --&gt;       46 . Boston              Cost</t>
+  </si>
+  <si>
+    <t>46 . Boston              --&gt;       47 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>47 . Topeka              --&gt;       48 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>48 . Providence          --&gt;       49 . Concord             Cost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,13 +608,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,27 +932,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P18"/>
+  <dimension ref="B1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="48.140625" customWidth="1"/>
     <col min="9" max="9" width="4.5703125" customWidth="1"/>
     <col min="11" max="11" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>0</v>
       </c>
@@ -508,12 +971,12 @@
       <c r="F3">
         <v>-84.863110000000006</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="4">
         <f>SQRT((E3-E4)^2 + (F3-F4)^2)</f>
         <v>9.3860571338892989</v>
       </c>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -529,12 +992,12 @@
       <c r="F4">
         <v>-75.526754999999994</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="4">
         <f>SQRT((E4-E5)^2 + (F4-F5)^2)</f>
         <v>18.496214623545704</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -550,467 +1013,873 @@
       <c r="F5">
         <v>-93.093999999999994</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="4">
         <f>SQRT((E5-E3)^2 + (F5-F3)^2)</f>
         <v>10.646448169374416</v>
       </c>
     </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
-      <c r="G6" s="3">
+      <c r="G6" s="5">
         <f>SUM(G3:G5)</f>
         <v>38.528719926809416</v>
       </c>
     </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8">
+        <v>41.767000000000003</v>
+      </c>
+      <c r="F8">
+        <v>-72.677000000000007</v>
+      </c>
+      <c r="G8" s="4">
+        <f>SQRT((E8-E9)^2 + (F8-F9)^2)</f>
+        <v>3.8610283806605139</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>39.161921</v>
+      </c>
+      <c r="F9">
+        <v>-75.526754999999994</v>
+      </c>
+      <c r="G9" s="4">
+        <f>SQRT((E9-E10)^2 + (F9-F10)^2)</f>
+        <v>12.343378233484788</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10">
+        <v>30.451799999999999</v>
+      </c>
+      <c r="F10">
+        <v>-84.272769999999994</v>
+      </c>
+      <c r="G10" s="4">
+        <f>SQRT((E10-E8)^2 + (F10-F8)^2)</f>
+        <v>16.201716974842505</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G11" s="5">
+        <f>SUM(G8:G10)</f>
+        <v>32.406123588987811</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13">
+        <v>58.301935</v>
+      </c>
+      <c r="F13">
+        <v>-134.41973999999999</v>
+      </c>
+      <c r="G13" s="4">
+        <f>SQRT((E13-E14)^2 + (F13-F14)^2)</f>
+        <v>33.422065117812515</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14">
+        <v>33.448456999999998</v>
+      </c>
+      <c r="F14">
+        <v>-112.07384399999999</v>
+      </c>
+      <c r="G14" s="4">
+        <f>SQRT((E14-E15)^2 + (F14-F15)^2)</f>
+        <v>10.693480559697486</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>38.555605</v>
+      </c>
+      <c r="F15">
+        <v>-121.468926</v>
+      </c>
+      <c r="G15" s="4">
+        <f>SQRT((E15-E13)^2 + (F15-F13)^2)</f>
+        <v>23.6144263477116</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G16" s="5">
+        <f>SUM(G13:G15)</f>
+        <v>67.729972025221599</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C23" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D23" t="s">
         <v>7</v>
       </c>
-      <c r="E9">
+      <c r="E23">
         <v>32.361538000000003</v>
       </c>
-      <c r="F9">
+      <c r="F23">
         <v>-86.279117999999997</v>
       </c>
-      <c r="G9">
-        <f>SQRT((E9-E10)^2 + (F9-F10)^2)</f>
+      <c r="G23" s="4">
+        <f>SQRT((E23-E24)^2 + (F23-F24)^2)</f>
         <v>54.684766462557853</v>
       </c>
-      <c r="H9" t="str">
-        <f>"("&amp;"'"&amp;C9&amp;"'"&amp;", "&amp;"'"&amp;D9&amp;"'"&amp;", "&amp;E9&amp;", "&amp;F9&amp;")"&amp;",\"</f>
+      <c r="H23" t="str">
+        <f>"("&amp;"'"&amp;C23&amp;"'"&amp;", "&amp;"'"&amp;D23&amp;"'"&amp;", "&amp;E23&amp;", "&amp;F23&amp;")"&amp;",\"</f>
         <v>('Alabama', 'Montgomery', 32.361538, -86.279118),\</v>
       </c>
-      <c r="J9">
+      <c r="J23">
         <v>0</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K23" t="s">
         <v>6</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L23" t="s">
         <v>7</v>
       </c>
-      <c r="M9">
+      <c r="M23">
         <v>32.361538000000003</v>
       </c>
-      <c r="N9">
+      <c r="N23">
         <v>-86.279117999999997</v>
       </c>
-      <c r="O9">
-        <f>SQRT((M9-M10)^2 + (N9-N10)^2)</f>
+      <c r="O23">
+        <f>SQRT((M23-M24)^2 + (N23-N24)^2)</f>
         <v>54.684766462557853</v>
       </c>
-      <c r="P9" t="str">
-        <f>"("&amp;"'"&amp;K9&amp;"'"&amp;", "&amp;"'"&amp;L9&amp;"'"&amp;", "&amp;M9&amp;", "&amp;N9&amp;")"&amp;",\"</f>
+      <c r="P23" t="str">
+        <f>"("&amp;"'"&amp;K23&amp;"'"&amp;", "&amp;"'"&amp;L23&amp;"'"&amp;", "&amp;M23&amp;", "&amp;N23&amp;")"&amp;",\"</f>
         <v>('Alabama', 'Montgomery', 32.361538, -86.279118),\</v>
       </c>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B24">
         <v>1</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C24" t="s">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D24" t="s">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="E24">
         <v>58.301935</v>
       </c>
-      <c r="F10">
+      <c r="F24">
         <v>-134.41973999999999</v>
       </c>
-      <c r="G10">
-        <f>SQRT((E10-E11)^2 + (F10-F11)^2)</f>
+      <c r="G24" s="4">
+        <f>SQRT((E24-E25)^2 + (F24-F25)^2)</f>
         <v>33.422065117812515</v>
       </c>
-      <c r="H10" t="str">
-        <f t="shared" ref="H10:H17" si="0">"("&amp;"'"&amp;C10&amp;"'"&amp;", "&amp;"'"&amp;D10&amp;"'"&amp;", "&amp;E10&amp;", "&amp;F10&amp;")"&amp;",\"</f>
+      <c r="H24" t="str">
+        <f t="shared" ref="H24:H31" si="0">"("&amp;"'"&amp;C24&amp;"'"&amp;", "&amp;"'"&amp;D24&amp;"'"&amp;", "&amp;E24&amp;", "&amp;F24&amp;")"&amp;",\"</f>
         <v>('Alaska', 'Juneau', 58.301935, -134.41974),\</v>
       </c>
-      <c r="J10">
+      <c r="J24">
         <v>1</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K24" t="s">
         <v>8</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L24" t="s">
         <v>9</v>
       </c>
-      <c r="M10">
+      <c r="M24">
         <v>58.301935</v>
       </c>
-      <c r="N10">
+      <c r="N24">
         <v>-134.41973999999999</v>
       </c>
-      <c r="O10">
-        <f t="shared" ref="O10:O16" si="1">SQRT((M10-M11)^2 + (N10-N11)^2)</f>
+      <c r="O24">
+        <f t="shared" ref="O24:O30" si="1">SQRT((M24-M25)^2 + (N24-N25)^2)</f>
         <v>34.799846620320231</v>
       </c>
-      <c r="P10" t="str">
-        <f t="shared" ref="P10:P17" si="2">"("&amp;"'"&amp;K10&amp;"'"&amp;", "&amp;"'"&amp;L10&amp;"'"&amp;", "&amp;M10&amp;", "&amp;N10&amp;")"&amp;",\"</f>
+      <c r="P24" t="str">
+        <f t="shared" ref="P24:P31" si="2">"("&amp;"'"&amp;K24&amp;"'"&amp;", "&amp;"'"&amp;L24&amp;"'"&amp;", "&amp;M24&amp;", "&amp;N24&amp;")"&amp;",\"</f>
         <v>('Alaska', 'Juneau', 58.301935, -134.41974),\</v>
       </c>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B25">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C25" t="s">
         <v>10</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D25" t="s">
         <v>11</v>
       </c>
-      <c r="E11">
+      <c r="E25">
         <v>33.448456999999998</v>
       </c>
-      <c r="F11">
+      <c r="F25">
         <v>-112.07384399999999</v>
       </c>
-      <c r="G11">
-        <f t="shared" ref="G11:G16" si="3">SQRT((E11-E12)^2 + (F11-F12)^2)</f>
+      <c r="G25" s="4">
+        <f t="shared" ref="G25:G30" si="3">SQRT((E25-E26)^2 + (F25-F26)^2)</f>
         <v>19.784662294868419</v>
       </c>
-      <c r="H11" t="str">
+      <c r="H25" t="str">
         <f t="shared" si="0"/>
         <v>('Arizona', 'Phoenix', 33.448457, -112.073844),\</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J25" s="2">
         <v>5</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M25" s="2">
         <v>39.739166699999998</v>
       </c>
-      <c r="N11" s="2">
+      <c r="N25" s="2">
         <v>-104.984167</v>
       </c>
-      <c r="O11" s="2">
+      <c r="O25" s="2">
         <f t="shared" si="1"/>
         <v>13.606290263811601</v>
       </c>
-      <c r="P11" t="str">
+      <c r="P25" t="str">
         <f t="shared" si="2"/>
         <v>('Colorado', 'Denver', 39.7391667, -104.984167),\</v>
       </c>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B12">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B26">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C26" t="s">
         <v>12</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D26" t="s">
         <v>13</v>
       </c>
-      <c r="E12">
+      <c r="E26">
         <v>34.736009000000003</v>
       </c>
-      <c r="F12">
+      <c r="F26">
         <v>-92.331121999999993</v>
       </c>
-      <c r="G12">
+      <c r="G26" s="4">
         <f t="shared" si="3"/>
         <v>29.387087905160527</v>
       </c>
-      <c r="H12" t="str">
+      <c r="H26" t="str">
         <f t="shared" si="0"/>
         <v>('Arkansas', 'Little Rock', 34.736009, -92.331122),\</v>
       </c>
-      <c r="J12">
+      <c r="J26">
         <v>3</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K26" t="s">
         <v>12</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L26" t="s">
         <v>13</v>
       </c>
-      <c r="M12">
+      <c r="M26">
         <v>34.736009000000003</v>
       </c>
-      <c r="N12">
+      <c r="N26">
         <v>-92.331121999999993</v>
       </c>
-      <c r="O12">
+      <c r="O26">
         <f t="shared" si="1"/>
         <v>29.387087905160527</v>
       </c>
-      <c r="P12" t="str">
+      <c r="P26" t="str">
         <f t="shared" si="2"/>
         <v>('Arkansas', 'Little Rock', 34.736009, -92.331122),\</v>
       </c>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B27">
         <v>4</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C27" t="s">
         <v>14</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D27" t="s">
         <v>15</v>
       </c>
-      <c r="E13">
+      <c r="E27">
         <v>38.555605</v>
       </c>
-      <c r="F13">
+      <c r="F27">
         <v>-121.468926</v>
       </c>
-      <c r="G13">
+      <c r="G27" s="4">
         <f t="shared" si="3"/>
         <v>16.527192671043313</v>
       </c>
-      <c r="H13" t="str">
+      <c r="H27" t="str">
         <f t="shared" si="0"/>
         <v>('California', 'Sacramento', 38.555605, -121.468926),\</v>
       </c>
-      <c r="J13">
+      <c r="J27">
         <v>4</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K27" t="s">
         <v>14</v>
       </c>
-      <c r="L13" t="s">
+      <c r="L27" t="s">
         <v>15</v>
       </c>
-      <c r="M13">
+      <c r="M27">
         <v>38.555605</v>
       </c>
-      <c r="N13">
+      <c r="N27">
         <v>-121.468926</v>
       </c>
-      <c r="O13">
+      <c r="O27">
         <f t="shared" si="1"/>
         <v>10.693480559697486</v>
       </c>
-      <c r="P13" t="str">
+      <c r="P27" t="str">
         <f t="shared" si="2"/>
         <v>('California', 'Sacramento', 38.555605, -121.468926),\</v>
       </c>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B28">
         <v>5</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C28" t="s">
         <v>16</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D28" t="s">
         <v>17</v>
       </c>
-      <c r="E14">
+      <c r="E28">
         <v>39.739166699999998</v>
       </c>
-      <c r="F14">
+      <c r="F28">
         <v>-104.984167</v>
       </c>
-      <c r="G14">
+      <c r="G28" s="4">
         <f t="shared" si="3"/>
         <v>32.370745241011633</v>
       </c>
-      <c r="H14" t="str">
+      <c r="H28" t="str">
         <f t="shared" si="0"/>
         <v>('Colorado', 'Denver', 39.7391667, -104.984167),\</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J28" s="2">
         <v>2</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M28" s="2">
         <v>33.448456999999998</v>
       </c>
-      <c r="N14" s="2">
+      <c r="N28" s="2">
         <v>-112.07384399999999</v>
       </c>
-      <c r="O14" s="2">
+      <c r="O28" s="2">
         <f t="shared" si="1"/>
         <v>40.265487390607653</v>
       </c>
-      <c r="P14" t="str">
+      <c r="P28" t="str">
         <f t="shared" si="2"/>
         <v>('Arizona', 'Phoenix', 33.448457, -112.073844),\</v>
       </c>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B29">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C29" t="s">
         <v>18</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D29" t="s">
         <v>19</v>
       </c>
-      <c r="E15">
+      <c r="E29">
         <v>41.767000000000003</v>
       </c>
-      <c r="F15">
+      <c r="F29">
         <v>-72.677000000000007</v>
       </c>
-      <c r="G15">
+      <c r="G29" s="4">
         <f t="shared" si="3"/>
         <v>3.8610283806605139</v>
       </c>
-      <c r="H15" t="str">
+      <c r="H29" t="str">
         <f t="shared" si="0"/>
         <v>('Connecticut', 'Hartford', 41.767, -72.677),\</v>
       </c>
-      <c r="J15">
+      <c r="J29">
         <v>6</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K29" t="s">
         <v>18</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L29" t="s">
         <v>19</v>
       </c>
-      <c r="M15">
+      <c r="M29">
         <v>41.767000000000003</v>
       </c>
-      <c r="N15">
+      <c r="N29">
         <v>-72.677000000000007</v>
       </c>
-      <c r="O15">
+      <c r="O29">
         <f t="shared" si="1"/>
         <v>3.8610283806605139</v>
       </c>
-      <c r="P15" t="str">
+      <c r="P29" t="str">
         <f t="shared" si="2"/>
         <v>('Connecticut', 'Hartford', 41.767, -72.677),\</v>
       </c>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B30">
         <v>7</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C30" t="s">
         <v>2</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D30" t="s">
         <v>3</v>
       </c>
-      <c r="E16">
+      <c r="E30">
         <v>39.161921</v>
       </c>
-      <c r="F16">
+      <c r="F30">
         <v>-75.526754999999994</v>
       </c>
-      <c r="G16">
+      <c r="G30" s="4">
         <f t="shared" si="3"/>
         <v>12.343378233484788</v>
       </c>
-      <c r="H16" t="str">
+      <c r="H30" t="str">
         <f t="shared" si="0"/>
         <v>('Delaware', 'Dover', 39.161921, -75.526755),\</v>
       </c>
-      <c r="J16">
+      <c r="J30">
         <v>7</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K30" t="s">
         <v>2</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L30" t="s">
         <v>3</v>
       </c>
-      <c r="M16">
+      <c r="M30">
         <v>39.161921</v>
       </c>
-      <c r="N16">
+      <c r="N30">
         <v>-75.526754999999994</v>
       </c>
-      <c r="O16">
+      <c r="O30">
         <f t="shared" si="1"/>
         <v>12.343378233484788</v>
       </c>
-      <c r="P16" t="str">
+      <c r="P30" t="str">
         <f t="shared" si="2"/>
         <v>('Delaware', 'Dover', 39.161921, -75.526755),\</v>
       </c>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B31">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C31" t="s">
         <v>20</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D31" t="s">
         <v>21</v>
       </c>
-      <c r="E17">
+      <c r="E31">
         <v>30.451799999999999</v>
       </c>
-      <c r="F17">
+      <c r="F31">
         <v>-84.272769999999994</v>
       </c>
-      <c r="G17">
-        <f>SQRT((E17-E9)^2 + (F17-F9)^2)</f>
+      <c r="G31" s="4">
+        <f>SQRT((E31-E23)^2 + (F31-F23)^2)</f>
         <v>2.7699334876036334</v>
       </c>
-      <c r="H17" t="str">
+      <c r="H31" t="str">
         <f t="shared" si="0"/>
         <v>('Florida', 'Tallahassee', 30.4518, -84.27277),\</v>
       </c>
-      <c r="J17">
+      <c r="J31">
         <v>8</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K31" t="s">
         <v>20</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L31" t="s">
         <v>21</v>
       </c>
-      <c r="M17">
+      <c r="M31">
         <v>30.451799999999999</v>
       </c>
-      <c r="N17">
+      <c r="N31">
         <v>-84.272769999999994</v>
       </c>
-      <c r="O17">
-        <f>SQRT((M17-M9)^2 + (N17-N9)^2)</f>
+      <c r="O31">
+        <f>SQRT((M31-M23)^2 + (N31-N23)^2)</f>
         <v>2.7699334876036334</v>
       </c>
-      <c r="P17" t="str">
+      <c r="P31" t="str">
         <f t="shared" si="2"/>
         <v>('Florida', 'Tallahassee', 30.4518, -84.27277),\</v>
       </c>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="G18" s="3">
-        <f>SUM(G9:G17)</f>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G32" s="5">
+        <f>SUM(G23:G31)</f>
         <v>205.15085979420317</v>
       </c>
-      <c r="O18" s="3">
-        <f>SUM(O9:O17)</f>
+      <c r="O32" s="3">
+        <f>SUM(O23:O31)</f>
         <v>202.41129930390429</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36">
+        <v>30.451799999999999</v>
+      </c>
+      <c r="F36">
+        <v>-84.272769999999994</v>
+      </c>
+      <c r="G36" s="4">
+        <f>SQRT((E36-E37)^2 + (F36-F37)^2)</f>
+        <v>57.361560471269648</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37">
+        <v>58.301935</v>
+      </c>
+      <c r="F37">
+        <v>-134.41973999999999</v>
+      </c>
+      <c r="G37" s="4">
+        <f>SQRT((E37-E38)^2 + (F37-F38)^2)</f>
+        <v>33.422065117812515</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>2</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>33.448456999999998</v>
+      </c>
+      <c r="F38">
+        <v>-112.07384399999999</v>
+      </c>
+      <c r="G38" s="4">
+        <f t="shared" ref="G38:G43" si="4">SQRT((E38-E39)^2 + (F38-F39)^2)</f>
+        <v>19.784662294868419</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39">
+        <v>34.736009000000003</v>
+      </c>
+      <c r="F39">
+        <v>-92.331121999999993</v>
+      </c>
+      <c r="G39" s="4">
+        <f t="shared" si="4"/>
+        <v>29.387087905160527</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>14</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40">
+        <v>38.555605</v>
+      </c>
+      <c r="F40">
+        <v>-121.468926</v>
+      </c>
+      <c r="G40" s="4">
+        <f t="shared" si="4"/>
+        <v>16.527192671043313</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E41">
+        <v>39.739166699999998</v>
+      </c>
+      <c r="F41">
+        <v>-104.984167</v>
+      </c>
+      <c r="G41" s="4">
+        <f t="shared" si="4"/>
+        <v>32.370745241011633</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>18</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42">
+        <v>41.767000000000003</v>
+      </c>
+      <c r="F42">
+        <v>-72.677000000000007</v>
+      </c>
+      <c r="G42" s="4">
+        <f t="shared" si="4"/>
+        <v>3.8610283806605139</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>39.161921</v>
+      </c>
+      <c r="F43">
+        <v>-75.526754999999994</v>
+      </c>
+      <c r="G43" s="4">
+        <f t="shared" si="4"/>
+        <v>12.722362949957764</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+      <c r="E44">
+        <v>32.361538000000003</v>
+      </c>
+      <c r="F44">
+        <v>-86.279117999999997</v>
+      </c>
+      <c r="G44" s="4">
+        <f>SQRT((E44-E36)^2 + (F44-F36)^2)</f>
+        <v>2.7699334876036334</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="5">
+        <f>SUM(G36:G44)</f>
+        <v>208.20663851938792</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B52">
+        <v>38.555605</v>
+      </c>
+      <c r="C52">
+        <v>-121.468926</v>
+      </c>
+      <c r="D52" s="4">
+        <f>SQRT((B52-B53)^2 + (C52-C53)^2)</f>
+        <v>16.8669151599427</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B53">
+        <v>41.145547999999998</v>
+      </c>
+      <c r="C53">
+        <v>-104.802042</v>
+      </c>
+      <c r="D53" s="4">
+        <f>SQRT((B53-B54)^2 + (C53-C54)^2)</f>
+        <v>27.940157310189253</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>40.269789000000003</v>
+      </c>
+      <c r="C54" s="6">
+        <v>-76.875613000000001</v>
+      </c>
+      <c r="D54" s="4">
+        <f>SQRT((B54-B52)^2 + (C54-C52)^2)</f>
+        <v>44.626247782015291</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="5">
+        <f>SUM(D52:D54)</f>
+        <v>89.43332025214724</v>
       </c>
     </row>
   </sheetData>
@@ -1020,4 +1889,1013 @@
     <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Classified: RMG – Internal</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:K52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="78" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3">
+        <v>9.39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H3">
+        <v>16.87</v>
+      </c>
+      <c r="J3" t="s">
+        <v>125</v>
+      </c>
+      <c r="K3">
+        <v>46.74</v>
+      </c>
+    </row>
+    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>37.25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4">
+        <v>27.94</v>
+      </c>
+      <c r="J4" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4">
+        <v>37.39</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5">
+        <v>21.69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5">
+        <v>5.87</v>
+      </c>
+      <c r="J5" t="s">
+        <v>127</v>
+      </c>
+      <c r="K5">
+        <v>14.19</v>
+      </c>
+    </row>
+    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6">
+        <v>28.81</v>
+      </c>
+      <c r="G6" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6">
+        <v>21.94</v>
+      </c>
+      <c r="J6" t="s">
+        <v>128</v>
+      </c>
+      <c r="K6">
+        <v>9.59</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>49.23</v>
+      </c>
+      <c r="G7" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7">
+        <v>22.45</v>
+      </c>
+      <c r="J7" t="s">
+        <v>129</v>
+      </c>
+      <c r="K7">
+        <v>7.58</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8">
+        <v>50.58</v>
+      </c>
+      <c r="G8" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8">
+        <v>13.23</v>
+      </c>
+      <c r="J8" t="s">
+        <v>130</v>
+      </c>
+      <c r="K8">
+        <v>38.840000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9">
+        <v>35.549999999999997</v>
+      </c>
+      <c r="G9" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9">
+        <v>7.72</v>
+      </c>
+      <c r="J9" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9">
+        <v>26.67</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10">
+        <v>7.81</v>
+      </c>
+      <c r="G10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10">
+        <v>15.32</v>
+      </c>
+      <c r="J10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11">
+        <v>27.42</v>
+      </c>
+      <c r="G11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11">
+        <v>18.78</v>
+      </c>
+      <c r="J11" t="s">
+        <v>133</v>
+      </c>
+      <c r="K11">
+        <v>6.65</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12">
+        <v>52.25</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12">
+        <v>8.14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12">
+        <v>8.84</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <v>63.92</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13">
+        <v>56.43</v>
+      </c>
+      <c r="J13" t="s">
+        <v>135</v>
+      </c>
+      <c r="K13">
+        <v>10.69</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14">
+        <v>13.61</v>
+      </c>
+      <c r="G14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14">
+        <v>17.559999999999999</v>
+      </c>
+      <c r="J14" t="s">
+        <v>136</v>
+      </c>
+      <c r="K14">
+        <v>9.61</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15">
+        <v>12.69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15">
+        <v>40.22</v>
+      </c>
+      <c r="J15" t="s">
+        <v>137</v>
+      </c>
+      <c r="K15">
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>8.43</v>
+      </c>
+      <c r="G16" t="s">
+        <v>89</v>
+      </c>
+      <c r="H16">
+        <v>14.19</v>
+      </c>
+      <c r="J16" t="s">
+        <v>138</v>
+      </c>
+      <c r="K16">
+        <v>12.32</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17">
+        <v>13.73</v>
+      </c>
+      <c r="G17" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17">
+        <v>27.58</v>
+      </c>
+      <c r="J17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K17">
+        <v>66.150000000000006</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18">
+        <v>8.84</v>
+      </c>
+      <c r="G18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H18">
+        <v>19.89</v>
+      </c>
+      <c r="J18" t="s">
+        <v>140</v>
+      </c>
+      <c r="K18">
+        <v>51.28</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19">
+        <v>7.63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19">
+        <v>12.07</v>
+      </c>
+      <c r="J19" t="s">
+        <v>141</v>
+      </c>
+      <c r="K19">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20">
+        <v>25.24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20">
+        <v>2.08</v>
+      </c>
+      <c r="J20" t="s">
+        <v>142</v>
+      </c>
+      <c r="K20">
+        <v>12.06</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21">
+        <v>16.79</v>
+      </c>
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21">
+        <v>22.76</v>
+      </c>
+      <c r="J21" t="s">
+        <v>143</v>
+      </c>
+      <c r="K21">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22">
+        <v>72.58</v>
+      </c>
+      <c r="G22" t="s">
+        <v>95</v>
+      </c>
+      <c r="H22">
+        <v>22.2</v>
+      </c>
+      <c r="J22" t="s">
+        <v>144</v>
+      </c>
+      <c r="K22">
+        <v>22.7</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23">
+        <v>47.34</v>
+      </c>
+      <c r="G23" t="s">
+        <v>96</v>
+      </c>
+      <c r="H23">
+        <v>17.32</v>
+      </c>
+      <c r="J23" t="s">
+        <v>145</v>
+      </c>
+      <c r="K23">
+        <v>9.48</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24">
+        <v>27.69</v>
+      </c>
+      <c r="G24" t="s">
+        <v>97</v>
+      </c>
+      <c r="H24">
+        <v>2.15</v>
+      </c>
+      <c r="J24" t="s">
+        <v>146</v>
+      </c>
+      <c r="K24">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25">
+        <v>33.340000000000003</v>
+      </c>
+      <c r="G25" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25">
+        <v>37.81</v>
+      </c>
+      <c r="J25" t="s">
+        <v>147</v>
+      </c>
+      <c r="K25">
+        <v>30.33</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26">
+        <v>36.49</v>
+      </c>
+      <c r="G26" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26">
+        <v>5.84</v>
+      </c>
+      <c r="J26" t="s">
+        <v>148</v>
+      </c>
+      <c r="K26">
+        <v>33.61</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>50</v>
+      </c>
+      <c r="D27">
+        <v>5.03</v>
+      </c>
+      <c r="G27" t="s">
+        <v>100</v>
+      </c>
+      <c r="H27">
+        <v>36.4</v>
+      </c>
+      <c r="J27" t="s">
+        <v>149</v>
+      </c>
+      <c r="K27">
+        <v>29.91</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28">
+        <v>25.9</v>
+      </c>
+      <c r="G28" t="s">
+        <v>101</v>
+      </c>
+      <c r="H28">
+        <v>14.4</v>
+      </c>
+      <c r="J28" t="s">
+        <v>150</v>
+      </c>
+      <c r="K28">
+        <v>9.44</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>52</v>
+      </c>
+      <c r="D29">
+        <v>24.69</v>
+      </c>
+      <c r="G29" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29">
+        <v>12.76</v>
+      </c>
+      <c r="J29" t="s">
+        <v>151</v>
+      </c>
+      <c r="K29">
+        <v>70.63</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30">
+        <v>12.29</v>
+      </c>
+      <c r="G30" t="s">
+        <v>103</v>
+      </c>
+      <c r="H30">
+        <v>17.329999999999998</v>
+      </c>
+      <c r="J30" t="s">
+        <v>152</v>
+      </c>
+      <c r="K30">
+        <v>49.88</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31">
+        <v>5.67</v>
+      </c>
+      <c r="G31" t="s">
+        <v>104</v>
+      </c>
+      <c r="H31">
+        <v>10.52</v>
+      </c>
+      <c r="J31" t="s">
+        <v>153</v>
+      </c>
+      <c r="K31">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32">
+        <v>11.73</v>
+      </c>
+      <c r="G32" t="s">
+        <v>105</v>
+      </c>
+      <c r="H32">
+        <v>16.190000000000001</v>
+      </c>
+      <c r="J32" t="s">
+        <v>154</v>
+      </c>
+      <c r="K32">
+        <v>21.32</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33">
+        <v>21.98</v>
+      </c>
+      <c r="G33" t="s">
+        <v>106</v>
+      </c>
+      <c r="H33">
+        <v>49.31</v>
+      </c>
+      <c r="J33" t="s">
+        <v>155</v>
+      </c>
+      <c r="K33">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34">
+        <v>9.32</v>
+      </c>
+      <c r="G34" t="s">
+        <v>107</v>
+      </c>
+      <c r="H34">
+        <v>46.42</v>
+      </c>
+      <c r="J34" t="s">
+        <v>156</v>
+      </c>
+      <c r="K34">
+        <v>9.6999999999999993</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35">
+        <v>9.35</v>
+      </c>
+      <c r="G35" t="s">
+        <v>108</v>
+      </c>
+      <c r="H35">
+        <v>42.32</v>
+      </c>
+      <c r="J35" t="s">
+        <v>157</v>
+      </c>
+      <c r="K35">
+        <v>27.75</v>
+      </c>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36">
+        <v>15.08</v>
+      </c>
+      <c r="G36" t="s">
+        <v>109</v>
+      </c>
+      <c r="H36">
+        <v>24.06</v>
+      </c>
+      <c r="J36" t="s">
+        <v>158</v>
+      </c>
+      <c r="K36">
+        <v>21.69</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37">
+        <v>43.25</v>
+      </c>
+      <c r="G37" t="s">
+        <v>110</v>
+      </c>
+      <c r="H37">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="J37" t="s">
+        <v>159</v>
+      </c>
+      <c r="K37">
+        <v>28.81</v>
+      </c>
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38">
+        <v>21.32</v>
+      </c>
+      <c r="G38" t="s">
+        <v>111</v>
+      </c>
+      <c r="H38">
+        <v>5.01</v>
+      </c>
+      <c r="J38" t="s">
+        <v>160</v>
+      </c>
+      <c r="K38">
+        <v>34.479999999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39">
+        <v>16.16</v>
+      </c>
+      <c r="G39" t="s">
+        <v>112</v>
+      </c>
+      <c r="H39">
+        <v>67.87</v>
+      </c>
+      <c r="J39" t="s">
+        <v>161</v>
+      </c>
+      <c r="K39">
+        <v>14.13</v>
+      </c>
+    </row>
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40">
+        <v>19.649999999999999</v>
+      </c>
+      <c r="G40" t="s">
+        <v>113</v>
+      </c>
+      <c r="H40">
+        <v>74.89</v>
+      </c>
+      <c r="J40" t="s">
+        <v>162</v>
+      </c>
+      <c r="K40">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41">
+        <v>15.74</v>
+      </c>
+      <c r="G41" t="s">
+        <v>114</v>
+      </c>
+      <c r="H41">
+        <v>31.84</v>
+      </c>
+      <c r="J41" t="s">
+        <v>163</v>
+      </c>
+      <c r="K41">
+        <v>7.27</v>
+      </c>
+    </row>
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>65</v>
+      </c>
+      <c r="D42">
+        <v>9.8800000000000008</v>
+      </c>
+      <c r="G42" t="s">
+        <v>115</v>
+      </c>
+      <c r="H42">
+        <v>46.48</v>
+      </c>
+      <c r="J42" t="s">
+        <v>164</v>
+      </c>
+      <c r="K42">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>66</v>
+      </c>
+      <c r="D43">
+        <v>29.78</v>
+      </c>
+      <c r="G43" t="s">
+        <v>116</v>
+      </c>
+      <c r="H43">
+        <v>23.34</v>
+      </c>
+      <c r="J43" t="s">
+        <v>165</v>
+      </c>
+      <c r="K43">
+        <v>8.73</v>
+      </c>
+    </row>
+    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D44">
+        <v>34.03</v>
+      </c>
+      <c r="G44" t="s">
+        <v>117</v>
+      </c>
+      <c r="H44">
+        <v>12.98</v>
+      </c>
+      <c r="J44" t="s">
+        <v>166</v>
+      </c>
+      <c r="K44">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45">
+        <v>8.15</v>
+      </c>
+      <c r="G45" t="s">
+        <v>118</v>
+      </c>
+      <c r="H45">
+        <v>21.98</v>
+      </c>
+      <c r="J45" t="s">
+        <v>167</v>
+      </c>
+      <c r="K45">
+        <v>27.58</v>
+      </c>
+    </row>
+    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>14.31</v>
+      </c>
+      <c r="G46" t="s">
+        <v>119</v>
+      </c>
+      <c r="H46">
+        <v>5.36</v>
+      </c>
+      <c r="J46" t="s">
+        <v>168</v>
+      </c>
+      <c r="K46">
+        <v>27.94</v>
+      </c>
+    </row>
+    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47">
+        <v>18.940000000000001</v>
+      </c>
+      <c r="G47" t="s">
+        <v>120</v>
+      </c>
+      <c r="H47">
+        <v>6.24</v>
+      </c>
+      <c r="J47" t="s">
+        <v>169</v>
+      </c>
+      <c r="K47">
+        <v>46.51</v>
+      </c>
+    </row>
+    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D48">
+        <v>19.07</v>
+      </c>
+      <c r="G48" t="s">
+        <v>121</v>
+      </c>
+      <c r="H48">
+        <v>22.31</v>
+      </c>
+      <c r="J48" t="s">
+        <v>170</v>
+      </c>
+      <c r="K48">
+        <v>52.09</v>
+      </c>
+    </row>
+    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="D49">
+        <v>8.18</v>
+      </c>
+      <c r="G49" t="s">
+        <v>122</v>
+      </c>
+      <c r="H49">
+        <v>8.43</v>
+      </c>
+      <c r="J49" t="s">
+        <v>171</v>
+      </c>
+      <c r="K49">
+        <v>24.87</v>
+      </c>
+    </row>
+    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+      <c r="D50">
+        <v>23.15</v>
+      </c>
+      <c r="G50" t="s">
+        <v>123</v>
+      </c>
+      <c r="H50">
+        <v>14.68</v>
+      </c>
+      <c r="J50" t="s">
+        <v>172</v>
+      </c>
+      <c r="K50">
+        <v>24.43</v>
+      </c>
+    </row>
+    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>74</v>
+      </c>
+      <c r="D51">
+        <v>53.27</v>
+      </c>
+      <c r="G51" t="s">
+        <v>124</v>
+      </c>
+      <c r="H51">
+        <v>16.03</v>
+      </c>
+      <c r="J51" t="s">
+        <v>173</v>
+      </c>
+      <c r="K51">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="H52">
+        <f>SUM(H3:H51)</f>
+        <v>1085.54</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C3:C51"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;10&amp;K000000Classified: RMG – Internal</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
optimised find_best_cycle - performing much better now
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="6990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="6990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="470">
   <si>
     <t>Kentucky</t>
   </si>
@@ -550,6 +550,894 @@
   </si>
   <si>
     <t>48 . Providence          --&gt;       49 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>0  . Pierre              --&gt;       1  . Dover               Cost</t>
+  </si>
+  <si>
+    <t>1  . Dover               --&gt;       2  . Boise               Cost</t>
+  </si>
+  <si>
+    <t>2  . Boise               --&gt;       3  . Austin              Cost</t>
+  </si>
+  <si>
+    <t>3  . Austin              --&gt;       4  . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>4  . Salt Lake City      --&gt;       5  . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>5  . Montpelier          --&gt;       6  . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>6  . Richmond            --&gt;       7  . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>7  . Olympia             --&gt;       8  . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>8  . Charleston          --&gt;       9  . Madison             Cost</t>
+  </si>
+  <si>
+    <t>9  . Madison             --&gt;       10 . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>10 . Cheyenne            --&gt;       11 . Salem               Cost</t>
+  </si>
+  <si>
+    <t>11 . Salem               --&gt;       12 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>12 . Juneau              --&gt;       13 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>13 . Columbia            --&gt;       14 . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>14 . Little Rock         --&gt;       15 . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>15 . Sacramento          --&gt;       16 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>16 . Denver              --&gt;       17 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>17 . Hartford            --&gt;       18 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>18 . Baton Rouge         --&gt;       19 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>19 . Tallahassee         --&gt;       20 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>20 . Atlanta             --&gt;       21 . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>21 . Honolulu            --&gt;       22 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>22 . Nashville           --&gt;       23 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>23 . Springfield         --&gt;       24 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>24 . Indianapolis        --&gt;       25 . Boston              Cost</t>
+  </si>
+  <si>
+    <t>25 . Boston              --&gt;       26 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>26 . Topeka              --&gt;       27 . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>27 . Frankfort           --&gt;       28 . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>28 . Harrisburg          --&gt;       29 . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>29 . Carson City         --&gt;       30 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>30 . Annapolis           --&gt;       31 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>31 . Oklahoma City       --&gt;       32 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>32 . Lansing             --&gt;       33 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>33 . Saint Paul          --&gt;       34 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>34 . Jackson             --&gt;       35 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>35 . Jefferson City      --&gt;       36 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>36 . Helana              --&gt;       37 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>37 . Lincoln             --&gt;       38 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>38 . Augusta             --&gt;       39 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>39 . Concord             --&gt;       40 . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>40 . Trenton             --&gt;       41 . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>41 . Santa Fe            --&gt;       42 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>42 . Albany              --&gt;       43 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>43 . Raleigh             --&gt;       44 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>44 . Bismarck            --&gt;       45 . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>45 . Columbus            --&gt;       46 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>46 . Des Moines          --&gt;       47 . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>47 . Montgomery          --&gt;       48 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>48 . Providence          --&gt;       49 . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>0  . Olympia             --&gt;       1  . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>1  . Charleston          --&gt;       2  . Madison             Cost</t>
+  </si>
+  <si>
+    <t>2  . Madison             --&gt;       3  . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>3  . Cheyenne            --&gt;       4  . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>4  . Montgomery          --&gt;       5  . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>5  . Tallahassee         --&gt;       6  . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>6  . Phoenix             --&gt;       7  . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>7  . Little Rock         --&gt;       8  . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>8  . Sacramento          --&gt;       9  . Denver              Cost</t>
+  </si>
+  <si>
+    <t>9  . Denver              --&gt;       10 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>10 . Hartford            --&gt;       11 . Dover               Cost</t>
+  </si>
+  <si>
+    <t>11 . Dover               --&gt;       12 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>12 . Nashville           --&gt;       13 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>13 . Atlanta             --&gt;       14 . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>14 . Honolulu            --&gt;       15 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>15 . Richmond            --&gt;       16 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>16 . Springfield         --&gt;       17 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>17 . Indianapolis        --&gt;       18 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>18 . Des Moines          --&gt;       19 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>19 . Topeka              --&gt;       20 . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>20 . Frankfort           --&gt;       21 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>21 . Baton Rouge         --&gt;       22 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>22 . Augusta             --&gt;       23 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>23 . Annapolis           --&gt;       24 . Boston              Cost</t>
+  </si>
+  <si>
+    <t>24 . Boston              --&gt;       25 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>25 . Lansing             --&gt;       26 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>26 . Saint Paul          --&gt;       27 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>27 . Jackson             --&gt;       28 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>28 . Jefferson City      --&gt;       29 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>29 . Helana              --&gt;       30 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>30 . Lincoln             --&gt;       31 . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>31 . Carson City         --&gt;       32 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>32 . Concord             --&gt;       33 . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>33 . Trenton             --&gt;       34 . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>34 . Santa Fe            --&gt;       35 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>35 . Albany              --&gt;       36 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>36 . Raleigh             --&gt;       37 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>37 . Bismarck            --&gt;       38 . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>38 . Columbus            --&gt;       39 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>39 . Oklahoma City       --&gt;       40 . Austin              Cost</t>
+  </si>
+  <si>
+    <t>40 . Austin              --&gt;       41 . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>41 . Harrisburg          --&gt;       42 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>42 . Providence          --&gt;       43 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>43 . Columbia            --&gt;       44 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>44 . Pierre              --&gt;       45 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>45 . Juneau              --&gt;       46 . Salem               Cost</t>
+  </si>
+  <si>
+    <t>46 . Salem               --&gt;       47 . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>47 . Salt Lake City      --&gt;       48 . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>48 . Montpelier          --&gt;       49 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>0  . Des Moines          --&gt;       1  . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>1  . Phoenix             --&gt;       2  . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>2  . Honolulu            --&gt;       3  . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>3  . Columbus            --&gt;       4  . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>4  . Little Rock         --&gt;       5  . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>5  . Trenton             --&gt;       6  . Concord             Cost</t>
+  </si>
+  <si>
+    <t>6  . Concord             --&gt;       7  . Providence          Cost</t>
+  </si>
+  <si>
+    <t>7  . Providence          --&gt;       8  . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>8  . Topeka              --&gt;       9  . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>9  . Bismarck            --&gt;       10 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>10 . Boise               --&gt;       11 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>11 . Lincoln             --&gt;       12 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>12 . Indianapolis        --&gt;       13 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>13 . Lansing             --&gt;       14 . Salem               Cost</t>
+  </si>
+  <si>
+    <t>14 . Salem               --&gt;       15 . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>15 . Olympia             --&gt;       16 . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>16 . Montgomery          --&gt;       17 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>17 . Atlanta             --&gt;       18 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>18 . Springfield         --&gt;       19 . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>19 . Frankfort           --&gt;       20 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>20 . Richmond            --&gt;       21 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>21 . Baton Rouge         --&gt;       22 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>22 . Saint Paul          --&gt;       23 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>23 . Jefferson City      --&gt;       24 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>24 . Raleigh             --&gt;       25 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>25 . Hartford            --&gt;       26 . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>26 . Harrisburg          --&gt;       27 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>27 . Columbia            --&gt;       28 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>28 . Juneau              --&gt;       29 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>29 . Denver              --&gt;       30 . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>30 . Cheyenne            --&gt;       31 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>31 . Helana              --&gt;       32 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>32 . Pierre              --&gt;       33 . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>33 . Sacramento          --&gt;       34 . Boston              Cost</t>
+  </si>
+  <si>
+    <t>34 . Boston              --&gt;       35 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>35 . Augusta             --&gt;       36 . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>36 . Montpelier          --&gt;       37 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>37 . Jackson             --&gt;       38 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>38 . Albany              --&gt;       39 . Dover               Cost</t>
+  </si>
+  <si>
+    <t>39 . Dover               --&gt;       40 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>40 . Nashville           --&gt;       41 . Austin              Cost</t>
+  </si>
+  <si>
+    <t>41 . Austin              --&gt;       42 . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>42 . Santa Fe            --&gt;       43 . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>43 . Carson City         --&gt;       44 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>44 . Annapolis           --&gt;       45 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>45 . Tallahassee         --&gt;       46 . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>46 . Charleston          --&gt;       47 . Madison             Cost</t>
+  </si>
+  <si>
+    <t>47 . Madison             --&gt;       48 . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>48 . Salt Lake City      --&gt;       49 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>0  . Raleigh             --&gt;       1  . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>1  . Salt Lake City      --&gt;       2  . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>2  . Charleston          --&gt;       3  . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>3  . Hartford            --&gt;       4  . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>4  . Trenton             --&gt;       5  . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>5  . Columbia            --&gt;       6  . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>6  . Augusta             --&gt;       7  . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>7  . Montpelier          --&gt;       8  . Boston              Cost</t>
+  </si>
+  <si>
+    <t>8  . Boston              --&gt;       9  . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>9  . Columbus            --&gt;       10 . Madison             Cost</t>
+  </si>
+  <si>
+    <t>10 . Madison             --&gt;       11 . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>11 . Montgomery          --&gt;       12 . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>12 . Phoenix             --&gt;       13 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>13 . Denver              --&gt;       14 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>14 . Boise               --&gt;       15 . Austin              Cost</t>
+  </si>
+  <si>
+    <t>15 . Austin              --&gt;       16 . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>16 . Cheyenne            --&gt;       17 . Salem               Cost</t>
+  </si>
+  <si>
+    <t>17 . Salem               --&gt;       18 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>18 . Springfield         --&gt;       19 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>19 . Baton Rouge         --&gt;       20 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>20 . Tallahassee         --&gt;       21 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>21 . Atlanta             --&gt;       22 . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>22 . Frankfort           --&gt;       23 . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>23 . Honolulu            --&gt;       24 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>24 . Juneau              --&gt;       25 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>25 . Pierre              --&gt;       26 . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>26 . Little Rock         --&gt;       27 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>27 . Nashville           --&gt;       28 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>28 . Bismarck            --&gt;       29 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>29 . Annapolis           --&gt;       30 . Dover               Cost</t>
+  </si>
+  <si>
+    <t>30 . Dover               --&gt;       31 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>31 . Jefferson City      --&gt;       32 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>32 . Topeka              --&gt;       33 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>33 . Lincoln             --&gt;       34 . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>34 . Carson City         --&gt;       35 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>35 . Concord             --&gt;       36 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>36 . Richmond            --&gt;       37 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>37 . Oklahoma City       --&gt;       38 . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>38 . Santa Fe            --&gt;       39 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>39 . Indianapolis        --&gt;       40 . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>40 . Sacramento          --&gt;       41 . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>41 . Olympia             --&gt;       42 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>42 . Des Moines          --&gt;       43 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>43 . Saint Paul          --&gt;       44 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>44 . Lansing             --&gt;       45 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>45 . Helana              --&gt;       46 . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>46 . Harrisburg          --&gt;       47 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>47 . Jackson             --&gt;       48 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>48 . Providence          --&gt;       49 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>0  . Providence          --&gt;       1  . Boston              Cost</t>
+  </si>
+  <si>
+    <t>1  . Boston              --&gt;       2  . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>2  . Montgomery          --&gt;       3  . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>3  . Montpelier          --&gt;       4  . Salem               Cost</t>
+  </si>
+  <si>
+    <t>4  . Salem               --&gt;       5  . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>5  . Honolulu            --&gt;       6  . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>6  . Sacramento          --&gt;       7  . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>7  . Cheyenne            --&gt;       8  . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>8  . Charleston          --&gt;       9  . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>9  . Phoenix             --&gt;       10 . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>10 . Salt Lake City      --&gt;       11 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>11 . Springfield         --&gt;       12 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>12 . Columbia            --&gt;       13 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>13 . Raleigh             --&gt;       14 . Dover               Cost</t>
+  </si>
+  <si>
+    <t>14 . Dover               --&gt;       15 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>15 . Tallahassee         --&gt;       16 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>16 . Hartford            --&gt;       17 . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>17 . Frankfort           --&gt;       18 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>18 . Oklahoma City       --&gt;       19 . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>19 . Harrisburg          --&gt;       20 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>20 . Augusta             --&gt;       21 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>21 . Concord             --&gt;       22 . Madison             Cost</t>
+  </si>
+  <si>
+    <t>22 . Madison             --&gt;       23 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>23 . Atlanta             --&gt;       24 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>24 . Richmond            --&gt;       25 . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>25 . Trenton             --&gt;       26 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>26 . Nashville           --&gt;       27 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>27 . Jefferson City      --&gt;       28 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>28 . Denver              --&gt;       29 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>29 . Lansing             --&gt;       30 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>30 . Bismarck            --&gt;       31 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>31 . Lincoln             --&gt;       32 . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>32 . Santa Fe            --&gt;       33 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>33 . Des Moines          --&gt;       34 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>34 . Pierre              --&gt;       35 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>35 . Saint Paul          --&gt;       36 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>36 . Baton Rouge         --&gt;       37 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>37 . Jackson             --&gt;       38 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>38 . Boise               --&gt;       39 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>39 . Helana              --&gt;       40 . Austin              Cost</t>
+  </si>
+  <si>
+    <t>40 . Austin              --&gt;       41 . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>41 . Carson City         --&gt;       42 . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>42 . Olympia             --&gt;       43 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>43 . Topeka              --&gt;       44 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>44 . Annapolis           --&gt;       45 . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>45 . Columbus            --&gt;       46 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>46 . Indianapolis        --&gt;       47 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>47 . Juneau              --&gt;       48 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>48 . Albany              --&gt;       49 . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>49 . Little Rock         --&gt;       0  . Providence          Cost</t>
+  </si>
+  <si>
+    <t>0  . Dover               --&gt;       1  . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>1  . Annapolis           --&gt;       2  . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>2  . Cheyenne            --&gt;       3  . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>3  . Olympia             --&gt;       4  . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>4  . Carson City         --&gt;       5  . Salem               Cost</t>
+  </si>
+  <si>
+    <t>5  . Salem               --&gt;       6  . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>6  . Juneau              --&gt;       7  . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>7  . Harrisburg          --&gt;       8  . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>8  . Montgomery          --&gt;       9  . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>9  . Richmond            --&gt;       10 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>10 . Lansing             --&gt;       11 . Madison             Cost</t>
+  </si>
+  <si>
+    <t>11 . Madison             --&gt;       12 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>12 . Des Moines          --&gt;       13 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>13 . Albany              --&gt;       14 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>14 . Denver              --&gt;       15 . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>15 . Phoenix             --&gt;       16 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>16 . Raleigh             --&gt;       17 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>17 . Baton Rouge         --&gt;       18 . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>18 . Trenton             --&gt;       19 . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>19 . Charleston          --&gt;       20 . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>20 . Little Rock         --&gt;       21 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>21 . Jackson             --&gt;       22 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>22 . Tallahassee         --&gt;       23 . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>23 . Columbus            --&gt;       24 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>24 . Atlanta             --&gt;       25 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>25 . Oklahoma City       --&gt;       26 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>26 . Topeka              --&gt;       27 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>27 . Boise               --&gt;       28 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>28 . Pierre              --&gt;       29 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>29 . Lincoln             --&gt;       30 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>30 . Jefferson City      --&gt;       31 . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>31 . Salt Lake City      --&gt;       32 . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>32 . Honolulu            --&gt;       33 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>33 . Saint Paul          --&gt;       34 . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>34 . Santa Fe            --&gt;       35 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>35 . Springfield         --&gt;       36 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>36 . Bismarck            --&gt;       37 . Austin              Cost</t>
+  </si>
+  <si>
+    <t>37 . Austin              --&gt;       38 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>38 . Columbia            --&gt;       39 . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>39 . Montpelier          --&gt;       40 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>40 . Indianapolis        --&gt;       41 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>41 . Concord             --&gt;       42 . Boston              Cost</t>
+  </si>
+  <si>
+    <t>42 . Boston              --&gt;       43 . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>43 . Frankfort           --&gt;       44 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>44 . Helana              --&gt;       45 . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>45 . Sacramento          --&gt;       46 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>46 . Nashville           --&gt;       47 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>47 . Providence          --&gt;       48 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>48 . Hartford            --&gt;       49 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>49 . Augusta             --&gt;       0  . Dover               Cost</t>
   </si>
 </sst>
 </file>
@@ -557,7 +1445,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -608,16 +1496,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -934,8 +1823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P55"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1893,10 +2782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:K52"/>
+  <dimension ref="C3:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AB23" sqref="AB23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,7 +2793,7 @@
     <col min="3" max="3" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>26</v>
       </c>
@@ -1923,8 +2812,44 @@
       <c r="K3">
         <v>46.74</v>
       </c>
-    </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>174</v>
+      </c>
+      <c r="N3">
+        <v>25.35</v>
+      </c>
+      <c r="P3" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q3">
+        <v>42.17</v>
+      </c>
+      <c r="S3" t="s">
+        <v>272</v>
+      </c>
+      <c r="T3">
+        <v>20.170000000000002</v>
+      </c>
+      <c r="V3" t="s">
+        <v>321</v>
+      </c>
+      <c r="W3">
+        <v>33.630000000000003</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>370</v>
+      </c>
+      <c r="Z3">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>420</v>
+      </c>
+      <c r="AC3">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="4" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>27</v>
       </c>
@@ -1943,8 +2868,44 @@
       <c r="K4">
         <v>37.39</v>
       </c>
-    </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>175</v>
+      </c>
+      <c r="N4">
+        <v>40.950000000000003</v>
+      </c>
+      <c r="P4" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q4">
+        <v>9.08</v>
+      </c>
+      <c r="S4" t="s">
+        <v>273</v>
+      </c>
+      <c r="T4">
+        <v>47.34</v>
+      </c>
+      <c r="V4" t="s">
+        <v>322</v>
+      </c>
+      <c r="W4">
+        <v>30.35</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>371</v>
+      </c>
+      <c r="Z4">
+        <v>18.170000000000002</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>421</v>
+      </c>
+      <c r="AC4">
+        <v>28.38</v>
+      </c>
+    </row>
+    <row r="5" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>28</v>
       </c>
@@ -1963,8 +2924,44 @@
       <c r="K5">
         <v>14.19</v>
       </c>
-    </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>176</v>
+      </c>
+      <c r="N5">
+        <v>22.8</v>
+      </c>
+      <c r="P5" t="s">
+        <v>225</v>
+      </c>
+      <c r="Q5">
+        <v>15.54</v>
+      </c>
+      <c r="S5" t="s">
+        <v>274</v>
+      </c>
+      <c r="T5">
+        <v>77.12</v>
+      </c>
+      <c r="V5" t="s">
+        <v>323</v>
+      </c>
+      <c r="W5">
+        <v>9.59</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>372</v>
+      </c>
+      <c r="Z5">
+        <v>18.16</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>422</v>
+      </c>
+      <c r="AC5">
+        <v>19.03</v>
+      </c>
+    </row>
+    <row r="6" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>29</v>
       </c>
@@ -1983,8 +2980,44 @@
       <c r="K6">
         <v>9.59</v>
       </c>
-    </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>177</v>
+      </c>
+      <c r="N6">
+        <v>17.61</v>
+      </c>
+      <c r="P6" t="s">
+        <v>226</v>
+      </c>
+      <c r="Q6">
+        <v>20.5</v>
+      </c>
+      <c r="S6" t="s">
+        <v>275</v>
+      </c>
+      <c r="T6">
+        <v>10.69</v>
+      </c>
+      <c r="V6" t="s">
+        <v>324</v>
+      </c>
+      <c r="W6">
+        <v>2.59</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>373</v>
+      </c>
+      <c r="Z6">
+        <v>50.46</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>423</v>
+      </c>
+      <c r="AC6">
+        <v>8.48</v>
+      </c>
+    </row>
+    <row r="7" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>30</v>
       </c>
@@ -2003,8 +3036,44 @@
       <c r="K7">
         <v>7.58</v>
       </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>178</v>
+      </c>
+      <c r="N7">
+        <v>39.479999999999997</v>
+      </c>
+      <c r="P7" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q7">
+        <v>2.77</v>
+      </c>
+      <c r="S7" t="s">
+        <v>276</v>
+      </c>
+      <c r="T7">
+        <v>18.41</v>
+      </c>
+      <c r="V7" t="s">
+        <v>325</v>
+      </c>
+      <c r="W7">
+        <v>8.84</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>374</v>
+      </c>
+      <c r="Z7">
+        <v>42.06</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>424</v>
+      </c>
+      <c r="AC7">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="8" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>31</v>
       </c>
@@ -2023,8 +3092,44 @@
       <c r="K8">
         <v>38.840000000000003</v>
       </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>179</v>
+      </c>
+      <c r="N8">
+        <v>8.31</v>
+      </c>
+      <c r="P8" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q8">
+        <v>27.96</v>
+      </c>
+      <c r="S8" t="s">
+        <v>277</v>
+      </c>
+      <c r="T8">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="V8" t="s">
+        <v>326</v>
+      </c>
+      <c r="W8">
+        <v>15.28</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>375</v>
+      </c>
+      <c r="Z8">
+        <v>40.24</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>425</v>
+      </c>
+      <c r="AC8">
+        <v>17.559999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>32</v>
       </c>
@@ -2043,8 +3148,44 @@
       <c r="K9">
         <v>26.67</v>
       </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>180</v>
+      </c>
+      <c r="N9">
+        <v>46.42</v>
+      </c>
+      <c r="P9" t="s">
+        <v>229</v>
+      </c>
+      <c r="Q9">
+        <v>19.78</v>
+      </c>
+      <c r="S9" t="s">
+        <v>278</v>
+      </c>
+      <c r="T9">
+        <v>1.4</v>
+      </c>
+      <c r="V9" t="s">
+        <v>327</v>
+      </c>
+      <c r="W9">
+        <v>2.81</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>376</v>
+      </c>
+      <c r="Z9">
+        <v>16.87</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>426</v>
+      </c>
+      <c r="AC9">
+        <v>60.3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>33</v>
       </c>
@@ -2063,8 +3204,44 @@
       <c r="K10">
         <v>12.1</v>
       </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>181</v>
+      </c>
+      <c r="N10">
+        <v>42.17</v>
+      </c>
+      <c r="P10" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q10">
+        <v>29.39</v>
+      </c>
+      <c r="S10" t="s">
+        <v>279</v>
+      </c>
+      <c r="T10">
+        <v>24.43</v>
+      </c>
+      <c r="V10" t="s">
+        <v>328</v>
+      </c>
+      <c r="W10">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>377</v>
+      </c>
+      <c r="Z10">
+        <v>23.34</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>427</v>
+      </c>
+      <c r="AC10">
+        <v>12.29</v>
+      </c>
+    </row>
+    <row r="11" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>34</v>
       </c>
@@ -2083,8 +3260,44 @@
       <c r="K11">
         <v>6.65</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>182</v>
+      </c>
+      <c r="N11">
+        <v>9.08</v>
+      </c>
+      <c r="P11" t="s">
+        <v>231</v>
+      </c>
+      <c r="Q11">
+        <v>16.53</v>
+      </c>
+      <c r="S11" t="s">
+        <v>280</v>
+      </c>
+      <c r="T11">
+        <v>11.02</v>
+      </c>
+      <c r="V11" t="s">
+        <v>329</v>
+      </c>
+      <c r="W11">
+        <v>12.19</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>378</v>
+      </c>
+      <c r="Z11">
+        <v>30.83</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>428</v>
+      </c>
+      <c r="AC11">
+        <v>10.23</v>
+      </c>
+    </row>
+    <row r="12" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -2103,8 +3316,44 @@
       <c r="K12">
         <v>8.84</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>183</v>
+      </c>
+      <c r="N12">
+        <v>15.54</v>
+      </c>
+      <c r="P12" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q12">
+        <v>32.369999999999997</v>
+      </c>
+      <c r="S12" t="s">
+        <v>281</v>
+      </c>
+      <c r="T12">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="V12" t="s">
+        <v>330</v>
+      </c>
+      <c r="W12">
+        <v>7.1</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>379</v>
+      </c>
+      <c r="Z12">
+        <v>7.31</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>429</v>
+      </c>
+      <c r="AC12">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="13" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>36</v>
       </c>
@@ -2123,8 +3372,44 @@
       <c r="K13">
         <v>10.69</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>184</v>
+      </c>
+      <c r="N13">
+        <v>18.62</v>
+      </c>
+      <c r="P13" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q13">
+        <v>3.86</v>
+      </c>
+      <c r="S13" t="s">
+        <v>282</v>
+      </c>
+      <c r="T13">
+        <v>19.760000000000002</v>
+      </c>
+      <c r="V13" t="s">
+        <v>331</v>
+      </c>
+      <c r="W13">
+        <v>11.15</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>380</v>
+      </c>
+      <c r="Z13">
+        <v>22.26</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>430</v>
+      </c>
+      <c r="AC13">
+        <v>4.8499999999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>37</v>
       </c>
@@ -2143,8 +3428,44 @@
       <c r="K14">
         <v>9.61</v>
       </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>185</v>
+      </c>
+      <c r="N14">
+        <v>17.559999999999999</v>
+      </c>
+      <c r="P14" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q14">
+        <v>11.65</v>
+      </c>
+      <c r="S14" t="s">
+        <v>283</v>
+      </c>
+      <c r="T14">
+        <v>10.58</v>
+      </c>
+      <c r="V14" t="s">
+        <v>332</v>
+      </c>
+      <c r="W14">
+        <v>25.82</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>381</v>
+      </c>
+      <c r="Z14">
+        <v>10.38</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>431</v>
+      </c>
+      <c r="AC14">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="15" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>38</v>
       </c>
@@ -2163,8 +3484,44 @@
       <c r="K15">
         <v>8.43</v>
       </c>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>186</v>
+      </c>
+      <c r="N15">
+        <v>58.66</v>
+      </c>
+      <c r="P15" t="s">
+        <v>235</v>
+      </c>
+      <c r="Q15">
+        <v>3.39</v>
+      </c>
+      <c r="S15" t="s">
+        <v>284</v>
+      </c>
+      <c r="T15">
+        <v>3.35</v>
+      </c>
+      <c r="V15" t="s">
+        <v>333</v>
+      </c>
+      <c r="W15">
+        <v>9.48</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>382</v>
+      </c>
+      <c r="Z15">
+        <v>2.98</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>432</v>
+      </c>
+      <c r="AC15">
+        <v>19.87</v>
+      </c>
+    </row>
+    <row r="16" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -2183,8 +3540,44 @@
       <c r="K16">
         <v>12.32</v>
       </c>
-    </row>
-    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>187</v>
+      </c>
+      <c r="N16">
+        <v>11.32</v>
+      </c>
+      <c r="P16" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q16">
+        <v>74.48</v>
+      </c>
+      <c r="S16" t="s">
+        <v>285</v>
+      </c>
+      <c r="T16">
+        <v>38.549999999999997</v>
+      </c>
+      <c r="V16" t="s">
+        <v>334</v>
+      </c>
+      <c r="W16">
+        <v>11.9</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z16">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>433</v>
+      </c>
+      <c r="AC16">
+        <v>31.34</v>
+      </c>
+    </row>
+    <row r="17" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>40</v>
       </c>
@@ -2203,8 +3596,44 @@
       <c r="K17">
         <v>66.150000000000006</v>
       </c>
-    </row>
-    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>188</v>
+      </c>
+      <c r="N17">
+        <v>29.39</v>
+      </c>
+      <c r="P17" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q17">
+        <v>81.99</v>
+      </c>
+      <c r="S17" t="s">
+        <v>286</v>
+      </c>
+      <c r="T17">
+        <v>2.12</v>
+      </c>
+      <c r="V17" t="s">
+        <v>335</v>
+      </c>
+      <c r="W17">
+        <v>22.8</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z17">
+        <v>12.34</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>434</v>
+      </c>
+      <c r="AC17">
+        <v>9.48</v>
+      </c>
+    </row>
+    <row r="18" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>41</v>
       </c>
@@ -2223,8 +3652,44 @@
       <c r="K18">
         <v>51.28</v>
       </c>
-    </row>
-    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>189</v>
+      </c>
+      <c r="N18">
+        <v>16.53</v>
+      </c>
+      <c r="P18" t="s">
+        <v>238</v>
+      </c>
+      <c r="Q18">
+        <v>12.4</v>
+      </c>
+      <c r="S18" t="s">
+        <v>287</v>
+      </c>
+      <c r="T18">
+        <v>39.450000000000003</v>
+      </c>
+      <c r="V18" t="s">
+        <v>336</v>
+      </c>
+      <c r="W18">
+        <v>12.96</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>385</v>
+      </c>
+      <c r="Z18">
+        <v>16.2</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>435</v>
+      </c>
+      <c r="AC18">
+        <v>33.520000000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>42</v>
       </c>
@@ -2243,8 +3708,44 @@
       <c r="K19">
         <v>6.56</v>
       </c>
-    </row>
-    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>190</v>
+      </c>
+      <c r="N19">
+        <v>32.369999999999997</v>
+      </c>
+      <c r="P19" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q19">
+        <v>3.5</v>
+      </c>
+      <c r="S19" t="s">
+        <v>288</v>
+      </c>
+      <c r="T19">
+        <v>2.35</v>
+      </c>
+      <c r="V19" t="s">
+        <v>337</v>
+      </c>
+      <c r="W19">
+        <v>18.62</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>386</v>
+      </c>
+      <c r="Z19">
+        <v>12.7</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>436</v>
+      </c>
+      <c r="AC19">
+        <v>13.58</v>
+      </c>
+    </row>
+    <row r="20" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>43</v>
       </c>
@@ -2263,8 +3764,44 @@
       <c r="K20">
         <v>12.06</v>
       </c>
-    </row>
-    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>191</v>
+      </c>
+      <c r="N20">
+        <v>21.65</v>
+      </c>
+      <c r="P20" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q20">
+        <v>7.69</v>
+      </c>
+      <c r="S20" t="s">
+        <v>289</v>
+      </c>
+      <c r="T20">
+        <v>8</v>
+      </c>
+      <c r="V20" t="s">
+        <v>338</v>
+      </c>
+      <c r="W20">
+        <v>33.770000000000003</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>387</v>
+      </c>
+      <c r="Z20">
+        <v>12.96</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>437</v>
+      </c>
+      <c r="AC20">
+        <v>19.07</v>
+      </c>
+    </row>
+    <row r="21" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>44</v>
       </c>
@@ -2283,8 +3820,44 @@
       <c r="K21">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>192</v>
+      </c>
+      <c r="N21">
+        <v>6.87</v>
+      </c>
+      <c r="P21" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q21">
+        <v>3.28</v>
+      </c>
+      <c r="S21" t="s">
+        <v>290</v>
+      </c>
+      <c r="T21">
+        <v>5.04</v>
+      </c>
+      <c r="V21" t="s">
+        <v>339</v>
+      </c>
+      <c r="W21">
+        <v>9.44</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z21">
+        <v>21.21</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>438</v>
+      </c>
+      <c r="AC21">
+        <v>7.13</v>
+      </c>
+    </row>
+    <row r="22" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>45</v>
       </c>
@@ -2303,8 +3876,44 @@
       <c r="K22">
         <v>22.7</v>
       </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>193</v>
+      </c>
+      <c r="N22">
+        <v>3.31</v>
+      </c>
+      <c r="P22" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q22">
+        <v>10.86</v>
+      </c>
+      <c r="S22" t="s">
+        <v>291</v>
+      </c>
+      <c r="T22">
+        <v>7.43</v>
+      </c>
+      <c r="V22" t="s">
+        <v>340</v>
+      </c>
+      <c r="W22">
+        <v>6.87</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>389</v>
+      </c>
+      <c r="Z22">
+        <v>8.18</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>439</v>
+      </c>
+      <c r="AC22">
+        <v>11.29</v>
+      </c>
+    </row>
+    <row r="23" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>46</v>
       </c>
@@ -2323,8 +3932,44 @@
       <c r="K23">
         <v>9.48</v>
       </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>194</v>
+      </c>
+      <c r="N23">
+        <v>74.48</v>
+      </c>
+      <c r="P23" t="s">
+        <v>243</v>
+      </c>
+      <c r="Q23">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="S23" t="s">
+        <v>292</v>
+      </c>
+      <c r="T23">
+        <v>15.4</v>
+      </c>
+      <c r="V23" t="s">
+        <v>341</v>
+      </c>
+      <c r="W23">
+        <v>3.31</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>390</v>
+      </c>
+      <c r="Z23">
+        <v>2.1</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>440</v>
+      </c>
+      <c r="AC23">
+        <v>3.22</v>
+      </c>
+    </row>
+    <row r="24" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>47</v>
       </c>
@@ -2343,8 +3988,44 @@
       <c r="K24">
         <v>10.99</v>
       </c>
-    </row>
-    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>195</v>
+      </c>
+      <c r="N24">
+        <v>72.58</v>
+      </c>
+      <c r="P24" t="s">
+        <v>244</v>
+      </c>
+      <c r="Q24">
+        <v>25.48</v>
+      </c>
+      <c r="S24" t="s">
+        <v>293</v>
+      </c>
+      <c r="T24">
+        <v>14.62</v>
+      </c>
+      <c r="V24" t="s">
+        <v>342</v>
+      </c>
+      <c r="W24">
+        <v>4.46</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>391</v>
+      </c>
+      <c r="Z24">
+        <v>17.84</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>441</v>
+      </c>
+      <c r="AC24">
+        <v>6.22</v>
+      </c>
+    </row>
+    <row r="25" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>48</v>
       </c>
@@ -2363,8 +4044,44 @@
       <c r="K25">
         <v>30.33</v>
       </c>
-    </row>
-    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>196</v>
+      </c>
+      <c r="N25">
+        <v>4.62</v>
+      </c>
+      <c r="P25" t="s">
+        <v>245</v>
+      </c>
+      <c r="Q25">
+        <v>8.6</v>
+      </c>
+      <c r="S25" t="s">
+        <v>294</v>
+      </c>
+      <c r="T25">
+        <v>6.44</v>
+      </c>
+      <c r="V25" t="s">
+        <v>343</v>
+      </c>
+      <c r="W25">
+        <v>74.89</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>392</v>
+      </c>
+      <c r="Z25">
+        <v>10.57</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>442</v>
+      </c>
+      <c r="AC25">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="26" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>49</v>
       </c>
@@ -2383,8 +4100,44 @@
       <c r="K26">
         <v>33.61</v>
       </c>
-    </row>
-    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>197</v>
+      </c>
+      <c r="N26">
+        <v>3.5</v>
+      </c>
+      <c r="P26" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q26">
+        <v>6.37</v>
+      </c>
+      <c r="S26" t="s">
+        <v>295</v>
+      </c>
+      <c r="T26">
+        <v>13.84</v>
+      </c>
+      <c r="V26" t="s">
+        <v>344</v>
+      </c>
+      <c r="W26">
+        <v>43.78</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>393</v>
+      </c>
+      <c r="Z26">
+        <v>7.89</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>443</v>
+      </c>
+      <c r="AC26">
+        <v>6.36</v>
+      </c>
+    </row>
+    <row r="27" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>50</v>
       </c>
@@ -2403,8 +4156,44 @@
       <c r="K27">
         <v>29.91</v>
       </c>
-    </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>198</v>
+      </c>
+      <c r="N27">
+        <v>15.32</v>
+      </c>
+      <c r="P27" t="s">
+        <v>247</v>
+      </c>
+      <c r="Q27">
+        <v>13.53</v>
+      </c>
+      <c r="S27" t="s">
+        <v>296</v>
+      </c>
+      <c r="T27">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="V27" t="s">
+        <v>345</v>
+      </c>
+      <c r="W27">
+        <v>36.82</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>394</v>
+      </c>
+      <c r="Z27">
+        <v>3.81</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>444</v>
+      </c>
+      <c r="AC27">
+        <v>13.26</v>
+      </c>
+    </row>
+    <row r="28" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>51</v>
       </c>
@@ -2423,8 +4212,44 @@
       <c r="K28">
         <v>9.44</v>
       </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>199</v>
+      </c>
+      <c r="N28">
+        <v>24.87</v>
+      </c>
+      <c r="P28" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q28">
+        <v>8.83</v>
+      </c>
+      <c r="S28" t="s">
+        <v>297</v>
+      </c>
+      <c r="T28">
+        <v>4.46</v>
+      </c>
+      <c r="V28" t="s">
+        <v>346</v>
+      </c>
+      <c r="W28">
+        <v>12.52</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>395</v>
+      </c>
+      <c r="Z28">
+        <v>12.69</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>445</v>
+      </c>
+      <c r="AC28">
+        <v>4.01</v>
+      </c>
+    </row>
+    <row r="29" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>52</v>
       </c>
@@ -2443,8 +4268,44 @@
       <c r="K29">
         <v>70.63</v>
       </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>200</v>
+      </c>
+      <c r="N29">
+        <v>10.86</v>
+      </c>
+      <c r="P29" t="s">
+        <v>249</v>
+      </c>
+      <c r="Q29">
+        <v>12.96</v>
+      </c>
+      <c r="S29" t="s">
+        <v>298</v>
+      </c>
+      <c r="T29">
+        <v>7.52</v>
+      </c>
+      <c r="V29" t="s">
+        <v>347</v>
+      </c>
+      <c r="W29">
+        <v>5.73</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z29">
+        <v>5.92</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>446</v>
+      </c>
+      <c r="AC29">
+        <v>21.05</v>
+      </c>
+    </row>
+    <row r="30" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>53</v>
       </c>
@@ -2463,8 +4324,44 @@
       <c r="K30">
         <v>49.88</v>
       </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>201</v>
+      </c>
+      <c r="N30">
+        <v>8.25</v>
+      </c>
+      <c r="P30" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q30">
+        <v>6.56</v>
+      </c>
+      <c r="S30" t="s">
+        <v>299</v>
+      </c>
+      <c r="T30">
+        <v>58.66</v>
+      </c>
+      <c r="V30" t="s">
+        <v>348</v>
+      </c>
+      <c r="W30">
+        <v>18.86</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>397</v>
+      </c>
+      <c r="Z30">
+        <v>12.85</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>447</v>
+      </c>
+      <c r="AC30">
+        <v>15.92</v>
+      </c>
+    </row>
+    <row r="31" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>54</v>
       </c>
@@ -2483,8 +4380,44 @@
       <c r="K31">
         <v>15.3</v>
       </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>202</v>
+      </c>
+      <c r="N31">
+        <v>42.89</v>
+      </c>
+      <c r="P31" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q31">
+        <v>21.4</v>
+      </c>
+      <c r="S31" t="s">
+        <v>300</v>
+      </c>
+      <c r="T31">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="V31" t="s">
+        <v>349</v>
+      </c>
+      <c r="W31">
+        <v>26.2</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>398</v>
+      </c>
+      <c r="Z31">
+        <v>20.66</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>448</v>
+      </c>
+      <c r="AC31">
+        <v>5.1100000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>55</v>
       </c>
@@ -2503,8 +4436,44 @@
       <c r="K32">
         <v>21.32</v>
       </c>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>203</v>
+      </c>
+      <c r="N32">
+        <v>43.25</v>
+      </c>
+      <c r="P32" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q32">
+        <v>16.41</v>
+      </c>
+      <c r="S32" t="s">
+        <v>301</v>
+      </c>
+      <c r="T32">
+        <v>1.42</v>
+      </c>
+      <c r="V32" t="s">
+        <v>350</v>
+      </c>
+      <c r="W32">
+        <v>0.99</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>399</v>
+      </c>
+      <c r="Z32">
+        <v>17.329999999999998</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>449</v>
+      </c>
+      <c r="AC32">
+        <v>5.01</v>
+      </c>
+    </row>
+    <row r="33" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>56</v>
       </c>
@@ -2523,8 +4492,44 @@
       <c r="K33">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>204</v>
+      </c>
+      <c r="N33">
+        <v>21.32</v>
+      </c>
+      <c r="P33" t="s">
+        <v>253</v>
+      </c>
+      <c r="Q33">
+        <v>23.14</v>
+      </c>
+      <c r="S33" t="s">
+        <v>302</v>
+      </c>
+      <c r="T33">
+        <v>9.0500000000000007</v>
+      </c>
+      <c r="V33" t="s">
+        <v>351</v>
+      </c>
+      <c r="W33">
+        <v>16.670000000000002</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>400</v>
+      </c>
+      <c r="Z33">
+        <v>8.99</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>450</v>
+      </c>
+      <c r="AC33">
+        <v>19.82</v>
+      </c>
+    </row>
+    <row r="34" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>57</v>
       </c>
@@ -2543,8 +4548,44 @@
       <c r="K34">
         <v>9.6999999999999993</v>
       </c>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>205</v>
+      </c>
+      <c r="N34">
+        <v>14.88</v>
+      </c>
+      <c r="P34" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q34">
+        <v>48.38</v>
+      </c>
+      <c r="S34" t="s">
+        <v>303</v>
+      </c>
+      <c r="T34">
+        <v>11.9</v>
+      </c>
+      <c r="V34" t="s">
+        <v>352</v>
+      </c>
+      <c r="W34">
+        <v>3.53</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z34">
+        <v>10.62</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>451</v>
+      </c>
+      <c r="AC34">
+        <v>49.88</v>
+      </c>
+    </row>
+    <row r="35" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>58</v>
       </c>
@@ -2563,8 +4604,44 @@
       <c r="K35">
         <v>27.75</v>
       </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>206</v>
+      </c>
+      <c r="N35">
+        <v>8.83</v>
+      </c>
+      <c r="P35" t="s">
+        <v>255</v>
+      </c>
+      <c r="Q35">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="S35" t="s">
+        <v>304</v>
+      </c>
+      <c r="T35">
+        <v>21.92</v>
+      </c>
+      <c r="V35" t="s">
+        <v>353</v>
+      </c>
+      <c r="W35">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>402</v>
+      </c>
+      <c r="Z35">
+        <v>13.69</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>452</v>
+      </c>
+      <c r="AC35">
+        <v>68.91</v>
+      </c>
+    </row>
+    <row r="36" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>59</v>
       </c>
@@ -2583,8 +4660,44 @@
       <c r="K36">
         <v>21.69</v>
       </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>207</v>
+      </c>
+      <c r="N36">
+        <v>12.96</v>
+      </c>
+      <c r="P36" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q36">
+        <v>31.54</v>
+      </c>
+      <c r="S36" t="s">
+        <v>305</v>
+      </c>
+      <c r="T36">
+        <v>50.58</v>
+      </c>
+      <c r="V36" t="s">
+        <v>354</v>
+      </c>
+      <c r="W36">
+        <v>23.14</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z36">
+        <v>7.27</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>453</v>
+      </c>
+      <c r="AC36">
+        <v>15.87</v>
+      </c>
+    </row>
+    <row r="37" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>60</v>
       </c>
@@ -2603,8 +4716,44 @@
       <c r="K37">
         <v>28.81</v>
       </c>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>208</v>
+      </c>
+      <c r="N37">
+        <v>6.56</v>
+      </c>
+      <c r="P37" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q37">
+        <v>32.93</v>
+      </c>
+      <c r="S37" t="s">
+        <v>306</v>
+      </c>
+      <c r="T37">
+        <v>2.44</v>
+      </c>
+      <c r="V37" t="s">
+        <v>355</v>
+      </c>
+      <c r="W37">
+        <v>48.38</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>404</v>
+      </c>
+      <c r="Z37">
+        <v>7.27</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>454</v>
+      </c>
+      <c r="AC37">
+        <v>16.829999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>61</v>
       </c>
@@ -2623,8 +4772,44 @@
       <c r="K38">
         <v>34.479999999999997</v>
       </c>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>209</v>
+      </c>
+      <c r="N38">
+        <v>21.4</v>
+      </c>
+      <c r="P38" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q38">
+        <v>8.43</v>
+      </c>
+      <c r="S38" t="s">
+        <v>307</v>
+      </c>
+      <c r="T38">
+        <v>2.81</v>
+      </c>
+      <c r="V38" t="s">
+        <v>356</v>
+      </c>
+      <c r="W38">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>405</v>
+      </c>
+      <c r="Z38">
+        <v>14.62</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>455</v>
+      </c>
+      <c r="AC38">
+        <v>14.33</v>
+      </c>
+    </row>
+    <row r="39" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>62</v>
       </c>
@@ -2643,8 +4828,44 @@
       <c r="K39">
         <v>14.13</v>
       </c>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>210</v>
+      </c>
+      <c r="N39">
+        <v>16.41</v>
+      </c>
+      <c r="P39" t="s">
+        <v>259</v>
+      </c>
+      <c r="Q39">
+        <v>25.7</v>
+      </c>
+      <c r="S39" t="s">
+        <v>308</v>
+      </c>
+      <c r="T39">
+        <v>21.3</v>
+      </c>
+      <c r="V39" t="s">
+        <v>357</v>
+      </c>
+      <c r="W39">
+        <v>20.18</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>406</v>
+      </c>
+      <c r="Z39">
+        <v>2.08</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>456</v>
+      </c>
+      <c r="AC39">
+        <v>18.79</v>
+      </c>
+    </row>
+    <row r="40" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>63</v>
       </c>
@@ -2663,8 +4884,44 @@
       <c r="K40">
         <v>4.47</v>
       </c>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>211</v>
+      </c>
+      <c r="N40">
+        <v>27.14</v>
+      </c>
+      <c r="P40" t="s">
+        <v>260</v>
+      </c>
+      <c r="Q40">
+        <v>19.86</v>
+      </c>
+      <c r="S40" t="s">
+        <v>309</v>
+      </c>
+      <c r="T40">
+        <v>19.41</v>
+      </c>
+      <c r="V40" t="s">
+        <v>358</v>
+      </c>
+      <c r="W40">
+        <v>8.43</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>407</v>
+      </c>
+      <c r="Z40">
+        <v>28.38</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>457</v>
+      </c>
+      <c r="AC40">
+        <v>17.13</v>
+      </c>
+    </row>
+    <row r="41" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>64</v>
       </c>
@@ -2683,8 +4940,44 @@
       <c r="K41">
         <v>7.27</v>
       </c>
-    </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>212</v>
+      </c>
+      <c r="N41">
+        <v>2.1</v>
+      </c>
+      <c r="P41" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q41">
+        <v>15.21</v>
+      </c>
+      <c r="S41" t="s">
+        <v>310</v>
+      </c>
+      <c r="T41">
+        <v>3.91</v>
+      </c>
+      <c r="V41" t="s">
+        <v>359</v>
+      </c>
+      <c r="W41">
+        <v>20.239999999999998</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>408</v>
+      </c>
+      <c r="Z41">
+        <v>5.16</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>458</v>
+      </c>
+      <c r="AC41">
+        <v>13.3</v>
+      </c>
+    </row>
+    <row r="42" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>65</v>
       </c>
@@ -2703,8 +4996,44 @@
       <c r="K42">
         <v>3.4</v>
       </c>
-    </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>213</v>
+      </c>
+      <c r="N42">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="P42" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q42">
+        <v>5.22</v>
+      </c>
+      <c r="S42" t="s">
+        <v>311</v>
+      </c>
+      <c r="T42">
+        <v>11.65</v>
+      </c>
+      <c r="V42" t="s">
+        <v>360</v>
+      </c>
+      <c r="W42">
+        <v>35.340000000000003</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>409</v>
+      </c>
+      <c r="Z42">
+        <v>21.69</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>459</v>
+      </c>
+      <c r="AC42">
+        <v>14.29</v>
+      </c>
+    </row>
+    <row r="43" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>66</v>
       </c>
@@ -2723,8 +5052,44 @@
       <c r="K43">
         <v>8.73</v>
       </c>
-    </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>214</v>
+      </c>
+      <c r="N43">
+        <v>31.54</v>
+      </c>
+      <c r="P43" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q43">
+        <v>23.15</v>
+      </c>
+      <c r="S43" t="s">
+        <v>312</v>
+      </c>
+      <c r="T43">
+        <v>12.45</v>
+      </c>
+      <c r="V43" t="s">
+        <v>361</v>
+      </c>
+      <c r="W43">
+        <v>8.61</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>410</v>
+      </c>
+      <c r="Z43">
+        <v>23.73</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>460</v>
+      </c>
+      <c r="AC43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>67</v>
       </c>
@@ -2743,8 +5108,44 @@
       <c r="K44">
         <v>9.42</v>
       </c>
-    </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M44" t="s">
+        <v>215</v>
+      </c>
+      <c r="N44">
+        <v>32.93</v>
+      </c>
+      <c r="P44" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q44">
+        <v>5.67</v>
+      </c>
+      <c r="S44" t="s">
+        <v>313</v>
+      </c>
+      <c r="T44">
+        <v>9.83</v>
+      </c>
+      <c r="V44" t="s">
+        <v>362</v>
+      </c>
+      <c r="W44">
+        <v>29.78</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>411</v>
+      </c>
+      <c r="Z44">
+        <v>8.48</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>461</v>
+      </c>
+      <c r="AC44">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>68</v>
       </c>
@@ -2763,8 +5164,44 @@
       <c r="K45">
         <v>27.58</v>
       </c>
-    </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>216</v>
+      </c>
+      <c r="N45">
+        <v>8.43</v>
+      </c>
+      <c r="P45" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q45">
+        <v>12.39</v>
+      </c>
+      <c r="S45" t="s">
+        <v>314</v>
+      </c>
+      <c r="T45">
+        <v>14.23</v>
+      </c>
+      <c r="V45" t="s">
+        <v>363</v>
+      </c>
+      <c r="W45">
+        <v>3.4</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>412</v>
+      </c>
+      <c r="Z45">
+        <v>28.36</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>462</v>
+      </c>
+      <c r="AC45">
+        <v>14.41</v>
+      </c>
+    </row>
+    <row r="46" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>69</v>
       </c>
@@ -2783,8 +5220,44 @@
       <c r="K46">
         <v>27.94</v>
       </c>
-    </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>217</v>
+      </c>
+      <c r="N46">
+        <v>25.7</v>
+      </c>
+      <c r="P46" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q46">
+        <v>21.91</v>
+      </c>
+      <c r="S46" t="s">
+        <v>315</v>
+      </c>
+      <c r="T46">
+        <v>43.25</v>
+      </c>
+      <c r="V46" t="s">
+        <v>364</v>
+      </c>
+      <c r="W46">
+        <v>8.83</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>413</v>
+      </c>
+      <c r="Z46">
+        <v>19.190000000000001</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>463</v>
+      </c>
+      <c r="AC46">
+        <v>28.43</v>
+      </c>
+    </row>
+    <row r="47" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>70</v>
       </c>
@@ -2803,8 +5276,44 @@
       <c r="K47">
         <v>46.51</v>
       </c>
-    </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>218</v>
+      </c>
+      <c r="N47">
+        <v>19.86</v>
+      </c>
+      <c r="P47" t="s">
+        <v>267</v>
+      </c>
+      <c r="Q47">
+        <v>36.82</v>
+      </c>
+      <c r="S47" t="s">
+        <v>316</v>
+      </c>
+      <c r="T47">
+        <v>11.53</v>
+      </c>
+      <c r="V47" t="s">
+        <v>365</v>
+      </c>
+      <c r="W47">
+        <v>27.75</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>414</v>
+      </c>
+      <c r="Z47">
+        <v>6.57</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>464</v>
+      </c>
+      <c r="AC47">
+        <v>12.4</v>
+      </c>
+    </row>
+    <row r="48" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>71</v>
       </c>
@@ -2823,8 +5332,44 @@
       <c r="K48">
         <v>52.09</v>
       </c>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M48" t="s">
+        <v>219</v>
+      </c>
+      <c r="N48">
+        <v>10.74</v>
+      </c>
+      <c r="P48" t="s">
+        <v>268</v>
+      </c>
+      <c r="Q48">
+        <v>17.559999999999999</v>
+      </c>
+      <c r="S48" t="s">
+        <v>317</v>
+      </c>
+      <c r="T48">
+        <v>8.33</v>
+      </c>
+      <c r="V48" t="s">
+        <v>366</v>
+      </c>
+      <c r="W48">
+        <v>35.72</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>415</v>
+      </c>
+      <c r="Z48">
+        <v>3.15</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>465</v>
+      </c>
+      <c r="AC48">
+        <v>34.770000000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>72</v>
       </c>
@@ -2843,8 +5388,44 @@
       <c r="K49">
         <v>24.87</v>
       </c>
-    </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>220</v>
+      </c>
+      <c r="N49">
+        <v>11.79</v>
+      </c>
+      <c r="P49" t="s">
+        <v>269</v>
+      </c>
+      <c r="Q49">
+        <v>11.89</v>
+      </c>
+      <c r="S49" t="s">
+        <v>318</v>
+      </c>
+      <c r="T49">
+        <v>9.08</v>
+      </c>
+      <c r="V49" t="s">
+        <v>367</v>
+      </c>
+      <c r="W49">
+        <v>15.52</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>416</v>
+      </c>
+      <c r="Z49">
+        <v>51.7</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>466</v>
+      </c>
+      <c r="AC49">
+        <v>16.37</v>
+      </c>
+    </row>
+    <row r="50" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>73</v>
       </c>
@@ -2863,8 +5444,44 @@
       <c r="K50">
         <v>24.43</v>
       </c>
-    </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>221</v>
+      </c>
+      <c r="N50">
+        <v>17.61</v>
+      </c>
+      <c r="P50" t="s">
+        <v>270</v>
+      </c>
+      <c r="Q50">
+        <v>39.479999999999997</v>
+      </c>
+      <c r="S50" t="s">
+        <v>319</v>
+      </c>
+      <c r="T50">
+        <v>22.63</v>
+      </c>
+      <c r="V50" t="s">
+        <v>368</v>
+      </c>
+      <c r="W50">
+        <v>21.05</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>417</v>
+      </c>
+      <c r="Z50">
+        <v>62.62</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>467</v>
+      </c>
+      <c r="AC50">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="51" spans="3:29" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>74</v>
       </c>
@@ -2883,11 +5500,65 @@
       <c r="K51">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="M51" t="s">
+        <v>222</v>
+      </c>
+      <c r="N51">
+        <v>41.51</v>
+      </c>
+      <c r="P51" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q51">
+        <v>43.67</v>
+      </c>
+      <c r="S51" t="s">
+        <v>320</v>
+      </c>
+      <c r="T51">
+        <v>15.3</v>
+      </c>
+      <c r="V51" t="s">
+        <v>369</v>
+      </c>
+      <c r="W51">
+        <v>2.5</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>418</v>
+      </c>
+      <c r="Z51">
+        <v>20.170000000000002</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>468</v>
+      </c>
+      <c r="AC51">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="52" spans="3:29" x14ac:dyDescent="0.25">
       <c r="H52">
         <f>SUM(H3:H51)</f>
         <v>1085.54</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>419</v>
+      </c>
+      <c r="Z52">
+        <v>22.08</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>469</v>
+      </c>
+      <c r="AC52">
+        <v>7.74</v>
+      </c>
+    </row>
+    <row r="53" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="Z53" s="7">
+        <f>SUM(Z3:Z52)</f>
+        <v>849.3000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added more exception handling and made pytest check for these
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="6990"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="6990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="520">
   <si>
     <t>Kentucky</t>
   </si>
@@ -1438,6 +1438,156 @@
   </si>
   <si>
     <t>49 . Augusta             --&gt;       0  . Dover               Cost</t>
+  </si>
+  <si>
+    <t>0  . Carson City         --&gt;       1  . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>1  . Sacramento          --&gt;       2  . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>2  . Honolulu            --&gt;       3  . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>3  . Juneau              --&gt;       4  . Helana              Cost</t>
+  </si>
+  <si>
+    <t>4  . Helana              --&gt;       5  . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>5  . Salt Lake City      --&gt;       6  . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>6  . Cheyenne            --&gt;       7  . Denver              Cost</t>
+  </si>
+  <si>
+    <t>7  . Denver              --&gt;       8  . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>8  . Santa Fe            --&gt;       9  . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>9  . Oklahoma City       --&gt;       10 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>10 . Jackson             --&gt;       11 . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>11 . Montgomery          --&gt;       12 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>12 . Tallahassee         --&gt;       13 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>13 . Atlanta             --&gt;       14 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>14 . Columbia            --&gt;       15 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>15 . Raleigh             --&gt;       16 . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>16 . Charleston          --&gt;       17 . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>17 . Columbus            --&gt;       18 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>18 . Lansing             --&gt;       19 . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>19 . Frankfort           --&gt;       20 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>20 . Indianapolis        --&gt;       21 . Madison             Cost</t>
+  </si>
+  <si>
+    <t>21 . Madison             --&gt;       22 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>22 . Des Moines          --&gt;       23 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>23 . Springfield         --&gt;       24 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>24 . Nashville           --&gt;       25 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>25 . Richmond            --&gt;       26 . Harrisburg          Cost</t>
+  </si>
+  <si>
+    <t>26 . Harrisburg          --&gt;       27 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>27 . Annapolis           --&gt;       28 . Dover               Cost</t>
+  </si>
+  <si>
+    <t>28 . Dover               --&gt;       29 . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>29 . Trenton             --&gt;       30 . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>30 . Montpelier          --&gt;       31 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>31 . Concord             --&gt;       32 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>32 . Augusta             --&gt;       33 . Boston              Cost</t>
+  </si>
+  <si>
+    <t>33 . Boston              --&gt;       34 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>34 . Providence          --&gt;       35 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>35 . Hartford            --&gt;       36 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>36 . Albany              --&gt;       37 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>37 . Saint Paul          --&gt;       38 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>38 . Bismarck            --&gt;       39 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>39 . Pierre              --&gt;       40 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>40 . Lincoln             --&gt;       41 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>41 . Topeka              --&gt;       42 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>42 . Jefferson City      --&gt;       43 . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>43 . Little Rock         --&gt;       44 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>44 . Baton Rouge         --&gt;       45 . Austin              Cost</t>
+  </si>
+  <si>
+    <t>45 . Austin              --&gt;       46 . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>46 . Phoenix             --&gt;       47 . Boise               Cost</t>
+  </si>
+  <si>
+    <t>47 . Boise               --&gt;       48 . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>48 . Olympia             --&gt;       49 . Salem               Cost</t>
+  </si>
+  <si>
+    <t>49 . Salem               --&gt;       0  . Carson City         Cost</t>
   </si>
 </sst>
 </file>
@@ -1823,7 +1973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A21" workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2782,10 +2932,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AC53"/>
+  <dimension ref="C3:AF53"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="AB23" sqref="AB23"/>
+    <sheetView tabSelected="1" topLeftCell="P26" workbookViewId="0">
+      <selection activeCell="AF3" sqref="AF3:AF52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2943,7 @@
     <col min="3" max="3" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>26</v>
       </c>
@@ -2848,8 +2998,14 @@
       <c r="AC3">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="4" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE3" t="s">
+        <v>470</v>
+      </c>
+      <c r="AF3">
+        <v>1.82</v>
+      </c>
+    </row>
+    <row r="4" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>27</v>
       </c>
@@ -2904,8 +3060,14 @@
       <c r="AC4">
         <v>28.38</v>
       </c>
-    </row>
-    <row r="5" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE4" t="s">
+        <v>471</v>
+      </c>
+      <c r="AF4">
+        <v>40.24</v>
+      </c>
+    </row>
+    <row r="5" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>28</v>
       </c>
@@ -2960,8 +3122,14 @@
       <c r="AC5">
         <v>19.03</v>
       </c>
-    </row>
-    <row r="6" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE5" t="s">
+        <v>472</v>
+      </c>
+      <c r="AF5">
+        <v>43.78</v>
+      </c>
+    </row>
+    <row r="6" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>29</v>
       </c>
@@ -3016,8 +3184,14 @@
       <c r="AC6">
         <v>8.48</v>
       </c>
-    </row>
-    <row r="7" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE6" t="s">
+        <v>473</v>
+      </c>
+      <c r="AF6">
+        <v>25.27</v>
+      </c>
+    </row>
+    <row r="7" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>30</v>
       </c>
@@ -3072,8 +3246,14 @@
       <c r="AC7">
         <v>6.63</v>
       </c>
-    </row>
-    <row r="8" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE7" t="s">
+        <v>474</v>
+      </c>
+      <c r="AF7">
+        <v>5.84</v>
+      </c>
+    </row>
+    <row r="8" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>31</v>
       </c>
@@ -3128,8 +3308,14 @@
       <c r="AC8">
         <v>17.559999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE8" t="s">
+        <v>475</v>
+      </c>
+      <c r="AF8">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>32</v>
       </c>
@@ -3184,8 +3370,14 @@
       <c r="AC9">
         <v>60.3</v>
       </c>
-    </row>
-    <row r="10" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE9" t="s">
+        <v>476</v>
+      </c>
+      <c r="AF9">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="10" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>33</v>
       </c>
@@ -3240,8 +3432,14 @@
       <c r="AC10">
         <v>12.29</v>
       </c>
-    </row>
-    <row r="11" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE10" t="s">
+        <v>477</v>
+      </c>
+      <c r="AF10">
+        <v>4.1900000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>34</v>
       </c>
@@ -3296,8 +3494,14 @@
       <c r="AC11">
         <v>10.23</v>
       </c>
-    </row>
-    <row r="12" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE11" t="s">
+        <v>478</v>
+      </c>
+      <c r="AF11">
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="12" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -3352,8 +3556,14 @@
       <c r="AC12">
         <v>8.7899999999999991</v>
       </c>
-    </row>
-    <row r="13" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE12" t="s">
+        <v>479</v>
+      </c>
+      <c r="AF12">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="13" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>36</v>
       </c>
@@ -3408,8 +3618,14 @@
       <c r="AC13">
         <v>4.8499999999999996</v>
       </c>
-    </row>
-    <row r="14" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE13" t="s">
+        <v>480</v>
+      </c>
+      <c r="AF13">
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="14" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>37</v>
       </c>
@@ -3464,8 +3680,14 @@
       <c r="AC14">
         <v>4.49</v>
       </c>
-    </row>
-    <row r="15" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE14" t="s">
+        <v>481</v>
+      </c>
+      <c r="AF14">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="15" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>38</v>
       </c>
@@ -3520,8 +3742,14 @@
       <c r="AC15">
         <v>19.87</v>
       </c>
-    </row>
-    <row r="16" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE15" t="s">
+        <v>482</v>
+      </c>
+      <c r="AF15">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="16" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -3576,8 +3804,14 @@
       <c r="AC16">
         <v>31.34</v>
       </c>
-    </row>
-    <row r="17" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE16" t="s">
+        <v>483</v>
+      </c>
+      <c r="AF16">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="17" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>40</v>
       </c>
@@ -3632,8 +3866,14 @@
       <c r="AC17">
         <v>9.48</v>
       </c>
-    </row>
-    <row r="18" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE17" t="s">
+        <v>484</v>
+      </c>
+      <c r="AF17">
+        <v>2.98</v>
+      </c>
+    </row>
+    <row r="18" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>41</v>
       </c>
@@ -3688,8 +3928,14 @@
       <c r="AC18">
         <v>33.520000000000003</v>
       </c>
-    </row>
-    <row r="19" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE18" t="s">
+        <v>485</v>
+      </c>
+      <c r="AF18">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="19" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>42</v>
       </c>
@@ -3744,8 +3990,14 @@
       <c r="AC19">
         <v>13.58</v>
       </c>
-    </row>
-    <row r="20" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE19" t="s">
+        <v>486</v>
+      </c>
+      <c r="AF19">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="20" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>43</v>
       </c>
@@ -3800,8 +4052,14 @@
       <c r="AC20">
         <v>19.07</v>
       </c>
-    </row>
-    <row r="21" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE20" t="s">
+        <v>487</v>
+      </c>
+      <c r="AF20">
+        <v>3.17</v>
+      </c>
+    </row>
+    <row r="21" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>44</v>
       </c>
@@ -3856,8 +4114,14 @@
       <c r="AC21">
         <v>7.13</v>
       </c>
-    </row>
-    <row r="22" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE21" t="s">
+        <v>488</v>
+      </c>
+      <c r="AF21">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="22" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>45</v>
       </c>
@@ -3912,8 +4176,14 @@
       <c r="AC22">
         <v>11.29</v>
       </c>
-    </row>
-    <row r="23" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE22" t="s">
+        <v>489</v>
+      </c>
+      <c r="AF22">
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>46</v>
       </c>
@@ -3968,8 +4238,14 @@
       <c r="AC23">
         <v>3.22</v>
       </c>
-    </row>
-    <row r="24" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE23" t="s">
+        <v>490</v>
+      </c>
+      <c r="AF23">
+        <v>4.6100000000000003</v>
+      </c>
+    </row>
+    <row r="24" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>47</v>
       </c>
@@ -4024,8 +4300,14 @@
       <c r="AC24">
         <v>6.22</v>
       </c>
-    </row>
-    <row r="25" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE24" t="s">
+        <v>491</v>
+      </c>
+      <c r="AF24">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="25" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>48</v>
       </c>
@@ -4080,8 +4362,14 @@
       <c r="AC25">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="26" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE25" t="s">
+        <v>492</v>
+      </c>
+      <c r="AF25">
+        <v>4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>49</v>
       </c>
@@ -4136,8 +4424,14 @@
       <c r="AC26">
         <v>6.36</v>
       </c>
-    </row>
-    <row r="27" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE26" t="s">
+        <v>493</v>
+      </c>
+      <c r="AF26">
+        <v>4.62</v>
+      </c>
+    </row>
+    <row r="27" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>50</v>
       </c>
@@ -4192,8 +4486,14 @@
       <c r="AC27">
         <v>13.26</v>
       </c>
-    </row>
-    <row r="28" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE27" t="s">
+        <v>494</v>
+      </c>
+      <c r="AF27">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="28" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>51</v>
       </c>
@@ -4248,8 +4548,14 @@
       <c r="AC28">
         <v>4.01</v>
       </c>
-    </row>
-    <row r="29" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE28" t="s">
+        <v>495</v>
+      </c>
+      <c r="AF28">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="29" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>52</v>
       </c>
@@ -4304,8 +4610,14 @@
       <c r="AC29">
         <v>21.05</v>
       </c>
-    </row>
-    <row r="30" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE29" t="s">
+        <v>496</v>
+      </c>
+      <c r="AF29">
+        <v>1.35</v>
+      </c>
+    </row>
+    <row r="30" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>53</v>
       </c>
@@ -4360,8 +4672,14 @@
       <c r="AC30">
         <v>15.92</v>
       </c>
-    </row>
-    <row r="31" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE30" t="s">
+        <v>497</v>
+      </c>
+      <c r="AF30">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="31" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>54</v>
       </c>
@@ -4416,8 +4734,14 @@
       <c r="AC31">
         <v>5.1100000000000003</v>
       </c>
-    </row>
-    <row r="32" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE31" t="s">
+        <v>498</v>
+      </c>
+      <c r="AF31">
+        <v>1.31</v>
+      </c>
+    </row>
+    <row r="32" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>55</v>
       </c>
@@ -4472,8 +4796,14 @@
       <c r="AC32">
         <v>5.01</v>
       </c>
-    </row>
-    <row r="33" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE32" t="s">
+        <v>499</v>
+      </c>
+      <c r="AF32">
+        <v>4.5999999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>56</v>
       </c>
@@ -4528,8 +4858,14 @@
       <c r="AC33">
         <v>19.82</v>
       </c>
-    </row>
-    <row r="34" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE33" t="s">
+        <v>500</v>
+      </c>
+      <c r="AF33">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="34" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>57</v>
       </c>
@@ -4584,8 +4920,14 @@
       <c r="AC34">
         <v>49.88</v>
       </c>
-    </row>
-    <row r="35" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE34" t="s">
+        <v>501</v>
+      </c>
+      <c r="AF34">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>58</v>
       </c>
@@ -4640,8 +4982,14 @@
       <c r="AC35">
         <v>68.91</v>
       </c>
-    </row>
-    <row r="36" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE35" t="s">
+        <v>502</v>
+      </c>
+      <c r="AF35">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="36" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>59</v>
       </c>
@@ -4696,8 +5044,14 @@
       <c r="AC36">
         <v>15.87</v>
       </c>
-    </row>
-    <row r="37" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE36" t="s">
+        <v>503</v>
+      </c>
+      <c r="AF36">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>60</v>
       </c>
@@ -4752,8 +5106,14 @@
       <c r="AC37">
         <v>16.829999999999998</v>
       </c>
-    </row>
-    <row r="38" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE37" t="s">
+        <v>504</v>
+      </c>
+      <c r="AF37">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="38" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>61</v>
       </c>
@@ -4808,8 +5168,14 @@
       <c r="AC38">
         <v>14.33</v>
       </c>
-    </row>
-    <row r="39" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE38" t="s">
+        <v>505</v>
+      </c>
+      <c r="AF38">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="39" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>62</v>
       </c>
@@ -4864,8 +5230,14 @@
       <c r="AC39">
         <v>18.79</v>
       </c>
-    </row>
-    <row r="40" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE39" t="s">
+        <v>506</v>
+      </c>
+      <c r="AF39">
+        <v>19.45</v>
+      </c>
+    </row>
+    <row r="40" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>63</v>
       </c>
@@ -4920,8 +5292,14 @@
       <c r="AC40">
         <v>17.13</v>
       </c>
-    </row>
-    <row r="41" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE40" t="s">
+        <v>507</v>
+      </c>
+      <c r="AF40">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="41" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>64</v>
       </c>
@@ -4976,8 +5354,14 @@
       <c r="AC41">
         <v>13.3</v>
       </c>
-    </row>
-    <row r="42" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE41" t="s">
+        <v>508</v>
+      </c>
+      <c r="AF41">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="42" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>65</v>
       </c>
@@ -5032,8 +5416,14 @@
       <c r="AC42">
         <v>14.29</v>
       </c>
-    </row>
-    <row r="43" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE42" t="s">
+        <v>509</v>
+      </c>
+      <c r="AF42">
+        <v>5.1100000000000003</v>
+      </c>
+    </row>
+    <row r="43" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>66</v>
       </c>
@@ -5088,8 +5478,14 @@
       <c r="AC43">
         <v>15</v>
       </c>
-    </row>
-    <row r="44" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE43" t="s">
+        <v>510</v>
+      </c>
+      <c r="AF43">
+        <v>2.0299999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>67</v>
       </c>
@@ -5144,8 +5540,14 @@
       <c r="AC44">
         <v>1.1100000000000001</v>
       </c>
-    </row>
-    <row r="45" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE44" t="s">
+        <v>511</v>
+      </c>
+      <c r="AF44">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="45" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>68</v>
       </c>
@@ -5200,8 +5602,14 @@
       <c r="AC45">
         <v>14.41</v>
       </c>
-    </row>
-    <row r="46" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE45" t="s">
+        <v>512</v>
+      </c>
+      <c r="AF45">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="46" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>69</v>
       </c>
@@ -5256,8 +5664,14 @@
       <c r="AC46">
         <v>28.43</v>
       </c>
-    </row>
-    <row r="47" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE46" t="s">
+        <v>513</v>
+      </c>
+      <c r="AF46">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>70</v>
       </c>
@@ -5312,8 +5726,14 @@
       <c r="AC47">
         <v>12.4</v>
       </c>
-    </row>
-    <row r="48" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE47" t="s">
+        <v>514</v>
+      </c>
+      <c r="AF47">
+        <v>6.61</v>
+      </c>
+    </row>
+    <row r="48" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>71</v>
       </c>
@@ -5368,8 +5788,14 @@
       <c r="AC48">
         <v>34.770000000000003</v>
       </c>
-    </row>
-    <row r="49" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE48" t="s">
+        <v>515</v>
+      </c>
+      <c r="AF48">
+        <v>14.67</v>
+      </c>
+    </row>
+    <row r="49" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>72</v>
       </c>
@@ -5424,8 +5850,14 @@
       <c r="AC49">
         <v>16.37</v>
       </c>
-    </row>
-    <row r="50" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE49" t="s">
+        <v>516</v>
+      </c>
+      <c r="AF49">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="50" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>73</v>
       </c>
@@ -5480,8 +5912,14 @@
       <c r="AC50">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="51" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE50" t="s">
+        <v>517</v>
+      </c>
+      <c r="AF50">
+        <v>7.49</v>
+      </c>
+    </row>
+    <row r="51" spans="3:32" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>74</v>
       </c>
@@ -5536,8 +5974,14 @@
       <c r="AC51">
         <v>3.87</v>
       </c>
-    </row>
-    <row r="52" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE51" t="s">
+        <v>518</v>
+      </c>
+      <c r="AF51">
+        <v>2.12</v>
+      </c>
+    </row>
+    <row r="52" spans="3:32" x14ac:dyDescent="0.25">
       <c r="H52">
         <f>SUM(H3:H51)</f>
         <v>1085.54</v>
@@ -5554,8 +5998,14 @@
       <c r="AC52">
         <v>7.74</v>
       </c>
-    </row>
-    <row r="53" spans="3:29" x14ac:dyDescent="0.25">
+      <c r="AE52" t="s">
+        <v>519</v>
+      </c>
+      <c r="AF52">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="53" spans="3:32" x14ac:dyDescent="0.25">
       <c r="Z53" s="7">
         <f>SUM(Z3:Z52)</f>
         <v>849.3000000000003</v>

</xml_diff>

<commit_message>
made file_name user changeable
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="570">
   <si>
     <t>Kentucky</t>
   </si>
@@ -1588,6 +1588,156 @@
   </si>
   <si>
     <t>49 . Salem               --&gt;       0  . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>0  . Harrisburg          --&gt;       1  . Charleston          Cost</t>
+  </si>
+  <si>
+    <t>1  . Charleston          --&gt;       2  . Columbus            Cost</t>
+  </si>
+  <si>
+    <t>2  . Columbus            --&gt;       3  . Frankfort           Cost</t>
+  </si>
+  <si>
+    <t>3  . Frankfort           --&gt;       4  . Austin              Cost</t>
+  </si>
+  <si>
+    <t>4  . Austin              --&gt;       5  . Santa Fe            Cost</t>
+  </si>
+  <si>
+    <t>5  . Santa Fe            --&gt;       6  . Salt Lake City      Cost</t>
+  </si>
+  <si>
+    <t>6  . Salt Lake City      --&gt;       7  . Boise               Cost</t>
+  </si>
+  <si>
+    <t>7  . Boise               --&gt;       8  . Carson City         Cost</t>
+  </si>
+  <si>
+    <t>8  . Carson City         --&gt;       9  . Phoenix             Cost</t>
+  </si>
+  <si>
+    <t>9  . Phoenix             --&gt;       10 . Albany              Cost</t>
+  </si>
+  <si>
+    <t>10 . Albany              --&gt;       11 . Boston              Cost</t>
+  </si>
+  <si>
+    <t>11 . Boston              --&gt;       12 . Providence          Cost</t>
+  </si>
+  <si>
+    <t>12 . Providence          --&gt;       13 . Columbia            Cost</t>
+  </si>
+  <si>
+    <t>13 . Columbia            --&gt;       14 . Tallahassee         Cost</t>
+  </si>
+  <si>
+    <t>14 . Tallahassee         --&gt;       15 . Montgomery          Cost</t>
+  </si>
+  <si>
+    <t>15 . Montgomery          --&gt;       16 . Little Rock         Cost</t>
+  </si>
+  <si>
+    <t>16 . Little Rock         --&gt;       17 . Baton Rouge         Cost</t>
+  </si>
+  <si>
+    <t>17 . Baton Rouge         --&gt;       18 . Jackson             Cost</t>
+  </si>
+  <si>
+    <t>18 . Jackson             --&gt;       19 . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>19 . Oklahoma City       --&gt;       20 . Lincoln             Cost</t>
+  </si>
+  <si>
+    <t>20 . Lincoln             --&gt;       21 . Denver              Cost</t>
+  </si>
+  <si>
+    <t>21 . Denver              --&gt;       22 . Cheyenne            Cost</t>
+  </si>
+  <si>
+    <t>22 . Cheyenne            --&gt;       23 . Olympia             Cost</t>
+  </si>
+  <si>
+    <t>23 . Olympia             --&gt;       24 . Juneau              Cost</t>
+  </si>
+  <si>
+    <t>24 . Juneau              --&gt;       25 . Honolulu            Cost</t>
+  </si>
+  <si>
+    <t>25 . Honolulu            --&gt;       26 . Sacramento          Cost</t>
+  </si>
+  <si>
+    <t>26 . Sacramento          --&gt;       27 . Salem               Cost</t>
+  </si>
+  <si>
+    <t>27 . Salem               --&gt;       28 . Helana              Cost</t>
+  </si>
+  <si>
+    <t>28 . Helana              --&gt;       29 . Bismarck            Cost</t>
+  </si>
+  <si>
+    <t>29 . Bismarck            --&gt;       30 . Pierre              Cost</t>
+  </si>
+  <si>
+    <t>30 . Pierre              --&gt;       31 . Saint Paul          Cost</t>
+  </si>
+  <si>
+    <t>31 . Saint Paul          --&gt;       32 . Lansing             Cost</t>
+  </si>
+  <si>
+    <t>32 . Lansing             --&gt;       33 . Montpelier          Cost</t>
+  </si>
+  <si>
+    <t>33 . Montpelier          --&gt;       34 . Augusta             Cost</t>
+  </si>
+  <si>
+    <t>34 . Augusta             --&gt;       35 . Concord             Cost</t>
+  </si>
+  <si>
+    <t>35 . Concord             --&gt;       36 . Hartford            Cost</t>
+  </si>
+  <si>
+    <t>36 . Hartford            --&gt;       37 . Trenton             Cost</t>
+  </si>
+  <si>
+    <t>37 . Trenton             --&gt;       38 . Indianapolis        Cost</t>
+  </si>
+  <si>
+    <t>38 . Indianapolis        --&gt;       39 . Springfield         Cost</t>
+  </si>
+  <si>
+    <t>39 . Springfield         --&gt;       40 . Madison             Cost</t>
+  </si>
+  <si>
+    <t>40 . Madison             --&gt;       41 . Des Moines          Cost</t>
+  </si>
+  <si>
+    <t>41 . Des Moines          --&gt;       42 . Topeka              Cost</t>
+  </si>
+  <si>
+    <t>42 . Topeka              --&gt;       43 . Jefferson City      Cost</t>
+  </si>
+  <si>
+    <t>43 . Jefferson City      --&gt;       44 . Nashville           Cost</t>
+  </si>
+  <si>
+    <t>44 . Nashville           --&gt;       45 . Atlanta             Cost</t>
+  </si>
+  <si>
+    <t>45 . Atlanta             --&gt;       46 . Raleigh             Cost</t>
+  </si>
+  <si>
+    <t>46 . Raleigh             --&gt;       47 . Richmond            Cost</t>
+  </si>
+  <si>
+    <t>47 . Richmond            --&gt;       48 . Annapolis           Cost</t>
+  </si>
+  <si>
+    <t>48 . Annapolis           --&gt;       49 . Dover               Cost</t>
+  </si>
+  <si>
+    <t>49 . Dover               --&gt;       0  . Harrisburg          Cost</t>
   </si>
 </sst>
 </file>
@@ -2932,10 +3082,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:AF53"/>
+  <dimension ref="C3:AI53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P26" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3:AF52"/>
+    <sheetView tabSelected="1" topLeftCell="P28" workbookViewId="0">
+      <selection activeCell="AL44" sqref="AL44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2943,7 +3093,7 @@
     <col min="3" max="3" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>26</v>
       </c>
@@ -3004,8 +3154,14 @@
       <c r="AF3">
         <v>1.82</v>
       </c>
-    </row>
-    <row r="4" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH3" t="s">
+        <v>520</v>
+      </c>
+      <c r="AI3">
+        <v>5.13</v>
+      </c>
+    </row>
+    <row r="4" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>27</v>
       </c>
@@ -3066,8 +3222,14 @@
       <c r="AF4">
         <v>40.24</v>
       </c>
-    </row>
-    <row r="5" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH4" t="s">
+        <v>521</v>
+      </c>
+      <c r="AI4">
+        <v>2.11</v>
+      </c>
+    </row>
+    <row r="5" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>28</v>
       </c>
@@ -3128,8 +3290,14 @@
       <c r="AF5">
         <v>43.78</v>
       </c>
-    </row>
-    <row r="6" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH5" t="s">
+        <v>522</v>
+      </c>
+      <c r="AI5">
+        <v>2.57</v>
+      </c>
+    </row>
+    <row r="6" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>29</v>
       </c>
@@ -3190,8 +3358,14 @@
       <c r="AF6">
         <v>25.27</v>
       </c>
-    </row>
-    <row r="7" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH6" t="s">
+        <v>523</v>
+      </c>
+      <c r="AI6">
+        <v>15.13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>30</v>
       </c>
@@ -3252,8 +3426,14 @@
       <c r="AF7">
         <v>5.84</v>
       </c>
-    </row>
-    <row r="8" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH7" t="s">
+        <v>524</v>
+      </c>
+      <c r="AI7">
+        <v>9.83</v>
+      </c>
+    </row>
+    <row r="8" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>31</v>
       </c>
@@ -3314,8 +3494,14 @@
       <c r="AF8">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="9" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH8" t="s">
+        <v>525</v>
+      </c>
+      <c r="AI8">
+        <v>7.81</v>
+      </c>
+    </row>
+    <row r="9" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>32</v>
       </c>
@@ -3376,8 +3562,14 @@
       <c r="AF9">
         <v>1.42</v>
       </c>
-    </row>
-    <row r="10" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH9" t="s">
+        <v>526</v>
+      </c>
+      <c r="AI9">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>33</v>
       </c>
@@ -3438,8 +3630,14 @@
       <c r="AF10">
         <v>4.1900000000000004</v>
       </c>
-    </row>
-    <row r="11" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH10" t="s">
+        <v>527</v>
+      </c>
+      <c r="AI10">
+        <v>5.67</v>
+      </c>
+    </row>
+    <row r="11" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>34</v>
       </c>
@@ -3500,8 +3698,14 @@
       <c r="AF11">
         <v>8.43</v>
       </c>
-    </row>
-    <row r="12" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH11" t="s">
+        <v>528</v>
+      </c>
+      <c r="AI11">
+        <v>9.57</v>
+      </c>
+    </row>
+    <row r="12" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -3562,8 +3766,14 @@
       <c r="AF12">
         <v>7.98</v>
       </c>
-    </row>
-    <row r="13" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH12" t="s">
+        <v>529</v>
+      </c>
+      <c r="AI12">
+        <v>39.380000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>36</v>
       </c>
@@ -3624,8 +3834,14 @@
       <c r="AF13">
         <v>3.93</v>
       </c>
-    </row>
-    <row r="14" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH13" t="s">
+        <v>530</v>
+      </c>
+      <c r="AI13">
+        <v>2.79</v>
+      </c>
+    </row>
+    <row r="14" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>37</v>
       </c>
@@ -3686,8 +3902,14 @@
       <c r="AF14">
         <v>2.77</v>
       </c>
-    </row>
-    <row r="15" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH14" t="s">
+        <v>531</v>
+      </c>
+      <c r="AI14">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>38</v>
       </c>
@@ -3748,8 +3970,14 @@
       <c r="AF15">
         <v>3.31</v>
       </c>
-    </row>
-    <row r="16" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH15" t="s">
+        <v>532</v>
+      </c>
+      <c r="AI15">
+        <v>12.39</v>
+      </c>
+    </row>
+    <row r="16" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -3810,8 +4038,14 @@
       <c r="AF16">
         <v>3.36</v>
       </c>
-    </row>
-    <row r="17" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH16" t="s">
+        <v>533</v>
+      </c>
+      <c r="AI16">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>40</v>
       </c>
@@ -3872,8 +4106,14 @@
       <c r="AF17">
         <v>2.98</v>
       </c>
-    </row>
-    <row r="18" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH17" t="s">
+        <v>534</v>
+      </c>
+      <c r="AI17">
+        <v>2.77</v>
+      </c>
+    </row>
+    <row r="18" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>41</v>
       </c>
@@ -3934,8 +4174,14 @@
       <c r="AF18">
         <v>3.95</v>
       </c>
-    </row>
-    <row r="19" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH18" t="s">
+        <v>535</v>
+      </c>
+      <c r="AI18">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="19" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>42</v>
       </c>
@@ -3996,8 +4242,14 @@
       <c r="AF19">
         <v>2.11</v>
       </c>
-    </row>
-    <row r="20" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH19" t="s">
+        <v>536</v>
+      </c>
+      <c r="AI19">
+        <v>4.4400000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>43</v>
       </c>
@@ -4058,8 +4310,14 @@
       <c r="AF20">
         <v>3.17</v>
       </c>
-    </row>
-    <row r="21" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH20" t="s">
+        <v>537</v>
+      </c>
+      <c r="AI20">
+        <v>2.08</v>
+      </c>
+    </row>
+    <row r="21" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>44</v>
       </c>
@@ -4120,8 +4378,14 @@
       <c r="AF21">
         <v>4.55</v>
       </c>
-    </row>
-    <row r="22" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH21" t="s">
+        <v>538</v>
+      </c>
+      <c r="AI21">
+        <v>7.98</v>
+      </c>
+    </row>
+    <row r="22" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>45</v>
       </c>
@@ -4182,8 +4446,14 @@
       <c r="AF22">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="23" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH22" t="s">
+        <v>539</v>
+      </c>
+      <c r="AI22">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="23" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>46</v>
       </c>
@@ -4244,8 +4514,14 @@
       <c r="AF23">
         <v>4.6100000000000003</v>
       </c>
-    </row>
-    <row r="24" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH23" t="s">
+        <v>540</v>
+      </c>
+      <c r="AI23">
+        <v>8.3800000000000008</v>
+      </c>
+    </row>
+    <row r="24" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>47</v>
       </c>
@@ -4306,8 +4582,14 @@
       <c r="AF24">
         <v>4.49</v>
       </c>
-    </row>
-    <row r="25" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH24" t="s">
+        <v>541</v>
+      </c>
+      <c r="AI24">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="25" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>48</v>
       </c>
@@ -4368,8 +4650,14 @@
       <c r="AF25">
         <v>4.3600000000000003</v>
       </c>
-    </row>
-    <row r="26" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH25" t="s">
+        <v>542</v>
+      </c>
+      <c r="AI25">
+        <v>19.03</v>
+      </c>
+    </row>
+    <row r="26" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>49</v>
       </c>
@@ -4430,8 +4718,14 @@
       <c r="AF26">
         <v>4.62</v>
       </c>
-    </row>
-    <row r="27" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH26" t="s">
+        <v>543</v>
+      </c>
+      <c r="AI26">
+        <v>16.11</v>
+      </c>
+    </row>
+    <row r="27" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>50</v>
       </c>
@@ -4492,8 +4786,14 @@
       <c r="AF27">
         <v>9.42</v>
       </c>
-    </row>
-    <row r="28" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH27" t="s">
+        <v>544</v>
+      </c>
+      <c r="AI27">
+        <v>43.78</v>
+      </c>
+    </row>
+    <row r="28" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>51</v>
       </c>
@@ -4554,8 +4854,14 @@
       <c r="AF28">
         <v>2.79</v>
       </c>
-    </row>
-    <row r="29" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH28" t="s">
+        <v>545</v>
+      </c>
+      <c r="AI28">
+        <v>40.24</v>
+      </c>
+    </row>
+    <row r="29" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>52</v>
       </c>
@@ -4616,8 +4922,14 @@
       <c r="AF29">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="30" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH29" t="s">
+        <v>546</v>
+      </c>
+      <c r="AI29">
+        <v>6.56</v>
+      </c>
+    </row>
+    <row r="30" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>53</v>
       </c>
@@ -4678,8 +4990,14 @@
       <c r="AF30">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="31" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH30" t="s">
+        <v>547</v>
+      </c>
+      <c r="AI30">
+        <v>11.13</v>
+      </c>
+    </row>
+    <row r="31" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>54</v>
       </c>
@@ -4740,8 +5058,14 @@
       <c r="AF31">
         <v>1.31</v>
       </c>
-    </row>
-    <row r="32" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH31" t="s">
+        <v>548</v>
+      </c>
+      <c r="AI31">
+        <v>11.46</v>
+      </c>
+    </row>
+    <row r="32" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>55</v>
       </c>
@@ -4802,8 +5126,14 @@
       <c r="AF32">
         <v>4.5999999999999996</v>
       </c>
-    </row>
-    <row r="33" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH32" t="s">
+        <v>549</v>
+      </c>
+      <c r="AI32">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="33" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>56</v>
       </c>
@@ -4864,8 +5194,14 @@
       <c r="AF33">
         <v>1.46</v>
       </c>
-    </row>
-    <row r="34" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH33" t="s">
+        <v>550</v>
+      </c>
+      <c r="AI33">
+        <v>7.27</v>
+      </c>
+    </row>
+    <row r="34" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>57</v>
       </c>
@@ -4926,8 +5262,14 @@
       <c r="AF34">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="35" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH34" t="s">
+        <v>551</v>
+      </c>
+      <c r="AI34">
+        <v>8.83</v>
+      </c>
+    </row>
+    <row r="35" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>58</v>
       </c>
@@ -4988,8 +5330,14 @@
       <c r="AF35">
         <v>2.44</v>
       </c>
-    </row>
-    <row r="36" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH35" t="s">
+        <v>552</v>
+      </c>
+      <c r="AI35">
+        <v>12.07</v>
+      </c>
+    </row>
+    <row r="36" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>59</v>
       </c>
@@ -5050,8 +5398,14 @@
       <c r="AF36">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="37" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH36" t="s">
+        <v>553</v>
+      </c>
+      <c r="AI36">
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="37" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>60</v>
       </c>
@@ -5112,8 +5466,14 @@
       <c r="AF37">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="38" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH37" t="s">
+        <v>554</v>
+      </c>
+      <c r="AI37">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>61</v>
       </c>
@@ -5174,8 +5534,14 @@
       <c r="AF38">
         <v>1.42</v>
       </c>
-    </row>
-    <row r="39" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH38" t="s">
+        <v>555</v>
+      </c>
+      <c r="AI38">
+        <v>1.84</v>
+      </c>
+    </row>
+    <row r="39" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>62</v>
       </c>
@@ -5236,8 +5602,14 @@
       <c r="AF39">
         <v>19.45</v>
       </c>
-    </row>
-    <row r="40" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH39" t="s">
+        <v>556</v>
+      </c>
+      <c r="AI39">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="40" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>63</v>
       </c>
@@ -5298,8 +5670,14 @@
       <c r="AF40">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="41" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH40" t="s">
+        <v>557</v>
+      </c>
+      <c r="AI40">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="41" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>64</v>
       </c>
@@ -5360,8 +5738,14 @@
       <c r="AF41">
         <v>4.47</v>
       </c>
-    </row>
-    <row r="42" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH41" t="s">
+        <v>558</v>
+      </c>
+      <c r="AI41">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="42" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>65</v>
       </c>
@@ -5422,8 +5806,14 @@
       <c r="AF42">
         <v>5.1100000000000003</v>
       </c>
-    </row>
-    <row r="43" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH42" t="s">
+        <v>559</v>
+      </c>
+      <c r="AI42">
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="43" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>66</v>
       </c>
@@ -5484,8 +5874,14 @@
       <c r="AF43">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="44" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH43" t="s">
+        <v>560</v>
+      </c>
+      <c r="AI43">
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="44" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>67</v>
       </c>
@@ -5546,8 +5942,14 @@
       <c r="AF44">
         <v>3.53</v>
       </c>
-    </row>
-    <row r="45" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH44" t="s">
+        <v>561</v>
+      </c>
+      <c r="AI44">
+        <v>3.28</v>
+      </c>
+    </row>
+    <row r="45" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>68</v>
       </c>
@@ -5608,8 +6010,14 @@
       <c r="AF45">
         <v>3.84</v>
       </c>
-    </row>
-    <row r="46" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH45" t="s">
+        <v>562</v>
+      </c>
+      <c r="AI45">
+        <v>3.53</v>
+      </c>
+    </row>
+    <row r="46" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>69</v>
       </c>
@@ -5670,8 +6078,14 @@
       <c r="AF46">
         <v>4.4400000000000004</v>
       </c>
-    </row>
-    <row r="47" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH46" t="s">
+        <v>563</v>
+      </c>
+      <c r="AI46">
+        <v>5.92</v>
+      </c>
+    </row>
+    <row r="47" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>70</v>
       </c>
@@ -5732,8 +6146,14 @@
       <c r="AF47">
         <v>6.61</v>
       </c>
-    </row>
-    <row r="48" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH47" t="s">
+        <v>564</v>
+      </c>
+      <c r="AI47">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="48" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>71</v>
       </c>
@@ -5794,8 +6214,14 @@
       <c r="AF48">
         <v>14.67</v>
       </c>
-    </row>
-    <row r="49" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH48" t="s">
+        <v>565</v>
+      </c>
+      <c r="AI48">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="49" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>72</v>
       </c>
@@ -5856,8 +6282,14 @@
       <c r="AF49">
         <v>10.99</v>
       </c>
-    </row>
-    <row r="50" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH49" t="s">
+        <v>566</v>
+      </c>
+      <c r="AI49">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="50" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>73</v>
       </c>
@@ -5918,8 +6350,14 @@
       <c r="AF50">
         <v>7.49</v>
       </c>
-    </row>
-    <row r="51" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH50" t="s">
+        <v>567</v>
+      </c>
+      <c r="AI50">
+        <v>1.72</v>
+      </c>
+    </row>
+    <row r="51" spans="3:35" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>74</v>
       </c>
@@ -5980,8 +6418,14 @@
       <c r="AF51">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="52" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH51" t="s">
+        <v>568</v>
+      </c>
+      <c r="AI51">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="52" spans="3:35" x14ac:dyDescent="0.25">
       <c r="H52">
         <f>SUM(H3:H51)</f>
         <v>1085.54</v>
@@ -6004,11 +6448,21 @@
       <c r="AF52">
         <v>6.63</v>
       </c>
-    </row>
-    <row r="53" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="AH52" t="s">
+        <v>569</v>
+      </c>
+      <c r="AI52">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="53" spans="3:35" x14ac:dyDescent="0.25">
       <c r="Z53" s="7">
         <f>SUM(Z3:Z52)</f>
         <v>849.3000000000003</v>
+      </c>
+      <c r="AI53" s="7">
+        <f>SUM(AI3:AI52)</f>
+        <v>403.69999999999987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tested on "world-capitals-test.txt" - works, assuming world is flat
</commit_message>
<xml_diff>
--- a/calculations.xlsx
+++ b/calculations.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="1064">
   <si>
     <t>Kentucky</t>
   </si>
@@ -2620,6 +2620,606 @@
   </si>
   <si>
     <t>49 . Topeka              --&gt;       0  . Oklahoma City       Cost</t>
+  </si>
+  <si>
+    <t>0  . Bogota              --&gt;       1  . Freetown            Cost</t>
+  </si>
+  <si>
+    <t>1  . Freetown            --&gt;       2  . Bissau              Cost</t>
+  </si>
+  <si>
+    <t>2  . Bissau              --&gt;       3  . Pyongyang           Cost</t>
+  </si>
+  <si>
+    <t>3  . Pyongyang           --&gt;       4  . Beijing             Cost</t>
+  </si>
+  <si>
+    <t>4  . Beijing             --&gt;       5  . Bishkek             Cost</t>
+  </si>
+  <si>
+    <t>5  . Bishkek             --&gt;       6  . Nairobi             Cost</t>
+  </si>
+  <si>
+    <t>6  . Nairobi             --&gt;       7  . Addis Ababa         Cost</t>
+  </si>
+  <si>
+    <t>7  . Addis Ababa         --&gt;       8  . Asmara              Cost</t>
+  </si>
+  <si>
+    <t>8  . Asmara              --&gt;       9  . Damascus            Cost</t>
+  </si>
+  <si>
+    <t>9  . Damascus            --&gt;       10 . Ankara              Cost</t>
+  </si>
+  <si>
+    <t>10 . Ankara              --&gt;       11 . Bucuresti           Cost</t>
+  </si>
+  <si>
+    <t>11 . Bucuresti           --&gt;       12 . Zagreb              Cost</t>
+  </si>
+  <si>
+    <t>12 . Zagreb              --&gt;       13 . Rome                Cost</t>
+  </si>
+  <si>
+    <t>13 . Rome                --&gt;       14 . Berlin              Cost</t>
+  </si>
+  <si>
+    <t>14 . Berlin              --&gt;       15 . Sarajevo            Cost</t>
+  </si>
+  <si>
+    <t>15 . Sarajevo            --&gt;       16 . Tripoli             Cost</t>
+  </si>
+  <si>
+    <t>16 . Tripoli             --&gt;       17 . Tunis               Cost</t>
+  </si>
+  <si>
+    <t>17 . Tunis               --&gt;       18 . Valletta            Cost</t>
+  </si>
+  <si>
+    <t>18 . Valletta            --&gt;       19 . Amman               Cost</t>
+  </si>
+  <si>
+    <t>19 . Amman               --&gt;       20 . Baghdad             Cost</t>
+  </si>
+  <si>
+    <t>20 . Baghdad             --&gt;       21 . Kuwait              Cost</t>
+  </si>
+  <si>
+    <t>21 . Kuwait              --&gt;       22 . Manama              Cost</t>
+  </si>
+  <si>
+    <t>22 . Manama              --&gt;       23 . Doha                Cost</t>
+  </si>
+  <si>
+    <t>23 . Doha                --&gt;       24 . Khartoum            Cost</t>
+  </si>
+  <si>
+    <t>24 . Khartoum            --&gt;       25 . Kinshasa            Cost</t>
+  </si>
+  <si>
+    <t>25 . Kinshasa            --&gt;       26 . Mbabane             Cost</t>
+  </si>
+  <si>
+    <t>26 . Mbabane             --&gt;       27 . Maseru              Cost</t>
+  </si>
+  <si>
+    <t>27 . Maseru              --&gt;       28 . Heard Island        Cost</t>
+  </si>
+  <si>
+    <t>28 . Heard Island        --&gt;       29 . Dili                Cost</t>
+  </si>
+  <si>
+    <t>29 . Dili                --&gt;       30 . Palikir             Cost</t>
+  </si>
+  <si>
+    <t>30 . Palikir             --&gt;       31 . Funafuti            Cost</t>
+  </si>
+  <si>
+    <t>31 . Funafuti            --&gt;       32 . Wellington          Cost</t>
+  </si>
+  <si>
+    <t>32 . Wellington          --&gt;       33 . Canberra            Cost</t>
+  </si>
+  <si>
+    <t>33 . Canberra            --&gt;       34 . Port Moresby        Cost</t>
+  </si>
+  <si>
+    <t>34 . Port Moresby        --&gt;       35 . Honiara             Cost</t>
+  </si>
+  <si>
+    <t>35 . Honiara             --&gt;       36 . Port-Vila           Cost</t>
+  </si>
+  <si>
+    <t>36 . Port-Vila           --&gt;       37 . Tarawa              Cost</t>
+  </si>
+  <si>
+    <t>37 . Tarawa              --&gt;       38 . Seoul               Cost</t>
+  </si>
+  <si>
+    <t>38 . Seoul               --&gt;       39 . Reykjavik           Cost</t>
+  </si>
+  <si>
+    <t>39 . Reykjavik           --&gt;       40 . West Indies         Cost</t>
+  </si>
+  <si>
+    <t>40 . West Indies         --&gt;       41 . Oranjestad          Cost</t>
+  </si>
+  <si>
+    <t>41 . Oranjestad          --&gt;       42 . Panama              Cost</t>
+  </si>
+  <si>
+    <t>42 . Panama              --&gt;       43 . San Jose            Cost</t>
+  </si>
+  <si>
+    <t>43 . San Jose            --&gt;       44 . Saint-Pierre        Cost</t>
+  </si>
+  <si>
+    <t>44 . Saint-Pierre        --&gt;       45 . London              Cost</t>
+  </si>
+  <si>
+    <t>45 . London              --&gt;       46 . Astana              Cost</t>
+  </si>
+  <si>
+    <t>46 . Astana              --&gt;       47 . Dushanbe            Cost</t>
+  </si>
+  <si>
+    <t>47 . Dushanbe            --&gt;       48 . Islamabad           Cost</t>
+  </si>
+  <si>
+    <t>48 . Islamabad           --&gt;       49 . Kabul               Cost</t>
+  </si>
+  <si>
+    <t>49 . Kabul               --&gt;       50 . Yaounde             Cost</t>
+  </si>
+  <si>
+    <t>50 . Yaounde             --&gt;       51 . Porto Novo          Cost</t>
+  </si>
+  <si>
+    <t>51 . Porto Novo          --&gt;       52 . Accra               Cost</t>
+  </si>
+  <si>
+    <t>52 . Accra               --&gt;       53 . Lome                Cost</t>
+  </si>
+  <si>
+    <t>53 . Lome                --&gt;       54 . Luanda              Cost</t>
+  </si>
+  <si>
+    <t>54 . Luanda              --&gt;       55 . Windhoek            Cost</t>
+  </si>
+  <si>
+    <t>55 . Windhoek            --&gt;       56 . Gaborone            Cost</t>
+  </si>
+  <si>
+    <t>56 . Gaborone            --&gt;       57 . Pretoria            Cost</t>
+  </si>
+  <si>
+    <t>57 . Pretoria            --&gt;       58 . Maputo              Cost</t>
+  </si>
+  <si>
+    <t>58 . Maputo              --&gt;       59 . Bujumbura           Cost</t>
+  </si>
+  <si>
+    <t>59 . Bujumbura           --&gt;       60 . Riyadh              Cost</t>
+  </si>
+  <si>
+    <t>60 . Riyadh              --&gt;       61 . Sofia               Cost</t>
+  </si>
+  <si>
+    <t>61 . Sofia               --&gt;       62 . Minsk               Cost</t>
+  </si>
+  <si>
+    <t>62 . Minsk               --&gt;       63 . Vilnius             Cost</t>
+  </si>
+  <si>
+    <t>63 . Vilnius             --&gt;       64 . Riga                Cost</t>
+  </si>
+  <si>
+    <t>64 . Riga                --&gt;       65 . Abuja               Cost</t>
+  </si>
+  <si>
+    <t>65 . Abuja               --&gt;       66 . Yamoussoukro        Cost</t>
+  </si>
+  <si>
+    <t>66 . Yamoussoukro        --&gt;       67 . Conakry             Cost</t>
+  </si>
+  <si>
+    <t>67 . Conakry             --&gt;       68 . Vienna              Cost</t>
+  </si>
+  <si>
+    <t>68 . Vienna              --&gt;       69 . Bratislava          Cost</t>
+  </si>
+  <si>
+    <t>69 . Bratislava          --&gt;       70 . Torshavn            Cost</t>
+  </si>
+  <si>
+    <t>70 . Torshavn            --&gt;       71 . Oslo                Cost</t>
+  </si>
+  <si>
+    <t>71 . Oslo                --&gt;       72 . Copenhagen          Cost</t>
+  </si>
+  <si>
+    <t>72 . Copenhagen          --&gt;       73 . Amsterdam           Cost</t>
+  </si>
+  <si>
+    <t>73 . Amsterdam           --&gt;       74 . Brussels            Cost</t>
+  </si>
+  <si>
+    <t>74 . Brussels            --&gt;       75 . Luxembourg          Cost</t>
+  </si>
+  <si>
+    <t>75 . Luxembourg          --&gt;       76 . Bern                Cost</t>
+  </si>
+  <si>
+    <t>76 . Bern                --&gt;       77 . Banjul              Cost</t>
+  </si>
+  <si>
+    <t>77 . Banjul              --&gt;       78 . Brasilia            Cost</t>
+  </si>
+  <si>
+    <t>78 . Brasilia            --&gt;       79 . Asuncion            Cost</t>
+  </si>
+  <si>
+    <t>79 . Asuncion            --&gt;       80 . Paramaribo          Cost</t>
+  </si>
+  <si>
+    <t>80 . Paramaribo          --&gt;       81 . San Salvador        Cost</t>
+  </si>
+  <si>
+    <t>81 . San Salvador        --&gt;       82 . Belmopan            Cost</t>
+  </si>
+  <si>
+    <t>82 . Belmopan            --&gt;       83 . Jerusalem           Cost</t>
+  </si>
+  <si>
+    <t>83 . Jerusalem           --&gt;       84 . Bamako              Cost</t>
+  </si>
+  <si>
+    <t>84 . Bamako              --&gt;       85 . Niamey              Cost</t>
+  </si>
+  <si>
+    <t>85 . Niamey              --&gt;       86 . Sao Tome            Cost</t>
+  </si>
+  <si>
+    <t>86 . Sao Tome            --&gt;       87 . Malabo              Cost</t>
+  </si>
+  <si>
+    <t>87 . Malabo              --&gt;       88 . Dhaka               Cost</t>
+  </si>
+  <si>
+    <t>88 . Dhaka               --&gt;       89 . Bangkok             Cost</t>
+  </si>
+  <si>
+    <t>89 . Bangkok             --&gt;       90 . Yangon              Cost</t>
+  </si>
+  <si>
+    <t>90 . Yangon              --&gt;       91 . Bandar Seri Begawan Cost</t>
+  </si>
+  <si>
+    <t>91 . Bandar Seri Begawan --&gt;       92 . Brazzaville         Cost</t>
+  </si>
+  <si>
+    <t>92 . Brazzaville         --&gt;       93 . Libreville          Cost</t>
+  </si>
+  <si>
+    <t>93 . Libreville          --&gt;       94 . Charlotte Amalie    Cost</t>
+  </si>
+  <si>
+    <t>94 . Charlotte Amalie    --&gt;       95 . San Juan            Cost</t>
+  </si>
+  <si>
+    <t>95 . San Juan            --&gt;       96 . Willemstad          Cost</t>
+  </si>
+  <si>
+    <t>96 . Willemstad          --&gt;       97 . Basseterre          Cost</t>
+  </si>
+  <si>
+    <t>97 . Basseterre          --&gt;       98 . Road Town           Cost</t>
+  </si>
+  <si>
+    <t>98 . Road Town           --&gt;       99 . St. Peter Port      Cost</t>
+  </si>
+  <si>
+    <t>99 . St. Peter Port      --&gt;       100. Paris               Cost</t>
+  </si>
+  <si>
+    <t>100. Paris               --&gt;       101. Stockholm           Cost</t>
+  </si>
+  <si>
+    <t>101. Stockholm           --&gt;       102. Warsaw              Cost</t>
+  </si>
+  <si>
+    <t>102. Warsaw              --&gt;       103. Budapest            Cost</t>
+  </si>
+  <si>
+    <t>103. Budapest            --&gt;       104. San Marino          Cost</t>
+  </si>
+  <si>
+    <t>104. San Marino          --&gt;       105. Dakar               Cost</t>
+  </si>
+  <si>
+    <t>105. Dakar               --&gt;       106. Praia               Cost</t>
+  </si>
+  <si>
+    <t>106. Praia               --&gt;       107. Port-au-Prince      Cost</t>
+  </si>
+  <si>
+    <t>107. Port-au-Prince      --&gt;       108. Santo Domingo       Cost</t>
+  </si>
+  <si>
+    <t>108. Santo Domingo       --&gt;       109. Caracas             Cost</t>
+  </si>
+  <si>
+    <t>109. Caracas             --&gt;       110. Kingstown           Cost</t>
+  </si>
+  <si>
+    <t>110. Kingstown           --&gt;       111. Bridgetown          Cost</t>
+  </si>
+  <si>
+    <t>111. Bridgetown          --&gt;       112. Lisbon              Cost</t>
+  </si>
+  <si>
+    <t>112. Lisbon              --&gt;       113. Dublin              Cost</t>
+  </si>
+  <si>
+    <t>113. Dublin              --&gt;       114. Nuuk                Cost</t>
+  </si>
+  <si>
+    <t>114. Nuuk                --&gt;       115. Ottawa              Cost</t>
+  </si>
+  <si>
+    <t>115. Ottawa              --&gt;       116. Washington DC       Cost</t>
+  </si>
+  <si>
+    <t>116. Washington DC       --&gt;       117. Mexico              Cost</t>
+  </si>
+  <si>
+    <t>117. Mexico              --&gt;       118. Pago Pago           Cost</t>
+  </si>
+  <si>
+    <t>118. Pago Pago           --&gt;       119. Apia                Cost</t>
+  </si>
+  <si>
+    <t>119. Apia                --&gt;       120. Nuku'alofa          Cost</t>
+  </si>
+  <si>
+    <t>120. Nuku'alofa          --&gt;       121. Papeete             Cost</t>
+  </si>
+  <si>
+    <t>121. Papeete             --&gt;       122. Guatemala           Cost</t>
+  </si>
+  <si>
+    <t>122. Guatemala           --&gt;       123. Nassau              Cost</t>
+  </si>
+  <si>
+    <t>123. Nassau              --&gt;       124. Algiers             Cost</t>
+  </si>
+  <si>
+    <t>124. Algiers             --&gt;       125. Vaduz               Cost</t>
+  </si>
+  <si>
+    <t>125. Vaduz               --&gt;       126. Madrid              Cost</t>
+  </si>
+  <si>
+    <t>126. Madrid              --&gt;       127. Andorra la Vella    Cost</t>
+  </si>
+  <si>
+    <t>127. Andorra la Vella    --&gt;       128. Havana              Cost</t>
+  </si>
+  <si>
+    <t>128. Havana              --&gt;       129. George Town         Cost</t>
+  </si>
+  <si>
+    <t>129. George Town         --&gt;       130. Tegucigalpa         Cost</t>
+  </si>
+  <si>
+    <t>130. Tegucigalpa         --&gt;       131. Roseau              Cost</t>
+  </si>
+  <si>
+    <t>131. Roseau              --&gt;       132. Basse-Terre         Cost</t>
+  </si>
+  <si>
+    <t>132. Basse-Terre         --&gt;       133. Fort-de-France      Cost</t>
+  </si>
+  <si>
+    <t>133. Fort-de-France      --&gt;       134. Castries            Cost</t>
+  </si>
+  <si>
+    <t>134. Castries            --&gt;       135. Georgetown          Cost</t>
+  </si>
+  <si>
+    <t>135. Georgetown          --&gt;       136. Santiago            Cost</t>
+  </si>
+  <si>
+    <t>136. Santiago            --&gt;       137. Stanley             Cost</t>
+  </si>
+  <si>
+    <t>137. Stanley             --&gt;       138. Buenos Aires        Cost</t>
+  </si>
+  <si>
+    <t>138. Buenos Aires        --&gt;       139. Montevideo          Cost</t>
+  </si>
+  <si>
+    <t>139. Montevideo          --&gt;       140. Tehran              Cost</t>
+  </si>
+  <si>
+    <t>140. Tehran              --&gt;       141. Kathmandu           Cost</t>
+  </si>
+  <si>
+    <t>141. Kathmandu           --&gt;       142. New Delhi           Cost</t>
+  </si>
+  <si>
+    <t>142. New Delhi           --&gt;       143. Baku                Cost</t>
+  </si>
+  <si>
+    <t>143. Baku                --&gt;       144. Belgrade            Cost</t>
+  </si>
+  <si>
+    <t>144. Belgrade            --&gt;       145. Ljubljana           Cost</t>
+  </si>
+  <si>
+    <t>145. Ljubljana           --&gt;       146. Skopje              Cost</t>
+  </si>
+  <si>
+    <t>146. Skopje              --&gt;       147. Kampala             Cost</t>
+  </si>
+  <si>
+    <t>147. Kampala             --&gt;       148. Moroni              Cost</t>
+  </si>
+  <si>
+    <t>148. Moroni              --&gt;       149. Mamoudzou           Cost</t>
+  </si>
+  <si>
+    <t>149. Mamoudzou           --&gt;       150. Male                Cost</t>
+  </si>
+  <si>
+    <t>150. Male                --&gt;       151. Masqat              Cost</t>
+  </si>
+  <si>
+    <t>151. Masqat              --&gt;       152. Abu Dhabi           Cost</t>
+  </si>
+  <si>
+    <t>152. Abu Dhabi           --&gt;       153. Ashgabat            Cost</t>
+  </si>
+  <si>
+    <t>153. Ashgabat            --&gt;       154. Tashkent            Cost</t>
+  </si>
+  <si>
+    <t>154. Tashkent            --&gt;       155. Moskva              Cost</t>
+  </si>
+  <si>
+    <t>155. Moskva              --&gt;       156. Kiev (Russia)       Cost</t>
+  </si>
+  <si>
+    <t>156. Kiev (Russia)       --&gt;       157. Helsinki            Cost</t>
+  </si>
+  <si>
+    <t>157. Helsinki            --&gt;       158. Tallinn             Cost</t>
+  </si>
+  <si>
+    <t>158. Tallinn             --&gt;       159. Prague              Cost</t>
+  </si>
+  <si>
+    <t>159. Prague              --&gt;       160. Chisinau            Cost</t>
+  </si>
+  <si>
+    <t>160. Chisinau            --&gt;       161. Nicosia             Cost</t>
+  </si>
+  <si>
+    <t>161. Nicosia             --&gt;       162. Yerevan             Cost</t>
+  </si>
+  <si>
+    <t>162. Yerevan             --&gt;       163. T'bilisi            Cost</t>
+  </si>
+  <si>
+    <t>163. T'bilisi            --&gt;       164. Dodoma              Cost</t>
+  </si>
+  <si>
+    <t>164. Dodoma              --&gt;       165. Harare              Cost</t>
+  </si>
+  <si>
+    <t>165. Harare              --&gt;       166. Lilongwe            Cost</t>
+  </si>
+  <si>
+    <t>166. Lilongwe            --&gt;       167. Mogadishu           Cost</t>
+  </si>
+  <si>
+    <t>167. Mogadishu           --&gt;       168. Djibouti            Cost</t>
+  </si>
+  <si>
+    <t>168. Djibouti            --&gt;       169. Athens              Cost</t>
+  </si>
+  <si>
+    <t>169. Athens              --&gt;       170. Tirane              Cost</t>
+  </si>
+  <si>
+    <t>170. Tirane              --&gt;       171. Cairo               Cost</t>
+  </si>
+  <si>
+    <t>171. Cairo               --&gt;       172. Beirut              Cost</t>
+  </si>
+  <si>
+    <t>172. Beirut              --&gt;       173. Thimphu             Cost</t>
+  </si>
+  <si>
+    <t>173. Thimphu             --&gt;       174. Macau               Cost</t>
+  </si>
+  <si>
+    <t>174. Macau               --&gt;       175. Koror               Cost</t>
+  </si>
+  <si>
+    <t>175. Koror               --&gt;       176. Saipan              Cost</t>
+  </si>
+  <si>
+    <t>176. Saipan              --&gt;       177. Manila              Cost</t>
+  </si>
+  <si>
+    <t>177. Manila              --&gt;       178. Hanoi               Cost</t>
+  </si>
+  <si>
+    <t>178. Hanoi               --&gt;       179. Vientiane           Cost</t>
+  </si>
+  <si>
+    <t>179. Vientiane           --&gt;       180. Noumea              Cost</t>
+  </si>
+  <si>
+    <t>180. Noumea              --&gt;       181. Kingston            Cost</t>
+  </si>
+  <si>
+    <t>181. Kingston            --&gt;       182. Suva                Cost</t>
+  </si>
+  <si>
+    <t>182. Suva                --&gt;       183. Antananarivo        Cost</t>
+  </si>
+  <si>
+    <t>183. Antananarivo        --&gt;       184. Nouakchott          Cost</t>
+  </si>
+  <si>
+    <t>184. Nouakchott          --&gt;       185. Kigali              Cost</t>
+  </si>
+  <si>
+    <t>185. Kigali              --&gt;       186. Bangui              Cost</t>
+  </si>
+  <si>
+    <t>186. Bangui              --&gt;       187. N'Djamena           Cost</t>
+  </si>
+  <si>
+    <t>187. N'Djamena           --&gt;       188. Kampala             Cost</t>
+  </si>
+  <si>
+    <t>188. Kampala             --&gt;       189. Kuala Lumpur        Cost</t>
+  </si>
+  <si>
+    <t>189. Kuala Lumpur        --&gt;       190. Phnom Penh          Cost</t>
+  </si>
+  <si>
+    <t>190. Phnom Penh          --&gt;       191. Jakarta             Cost</t>
+  </si>
+  <si>
+    <t>191. Jakarta             --&gt;       192. Lusaka              Cost</t>
+  </si>
+  <si>
+    <t>192. Lusaka              --&gt;       193. Ouagadougou         Cost</t>
+  </si>
+  <si>
+    <t>193. Ouagadougou         --&gt;       194. Monrovia            Cost</t>
+  </si>
+  <si>
+    <t>194. Monrovia            --&gt;       195. Cayenne             Cost</t>
+  </si>
+  <si>
+    <t>195. Cayenne             --&gt;       196. Managua             Cost</t>
+  </si>
+  <si>
+    <t>196. Managua             --&gt;       197. Lima                Cost</t>
+  </si>
+  <si>
+    <t>197. Lima                --&gt;       198. La Paz              Cost</t>
+  </si>
+  <si>
+    <t>198. La Paz              --&gt;       199. Quito               Cost</t>
+  </si>
+  <si>
+    <t>199. Quito               --&gt;       0  . Bogota              Cost</t>
   </si>
 </sst>
 </file>
@@ -3964,10 +4564,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:BB53"/>
+  <dimension ref="C3:BE203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH31" workbookViewId="0">
-      <selection activeCell="AP42" sqref="AP42"/>
+    <sheetView tabSelected="1" topLeftCell="AM1" workbookViewId="0">
+      <selection activeCell="BA188" sqref="BA188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3975,7 +4575,7 @@
     <col min="3" max="3" width="78" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:54" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>26</v>
       </c>
@@ -4075,8 +4675,14 @@
       <c r="BB3">
         <v>8.58</v>
       </c>
-    </row>
-    <row r="4" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD3" t="s">
+        <v>864</v>
+      </c>
+      <c r="BE3">
+        <v>60.96</v>
+      </c>
+    </row>
+    <row r="4" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>27</v>
       </c>
@@ -4176,8 +4782,14 @@
       <c r="BB4">
         <v>1.42</v>
       </c>
-    </row>
-    <row r="5" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD4" t="s">
+        <v>865</v>
+      </c>
+      <c r="BE4">
+        <v>3.89</v>
+      </c>
+    </row>
+    <row r="5" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>28</v>
       </c>
@@ -4277,8 +4889,14 @@
       <c r="BB5">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="6" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD5" t="s">
+        <v>866</v>
+      </c>
+      <c r="BE5">
+        <v>143.44</v>
+      </c>
+    </row>
+    <row r="6" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>29</v>
       </c>
@@ -4378,8 +4996,14 @@
       <c r="BB6">
         <v>5.2</v>
       </c>
-    </row>
-    <row r="7" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD6" t="s">
+        <v>867</v>
+      </c>
+      <c r="BE6">
+        <v>9.11</v>
+      </c>
+    </row>
+    <row r="7" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>30</v>
       </c>
@@ -4479,8 +5103,14 @@
       <c r="BB7">
         <v>47.19</v>
       </c>
-    </row>
-    <row r="8" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD7" t="s">
+        <v>868</v>
+      </c>
+      <c r="BE7">
+        <v>41.85</v>
+      </c>
+    </row>
+    <row r="8" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>31</v>
       </c>
@@ -4580,8 +5210,14 @@
       <c r="BB8">
         <v>43.78</v>
       </c>
-    </row>
-    <row r="9" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD8" t="s">
+        <v>869</v>
+      </c>
+      <c r="BE8">
+        <v>57.91</v>
+      </c>
+    </row>
+    <row r="9" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>32</v>
       </c>
@@ -4681,8 +5317,14 @@
       <c r="BB9">
         <v>16.11</v>
       </c>
-    </row>
-    <row r="10" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD9" t="s">
+        <v>870</v>
+      </c>
+      <c r="BE9">
+        <v>10.37</v>
+      </c>
+    </row>
+    <row r="10" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>33</v>
       </c>
@@ -4782,8 +5424,14 @@
       <c r="BB10">
         <v>2.12</v>
       </c>
-    </row>
-    <row r="11" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD10" t="s">
+        <v>871</v>
+      </c>
+      <c r="BE10">
+        <v>6.17</v>
+      </c>
+    </row>
+    <row r="11" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>34</v>
       </c>
@@ -4883,8 +5531,14 @@
       <c r="BB11">
         <v>11.13</v>
       </c>
-    </row>
-    <row r="12" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD11" t="s">
+        <v>872</v>
+      </c>
+      <c r="BE11">
+        <v>18.260000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>35</v>
       </c>
@@ -4984,8 +5638,14 @@
       <c r="BB12">
         <v>11.46</v>
       </c>
-    </row>
-    <row r="13" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD12" t="s">
+        <v>873</v>
+      </c>
+      <c r="BE12">
+        <v>7.25</v>
+      </c>
+    </row>
+    <row r="13" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>36</v>
       </c>
@@ -5085,8 +5745,14 @@
       <c r="BB13">
         <v>4.47</v>
       </c>
-    </row>
-    <row r="14" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD13" t="s">
+        <v>874</v>
+      </c>
+      <c r="BE13">
+        <v>7.97</v>
+      </c>
+    </row>
+    <row r="14" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>37</v>
       </c>
@@ -5186,8 +5852,14 @@
       <c r="BB14">
         <v>7.27</v>
       </c>
-    </row>
-    <row r="15" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD14" t="s">
+        <v>875</v>
+      </c>
+      <c r="BE14">
+        <v>10.59</v>
+      </c>
+    </row>
+    <row r="15" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>38</v>
       </c>
@@ -5287,8 +5959,14 @@
       <c r="BB15">
         <v>4.16</v>
       </c>
-    </row>
-    <row r="16" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD15" t="s">
+        <v>876</v>
+      </c>
+      <c r="BE15">
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="16" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>39</v>
       </c>
@@ -5388,8 +6066,14 @@
       <c r="BB16">
         <v>4.8499999999999996</v>
       </c>
-    </row>
-    <row r="17" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD16" t="s">
+        <v>877</v>
+      </c>
+      <c r="BE16">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="17" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>40</v>
       </c>
@@ -5489,8 +6173,14 @@
       <c r="BB17">
         <v>8.06</v>
       </c>
-    </row>
-    <row r="18" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD17" t="s">
+        <v>878</v>
+      </c>
+      <c r="BE17">
+        <v>10.11</v>
+      </c>
+    </row>
+    <row r="18" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>41</v>
       </c>
@@ -5590,8 +6280,14 @@
       <c r="BB18">
         <v>1.35</v>
       </c>
-    </row>
-    <row r="19" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD18" t="s">
+        <v>879</v>
+      </c>
+      <c r="BE18">
+        <v>12.19</v>
+      </c>
+    </row>
+    <row r="19" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
         <v>42</v>
       </c>
@@ -5691,8 +6387,14 @@
       <c r="BB19">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="20" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD19" t="s">
+        <v>880</v>
+      </c>
+      <c r="BE19">
+        <v>4.9800000000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>43</v>
       </c>
@@ -5792,8 +6494,14 @@
       <c r="BB20">
         <v>2.13</v>
       </c>
-    </row>
-    <row r="21" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD20" t="s">
+        <v>881</v>
+      </c>
+      <c r="BE20">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="21" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
         <v>44</v>
       </c>
@@ -5893,8 +6601,14 @@
       <c r="BB21">
         <v>2.98</v>
       </c>
-    </row>
-    <row r="22" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD21" t="s">
+        <v>882</v>
+      </c>
+      <c r="BE21">
+        <v>21.58</v>
+      </c>
+    </row>
+    <row r="22" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>45</v>
       </c>
@@ -5994,8 +6708,14 @@
       <c r="BB22">
         <v>11.32</v>
       </c>
-    </row>
-    <row r="23" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD22" t="s">
+        <v>883</v>
+      </c>
+      <c r="BE22">
+        <v>8.93</v>
+      </c>
+    </row>
+    <row r="23" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>46</v>
       </c>
@@ -6095,8 +6815,14 @@
       <c r="BB23">
         <v>13.67</v>
       </c>
-    </row>
-    <row r="24" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD23" t="s">
+        <v>884</v>
+      </c>
+      <c r="BE23">
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="24" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
         <v>47</v>
       </c>
@@ -6196,8 +6922,14 @@
       <c r="BB24">
         <v>14.23</v>
       </c>
-    </row>
-    <row r="25" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD24" t="s">
+        <v>885</v>
+      </c>
+      <c r="BE24">
+        <v>3.94</v>
+      </c>
+    </row>
+    <row r="25" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>48</v>
       </c>
@@ -6297,8 +7029,14 @@
       <c r="BB25">
         <v>1.82</v>
       </c>
-    </row>
-    <row r="26" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD25" t="s">
+        <v>886</v>
+      </c>
+      <c r="BE25">
+        <v>1.42</v>
+      </c>
+    </row>
+    <row r="26" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>49</v>
       </c>
@@ -6398,8 +7136,14 @@
       <c r="BB26">
         <v>10.69</v>
       </c>
-    </row>
-    <row r="27" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD26" t="s">
+        <v>887</v>
+      </c>
+      <c r="BE26">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="27" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>50</v>
       </c>
@@ -6499,8 +7243,14 @@
       <c r="BB27">
         <v>14.67</v>
       </c>
-    </row>
-    <row r="28" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD27" t="s">
+        <v>888</v>
+      </c>
+      <c r="BE27">
+        <v>26.01</v>
+      </c>
+    </row>
+    <row r="28" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
         <v>51</v>
       </c>
@@ -6600,8 +7350,14 @@
       <c r="BB28">
         <v>6.61</v>
       </c>
-    </row>
-    <row r="29" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD28" t="s">
+        <v>889</v>
+      </c>
+      <c r="BE28">
+        <v>27.13</v>
+      </c>
+    </row>
+    <row r="29" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>52</v>
       </c>
@@ -6701,8 +7457,14 @@
       <c r="BB29">
         <v>2.08</v>
       </c>
-    </row>
-    <row r="30" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD29" t="s">
+        <v>890</v>
+      </c>
+      <c r="BE29">
+        <v>4.8099999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>53</v>
       </c>
@@ -6802,8 +7564,14 @@
       <c r="BB30">
         <v>3.93</v>
       </c>
-    </row>
-    <row r="31" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD30" t="s">
+        <v>891</v>
+      </c>
+      <c r="BE30">
+        <v>52.42</v>
+      </c>
+    </row>
+    <row r="31" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>54</v>
       </c>
@@ -6903,8 +7671,14 @@
       <c r="BB31">
         <v>2.77</v>
       </c>
-    </row>
-    <row r="32" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD31" t="s">
+        <v>892</v>
+      </c>
+      <c r="BE31">
+        <v>68.08</v>
+      </c>
+    </row>
+    <row r="32" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>55</v>
       </c>
@@ -7004,8 +7778,14 @@
       <c r="BB32">
         <v>3.31</v>
       </c>
-    </row>
-    <row r="33" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD32" t="s">
+        <v>893</v>
+      </c>
+      <c r="BE32">
+        <v>35.96</v>
+      </c>
+    </row>
+    <row r="33" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>56</v>
       </c>
@@ -7105,8 +7885,14 @@
       <c r="BB33">
         <v>3.39</v>
       </c>
-    </row>
-    <row r="34" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD33" t="s">
+        <v>894</v>
+      </c>
+      <c r="BE33">
+        <v>25.76</v>
+      </c>
+    </row>
+    <row r="34" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>57</v>
       </c>
@@ -7206,8 +7992,14 @@
       <c r="BB34">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="35" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD34" t="s">
+        <v>895</v>
+      </c>
+      <c r="BE34">
+        <v>33.21</v>
+      </c>
+    </row>
+    <row r="35" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>58</v>
       </c>
@@ -7307,8 +8099,14 @@
       <c r="BB35">
         <v>2.0499999999999998</v>
       </c>
-    </row>
-    <row r="36" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD35" t="s">
+        <v>896</v>
+      </c>
+      <c r="BE35">
+        <v>26.09</v>
+      </c>
+    </row>
+    <row r="36" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>59</v>
       </c>
@@ -7408,8 +8206,14 @@
       <c r="BB36">
         <v>3.15</v>
       </c>
-    </row>
-    <row r="37" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD36" t="s">
+        <v>897</v>
+      </c>
+      <c r="BE36">
+        <v>25.99</v>
+      </c>
+    </row>
+    <row r="37" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
         <v>60</v>
       </c>
@@ -7509,8 +8313,14 @@
       <c r="BB37">
         <v>2.11</v>
       </c>
-    </row>
-    <row r="38" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD37" t="s">
+        <v>898</v>
+      </c>
+      <c r="BE37">
+        <v>12.49</v>
+      </c>
+    </row>
+    <row r="38" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>61</v>
       </c>
@@ -7610,8 +8420,14 @@
       <c r="BB38">
         <v>6.16</v>
       </c>
-    </row>
-    <row r="39" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD38" t="s">
+        <v>899</v>
+      </c>
+      <c r="BE38">
+        <v>11.88</v>
+      </c>
+    </row>
+    <row r="39" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>62</v>
       </c>
@@ -7711,8 +8527,14 @@
       <c r="BB39">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="40" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD39" t="s">
+        <v>900</v>
+      </c>
+      <c r="BE39">
+        <v>19.36</v>
+      </c>
+    </row>
+    <row r="40" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>63</v>
       </c>
@@ -7812,8 +8634,14 @@
       <c r="BB40">
         <v>1.46</v>
       </c>
-    </row>
-    <row r="41" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD40" t="s">
+        <v>901</v>
+      </c>
+      <c r="BE40">
+        <v>58.75</v>
+      </c>
+    </row>
+    <row r="41" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>64</v>
       </c>
@@ -7913,8 +8741,14 @@
       <c r="BB41">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="42" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD41" t="s">
+        <v>902</v>
+      </c>
+      <c r="BE41">
+        <v>150.55000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>65</v>
       </c>
@@ -8014,8 +8848,14 @@
       <c r="BB42">
         <v>2.44</v>
       </c>
-    </row>
-    <row r="43" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD42" t="s">
+        <v>903</v>
+      </c>
+      <c r="BE42">
+        <v>61.58</v>
+      </c>
+    </row>
+    <row r="43" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>66</v>
       </c>
@@ -8115,8 +8955,14 @@
       <c r="BB43">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="44" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD43" t="s">
+        <v>904</v>
+      </c>
+      <c r="BE43">
+        <v>9.84</v>
+      </c>
+    </row>
+    <row r="44" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>67</v>
       </c>
@@ -8216,8 +9062,14 @@
       <c r="BB44">
         <v>1.26</v>
       </c>
-    </row>
-    <row r="45" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD44" t="s">
+        <v>905</v>
+      </c>
+      <c r="BE44">
+        <v>9.81</v>
+      </c>
+    </row>
+    <row r="45" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>68</v>
       </c>
@@ -8317,8 +9169,14 @@
       <c r="BB45">
         <v>1.42</v>
       </c>
-    </row>
-    <row r="46" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD45" t="s">
+        <v>906</v>
+      </c>
+      <c r="BE45">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="46" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>69</v>
       </c>
@@ -8418,8 +9276,14 @@
       <c r="BB46">
         <v>2.63</v>
       </c>
-    </row>
-    <row r="47" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD46" t="s">
+        <v>907</v>
+      </c>
+      <c r="BE46">
+        <v>46.27</v>
+      </c>
+    </row>
+    <row r="47" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
         <v>70</v>
       </c>
@@ -8519,8 +9383,14 @@
       <c r="BB47">
         <v>14.9</v>
       </c>
-    </row>
-    <row r="48" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD47" t="s">
+        <v>908</v>
+      </c>
+      <c r="BE47">
+        <v>56.28</v>
+      </c>
+    </row>
+    <row r="48" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>71</v>
       </c>
@@ -8620,8 +9490,14 @@
       <c r="BB48">
         <v>2.81</v>
       </c>
-    </row>
-    <row r="49" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD48" t="s">
+        <v>909</v>
+      </c>
+      <c r="BE48">
+        <v>71.349999999999994</v>
+      </c>
+    </row>
+    <row r="49" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>72</v>
       </c>
@@ -8721,8 +9597,14 @@
       <c r="BB49">
         <v>3.34</v>
       </c>
-    </row>
-    <row r="50" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD49" t="s">
+        <v>910</v>
+      </c>
+      <c r="BE49">
+        <v>13.08</v>
+      </c>
+    </row>
+    <row r="50" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>73</v>
       </c>
@@ -8822,8 +9704,14 @@
       <c r="BB50">
         <v>3.15</v>
       </c>
-    </row>
-    <row r="51" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD50" t="s">
+        <v>911</v>
+      </c>
+      <c r="BE50">
+        <v>6.76</v>
+      </c>
+    </row>
+    <row r="51" spans="3:57" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>74</v>
       </c>
@@ -8923,8 +9811,14 @@
       <c r="BB51">
         <v>2.0299999999999998</v>
       </c>
-    </row>
-    <row r="52" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD51" t="s">
+        <v>912</v>
+      </c>
+      <c r="BE51">
+        <v>4.09</v>
+      </c>
+    </row>
+    <row r="52" spans="3:57" x14ac:dyDescent="0.25">
       <c r="H52">
         <f>SUM(H3:H51)</f>
         <v>1085.54</v>
@@ -8986,8 +9880,14 @@
       <c r="BB52">
         <v>4.01</v>
       </c>
-    </row>
-    <row r="53" spans="3:54" x14ac:dyDescent="0.25">
+      <c r="BD52" t="s">
+        <v>913</v>
+      </c>
+      <c r="BE52">
+        <v>65.45</v>
+      </c>
+    </row>
+    <row r="53" spans="3:57" x14ac:dyDescent="0.25">
       <c r="Z53" s="7">
         <f>SUM(Z3:Z52)</f>
         <v>849.3000000000003</v>
@@ -9015,6 +9915,1210 @@
       <c r="BB53">
         <f>SUM(BB3:BB52)</f>
         <v>343.85999999999984</v>
+      </c>
+      <c r="BD53" t="s">
+        <v>914</v>
+      </c>
+      <c r="BE53">
+        <v>9.34</v>
+      </c>
+    </row>
+    <row r="54" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD54" t="s">
+        <v>915</v>
+      </c>
+      <c r="BE54">
+        <v>2.63</v>
+      </c>
+    </row>
+    <row r="55" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD55" t="s">
+        <v>916</v>
+      </c>
+      <c r="BE55">
+        <v>1.46</v>
+      </c>
+    </row>
+    <row r="56" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD56" t="s">
+        <v>917</v>
+      </c>
+      <c r="BE56">
+        <v>18.86</v>
+      </c>
+    </row>
+    <row r="57" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD57" t="s">
+        <v>918</v>
+      </c>
+      <c r="BE57">
+        <v>14.39</v>
+      </c>
+    </row>
+    <row r="58" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD58" t="s">
+        <v>919</v>
+      </c>
+      <c r="BE58">
+        <v>8.7799999999999994</v>
+      </c>
+    </row>
+    <row r="59" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD59" t="s">
+        <v>920</v>
+      </c>
+      <c r="BE59">
+        <v>2.74</v>
+      </c>
+    </row>
+    <row r="60" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD60" t="s">
+        <v>921</v>
+      </c>
+      <c r="BE60">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="61" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD61" t="s">
+        <v>922</v>
+      </c>
+      <c r="BE61">
+        <v>22.64</v>
+      </c>
+    </row>
+    <row r="62" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD62" t="s">
+        <v>923</v>
+      </c>
+      <c r="BE62">
+        <v>32.520000000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD63" t="s">
+        <v>924</v>
+      </c>
+      <c r="BE63">
+        <v>29.4</v>
+      </c>
+    </row>
+    <row r="64" spans="3:57" x14ac:dyDescent="0.25">
+      <c r="BD64" t="s">
+        <v>925</v>
+      </c>
+      <c r="BE64">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="65" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD65" t="s">
+        <v>926</v>
+      </c>
+      <c r="BE65">
+        <v>2.2799999999999998</v>
+      </c>
+    </row>
+    <row r="66" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD66" t="s">
+        <v>927</v>
+      </c>
+      <c r="BE66">
+        <v>2.42</v>
+      </c>
+    </row>
+    <row r="67" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD67" t="s">
+        <v>928</v>
+      </c>
+      <c r="BE67">
+        <v>50.35</v>
+      </c>
+    </row>
+    <row r="68" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD68" t="s">
+        <v>929</v>
+      </c>
+      <c r="BE68">
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="69" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD69" t="s">
+        <v>930</v>
+      </c>
+      <c r="BE69">
+        <v>8.7799999999999994</v>
+      </c>
+    </row>
+    <row r="70" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD70" t="s">
+        <v>931</v>
+      </c>
+      <c r="BE70">
+        <v>48.89</v>
+      </c>
+    </row>
+    <row r="71" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD71" t="s">
+        <v>932</v>
+      </c>
+      <c r="BE71">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="72" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD72" t="s">
+        <v>933</v>
+      </c>
+      <c r="BE72">
+        <v>27.44</v>
+      </c>
+    </row>
+    <row r="73" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD73" t="s">
+        <v>934</v>
+      </c>
+      <c r="BE73">
+        <v>17.190000000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD74" t="s">
+        <v>935</v>
+      </c>
+      <c r="BE74">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="75" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD75" t="s">
+        <v>936</v>
+      </c>
+      <c r="BE75">
+        <v>8.42</v>
+      </c>
+    </row>
+    <row r="76" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD76" t="s">
+        <v>937</v>
+      </c>
+      <c r="BE76">
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="77" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD77" t="s">
+        <v>938</v>
+      </c>
+      <c r="BE77">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD78" t="s">
+        <v>939</v>
+      </c>
+      <c r="BE78">
+        <v>3.04</v>
+      </c>
+    </row>
+    <row r="79" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD79" t="s">
+        <v>940</v>
+      </c>
+      <c r="BE79">
+        <v>40.85</v>
+      </c>
+    </row>
+    <row r="80" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD80" t="s">
+        <v>941</v>
+      </c>
+      <c r="BE80">
+        <v>42.39</v>
+      </c>
+    </row>
+    <row r="81" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD81" t="s">
+        <v>942</v>
+      </c>
+      <c r="BE81">
+        <v>13.7</v>
+      </c>
+    </row>
+    <row r="82" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD82" t="s">
+        <v>943</v>
+      </c>
+      <c r="BE82">
+        <v>30.68</v>
+      </c>
+    </row>
+    <row r="83" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD83" t="s">
+        <v>944</v>
+      </c>
+      <c r="BE83">
+        <v>34.909999999999997</v>
+      </c>
+    </row>
+    <row r="84" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD84" t="s">
+        <v>945</v>
+      </c>
+      <c r="BE84">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="85" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD85" t="s">
+        <v>946</v>
+      </c>
+      <c r="BE85">
+        <v>55.15</v>
+      </c>
+    </row>
+    <row r="86" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD86" t="s">
+        <v>947</v>
+      </c>
+      <c r="BE86">
+        <v>33.68</v>
+      </c>
+    </row>
+    <row r="87" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD87" t="s">
+        <v>948</v>
+      </c>
+      <c r="BE87">
+        <v>9.65</v>
+      </c>
+    </row>
+    <row r="88" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD88" t="s">
+        <v>949</v>
+      </c>
+      <c r="BE88">
+        <v>13.86</v>
+      </c>
+    </row>
+    <row r="89" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD89" t="s">
+        <v>950</v>
+      </c>
+      <c r="BE89">
+        <v>3.96</v>
+      </c>
+    </row>
+    <row r="90" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD90" t="s">
+        <v>951</v>
+      </c>
+      <c r="BE90">
+        <v>84.17</v>
+      </c>
+    </row>
+    <row r="91" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD91" t="s">
+        <v>952</v>
+      </c>
+      <c r="BE91">
+        <v>14.19</v>
+      </c>
+    </row>
+    <row r="92" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD92" t="s">
+        <v>953</v>
+      </c>
+      <c r="BE92">
+        <v>5.12</v>
+      </c>
+    </row>
+    <row r="93" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD93" t="s">
+        <v>954</v>
+      </c>
+      <c r="BE93">
+        <v>22.27</v>
+      </c>
+    </row>
+    <row r="94" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD94" t="s">
+        <v>955</v>
+      </c>
+      <c r="BE94">
+        <v>100.25</v>
+      </c>
+    </row>
+    <row r="95" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD95" t="s">
+        <v>956</v>
+      </c>
+      <c r="BE95">
+        <v>7.29</v>
+      </c>
+    </row>
+    <row r="96" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD96" t="s">
+        <v>957</v>
+      </c>
+      <c r="BE96">
+        <v>75.97</v>
+      </c>
+    </row>
+    <row r="97" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD97" t="s">
+        <v>958</v>
+      </c>
+      <c r="BE97">
+        <v>1.51</v>
+      </c>
+    </row>
+    <row r="98" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD98" t="s">
+        <v>959</v>
+      </c>
+      <c r="BE98">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="99" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD99" t="s">
+        <v>960</v>
+      </c>
+      <c r="BE99">
+        <v>8.33</v>
+      </c>
+    </row>
+    <row r="100" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD100" t="s">
+        <v>961</v>
+      </c>
+      <c r="BE100">
+        <v>2.23</v>
+      </c>
+    </row>
+    <row r="101" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD101" t="s">
+        <v>962</v>
+      </c>
+      <c r="BE101">
+        <v>69.349999999999994</v>
+      </c>
+    </row>
+    <row r="102" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD102" t="s">
+        <v>963</v>
+      </c>
+      <c r="BE102">
+        <v>4.59</v>
+      </c>
+    </row>
+    <row r="103" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD103" t="s">
+        <v>964</v>
+      </c>
+      <c r="BE103">
+        <v>19.11</v>
+      </c>
+    </row>
+    <row r="104" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD104" t="s">
+        <v>965</v>
+      </c>
+      <c r="BE104">
+        <v>7.67</v>
+      </c>
+    </row>
+    <row r="105" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD105" t="s">
+        <v>966</v>
+      </c>
+      <c r="BE105">
+        <v>5.22</v>
+      </c>
+    </row>
+    <row r="106" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD106" t="s">
+        <v>967</v>
+      </c>
+      <c r="BE106">
+        <v>7.72</v>
+      </c>
+    </row>
+    <row r="107" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD107" t="s">
+        <v>968</v>
+      </c>
+      <c r="BE107">
+        <v>41.58</v>
+      </c>
+    </row>
+    <row r="108" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD108" t="s">
+        <v>969</v>
+      </c>
+      <c r="BE108">
+        <v>6.09</v>
+      </c>
+    </row>
+    <row r="109" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD109" t="s">
+        <v>970</v>
+      </c>
+      <c r="BE109">
+        <v>48.98</v>
+      </c>
+    </row>
+    <row r="110" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD110" t="s">
+        <v>971</v>
+      </c>
+      <c r="BE110">
+        <v>2.61</v>
+      </c>
+    </row>
+    <row r="111" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD111" t="s">
+        <v>972</v>
+      </c>
+      <c r="BE111">
+        <v>8.56</v>
+      </c>
+    </row>
+    <row r="112" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD112" t="s">
+        <v>973</v>
+      </c>
+      <c r="BE112">
+        <v>6.13</v>
+      </c>
+    </row>
+    <row r="113" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD113" t="s">
+        <v>974</v>
+      </c>
+      <c r="BE113">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="114" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD114" t="s">
+        <v>975</v>
+      </c>
+      <c r="BE114">
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="115" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD115" t="s">
+        <v>976</v>
+      </c>
+      <c r="BE115">
+        <v>15.08</v>
+      </c>
+    </row>
+    <row r="116" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD116" t="s">
+        <v>977</v>
+      </c>
+      <c r="BE116">
+        <v>46.49</v>
+      </c>
+    </row>
+    <row r="117" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD117" t="s">
+        <v>978</v>
+      </c>
+      <c r="BE117">
+        <v>30.56</v>
+      </c>
+    </row>
+    <row r="118" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD118" t="s">
+        <v>979</v>
+      </c>
+      <c r="BE118">
+        <v>5.59</v>
+      </c>
+    </row>
+    <row r="119" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD119" t="s">
+        <v>980</v>
+      </c>
+      <c r="BE119">
+        <v>30.27</v>
+      </c>
+    </row>
+    <row r="120" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD120" t="s">
+        <v>981</v>
+      </c>
+      <c r="BE120">
+        <v>78.75</v>
+      </c>
+    </row>
+    <row r="121" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD121" t="s">
+        <v>982</v>
+      </c>
+      <c r="BE121">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="122" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD122" t="s">
+        <v>983</v>
+      </c>
+      <c r="BE122">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="123" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD123" t="s">
+        <v>984</v>
+      </c>
+      <c r="BE123">
+        <v>24.95</v>
+      </c>
+    </row>
+    <row r="124" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD124" t="s">
+        <v>985</v>
+      </c>
+      <c r="BE124">
+        <v>67.09</v>
+      </c>
+    </row>
+    <row r="125" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD125" t="s">
+        <v>986</v>
+      </c>
+      <c r="BE125">
+        <v>16.82</v>
+      </c>
+    </row>
+    <row r="126" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD126" t="s">
+        <v>987</v>
+      </c>
+      <c r="BE126">
+        <v>81.08</v>
+      </c>
+    </row>
+    <row r="127" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD127" t="s">
+        <v>988</v>
+      </c>
+      <c r="BE127">
+        <v>12.35</v>
+      </c>
+    </row>
+    <row r="128" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD128" t="s">
+        <v>989</v>
+      </c>
+      <c r="BE128">
+        <v>14.47</v>
+      </c>
+    </row>
+    <row r="129" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD129" t="s">
+        <v>990</v>
+      </c>
+      <c r="BE129">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="130" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD130" t="s">
+        <v>991</v>
+      </c>
+      <c r="BE130">
+        <v>85.72</v>
+      </c>
+    </row>
+    <row r="131" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD131" t="s">
+        <v>992</v>
+      </c>
+      <c r="BE131">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD132" t="s">
+        <v>993</v>
+      </c>
+      <c r="BE132">
+        <v>7.83</v>
+      </c>
+    </row>
+    <row r="133" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD133" t="s">
+        <v>994</v>
+      </c>
+      <c r="BE133">
+        <v>25.93</v>
+      </c>
+    </row>
+    <row r="134" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD134" t="s">
+        <v>995</v>
+      </c>
+      <c r="BE134">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="135" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD135" t="s">
+        <v>996</v>
+      </c>
+      <c r="BE135">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="136" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD136" t="s">
+        <v>997</v>
+      </c>
+      <c r="BE136">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="137" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD137" t="s">
+        <v>998</v>
+      </c>
+      <c r="BE137">
+        <v>7.91</v>
+      </c>
+    </row>
+    <row r="138" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD138" t="s">
+        <v>999</v>
+      </c>
+      <c r="BE138">
+        <v>41.59</v>
+      </c>
+    </row>
+    <row r="139" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD139" t="s">
+        <v>1000</v>
+      </c>
+      <c r="BE139">
+        <v>21.17</v>
+      </c>
+    </row>
+    <row r="140" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD140" t="s">
+        <v>1001</v>
+      </c>
+      <c r="BE140">
+        <v>15.11</v>
+      </c>
+    </row>
+    <row r="141" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD141" t="s">
+        <v>1002</v>
+      </c>
+      <c r="BE141">
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="142" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD142" t="s">
+        <v>1003</v>
+      </c>
+      <c r="BE142">
+        <v>128.16999999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD143" t="s">
+        <v>1004</v>
+      </c>
+      <c r="BE143">
+        <v>34.83</v>
+      </c>
+    </row>
+    <row r="144" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD144" t="s">
+        <v>1005</v>
+      </c>
+      <c r="BE144">
+        <v>8.1199999999999992</v>
+      </c>
+    </row>
+    <row r="145" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD145" t="s">
+        <v>1006</v>
+      </c>
+      <c r="BE145">
+        <v>30.04</v>
+      </c>
+    </row>
+    <row r="146" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD146" t="s">
+        <v>1007</v>
+      </c>
+      <c r="BE146">
+        <v>29.49</v>
+      </c>
+    </row>
+    <row r="147" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD147" t="s">
+        <v>1008</v>
+      </c>
+      <c r="BE147">
+        <v>6.23</v>
+      </c>
+    </row>
+    <row r="148" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD148" t="s">
+        <v>1009</v>
+      </c>
+      <c r="BE148">
+        <v>8.02</v>
+      </c>
+    </row>
+    <row r="149" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD149" t="s">
+        <v>1010</v>
+      </c>
+      <c r="BE149">
+        <v>43.24</v>
+      </c>
+    </row>
+    <row r="150" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD150" t="s">
+        <v>1011</v>
+      </c>
+      <c r="BE150">
+        <v>15.89</v>
+      </c>
+    </row>
+    <row r="151" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD151" t="s">
+        <v>1012</v>
+      </c>
+      <c r="BE151">
+        <v>2.2599999999999998</v>
+      </c>
+    </row>
+    <row r="152" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD152" t="s">
+        <v>1013</v>
+      </c>
+      <c r="BE152">
+        <v>32.61</v>
+      </c>
+    </row>
+    <row r="153" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD153" t="s">
+        <v>1014</v>
+      </c>
+      <c r="BE153">
+        <v>24.45</v>
+      </c>
+    </row>
+    <row r="154" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD154" t="s">
+        <v>1015</v>
+      </c>
+      <c r="BE154">
+        <v>4.24</v>
+      </c>
+    </row>
+    <row r="155" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD155" t="s">
+        <v>1016</v>
+      </c>
+      <c r="BE155">
+        <v>14.11</v>
+      </c>
+    </row>
+    <row r="156" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD156" t="s">
+        <v>1017</v>
+      </c>
+      <c r="BE156">
+        <v>12.03</v>
+      </c>
+    </row>
+    <row r="157" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD157" t="s">
+        <v>1018</v>
+      </c>
+      <c r="BE157">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="158" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD158" t="s">
+        <v>1019</v>
+      </c>
+      <c r="BE158">
+        <v>8.75</v>
+      </c>
+    </row>
+    <row r="159" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD159" t="s">
+        <v>1020</v>
+      </c>
+      <c r="BE159">
+        <v>11.16</v>
+      </c>
+    </row>
+    <row r="160" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD160" t="s">
+        <v>1021</v>
+      </c>
+      <c r="BE160">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="161" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD161" t="s">
+        <v>1022</v>
+      </c>
+      <c r="BE161">
+        <v>13.76</v>
+      </c>
+    </row>
+    <row r="162" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD162" t="s">
+        <v>1023</v>
+      </c>
+      <c r="BE162">
+        <v>14.6</v>
+      </c>
+    </row>
+    <row r="163" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD163" t="s">
+        <v>1024</v>
+      </c>
+      <c r="BE163">
+        <v>12.83</v>
+      </c>
+    </row>
+    <row r="164" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD164" t="s">
+        <v>1025</v>
+      </c>
+      <c r="BE164">
+        <v>12.14</v>
+      </c>
+    </row>
+    <row r="165" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD165" t="s">
+        <v>1026</v>
+      </c>
+      <c r="BE165">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="166" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD166" t="s">
+        <v>1027</v>
+      </c>
+      <c r="BE166">
+        <v>48.36</v>
+      </c>
+    </row>
+    <row r="167" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD167" t="s">
+        <v>1028</v>
+      </c>
+      <c r="BE167">
+        <v>12.18</v>
+      </c>
+    </row>
+    <row r="168" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD168" t="s">
+        <v>1029</v>
+      </c>
+      <c r="BE168">
+        <v>4.22</v>
+      </c>
+    </row>
+    <row r="169" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD169" t="s">
+        <v>1030</v>
+      </c>
+      <c r="BE169">
+        <v>19.88</v>
+      </c>
+    </row>
+    <row r="170" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD170" t="s">
+        <v>1031</v>
+      </c>
+      <c r="BE170">
+        <v>9.56</v>
+      </c>
+    </row>
+    <row r="171" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD171" t="s">
+        <v>1032</v>
+      </c>
+      <c r="BE171">
+        <v>32.46</v>
+      </c>
+    </row>
+    <row r="172" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD172" t="s">
+        <v>1033</v>
+      </c>
+      <c r="BE172">
+        <v>5.36</v>
+      </c>
+    </row>
+    <row r="173" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD173" t="s">
+        <v>1034</v>
+      </c>
+      <c r="BE173">
+        <v>16.14</v>
+      </c>
+    </row>
+    <row r="174" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD174" t="s">
+        <v>1035</v>
+      </c>
+      <c r="BE174">
+        <v>5.46</v>
+      </c>
+    </row>
+    <row r="175" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD175" t="s">
+        <v>1036</v>
+      </c>
+      <c r="BE175">
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="176" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD176" t="s">
+        <v>1037</v>
+      </c>
+      <c r="BE176">
+        <v>24.44</v>
+      </c>
+    </row>
+    <row r="177" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD177" t="s">
+        <v>1038</v>
+      </c>
+      <c r="BE177">
+        <v>25.72</v>
+      </c>
+    </row>
+    <row r="178" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD178" t="s">
+        <v>1039</v>
+      </c>
+      <c r="BE178">
+        <v>13.69</v>
+      </c>
+    </row>
+    <row r="179" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD179" t="s">
+        <v>1040</v>
+      </c>
+      <c r="BE179">
+        <v>24.43</v>
+      </c>
+    </row>
+    <row r="180" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD180" t="s">
+        <v>1041</v>
+      </c>
+      <c r="BE180">
+        <v>16.850000000000001</v>
+      </c>
+    </row>
+    <row r="181" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD181" t="s">
+        <v>1042</v>
+      </c>
+      <c r="BE181">
+        <v>4.71</v>
+      </c>
+    </row>
+    <row r="182" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD182" t="s">
+        <v>1043</v>
+      </c>
+      <c r="BE182">
+        <v>75.290000000000006</v>
+      </c>
+    </row>
+    <row r="183" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD183" t="s">
+        <v>1044</v>
+      </c>
+      <c r="BE183">
+        <v>23.13</v>
+      </c>
+    </row>
+    <row r="184" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD184" t="s">
+        <v>1045</v>
+      </c>
+      <c r="BE184">
+        <v>28.88</v>
+      </c>
+    </row>
+    <row r="185" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD185" t="s">
+        <v>1046</v>
+      </c>
+      <c r="BE185">
+        <v>130.99</v>
+      </c>
+    </row>
+    <row r="186" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD186" t="s">
+        <v>1047</v>
+      </c>
+      <c r="BE186">
+        <v>10.11</v>
+      </c>
+    </row>
+    <row r="187" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD187" t="s">
+        <v>1048</v>
+      </c>
+      <c r="BE187">
+        <v>32.950000000000003</v>
+      </c>
+    </row>
+    <row r="188" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD188" t="s">
+        <v>1049</v>
+      </c>
+      <c r="BE188">
+        <v>13.06</v>
+      </c>
+    </row>
+    <row r="189" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD189" t="s">
+        <v>1050</v>
+      </c>
+      <c r="BE189">
+        <v>8.7200000000000006</v>
+      </c>
+    </row>
+    <row r="190" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD190" t="s">
+        <v>1051</v>
+      </c>
+      <c r="BE190">
+        <v>21.34</v>
+      </c>
+    </row>
+    <row r="191" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD191" t="s">
+        <v>1052</v>
+      </c>
+      <c r="BE191">
+        <v>69.17</v>
+      </c>
+    </row>
+    <row r="192" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD192" t="s">
+        <v>1053</v>
+      </c>
+      <c r="BE192">
+        <v>8.82</v>
+      </c>
+    </row>
+    <row r="193" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD193" t="s">
+        <v>1054</v>
+      </c>
+      <c r="BE193">
+        <v>17.53</v>
+      </c>
+    </row>
+    <row r="194" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD194" t="s">
+        <v>1055</v>
+      </c>
+      <c r="BE194">
+        <v>78.87</v>
+      </c>
+    </row>
+    <row r="195" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD195" t="s">
+        <v>1056</v>
+      </c>
+      <c r="BE195">
+        <v>40.25</v>
+      </c>
+    </row>
+    <row r="196" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD196" t="s">
+        <v>1057</v>
+      </c>
+      <c r="BE196">
+        <v>10.94</v>
+      </c>
+    </row>
+    <row r="197" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD197" t="s">
+        <v>1058</v>
+      </c>
+      <c r="BE197">
+        <v>41.73</v>
+      </c>
+    </row>
+    <row r="198" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD198" t="s">
+        <v>1059</v>
+      </c>
+      <c r="BE198">
+        <v>34.729999999999997</v>
+      </c>
+    </row>
+    <row r="199" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD199" t="s">
+        <v>1060</v>
+      </c>
+      <c r="BE199">
+        <v>25.76</v>
+      </c>
+    </row>
+    <row r="200" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD200" t="s">
+        <v>1061</v>
+      </c>
+      <c r="BE200">
+        <v>9.84</v>
+      </c>
+    </row>
+    <row r="201" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD201" t="s">
+        <v>1062</v>
+      </c>
+      <c r="BE201">
+        <v>19.04</v>
+      </c>
+    </row>
+    <row r="202" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BD202" t="s">
+        <v>1063</v>
+      </c>
+      <c r="BE202">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="203" spans="56:57" x14ac:dyDescent="0.25">
+      <c r="BE203">
+        <f>SUM(BE3:BE202)</f>
+        <v>4846.1199999999981</v>
       </c>
     </row>
   </sheetData>

</xml_diff>